<commit_message>
[SIT] Add data-type for date import + fix convert data from date to data submit + remove fake data in file excel import.
</commit_message>
<xml_diff>
--- a/apps/core/fimport/static/fimport/template/mega-import.xlsx
+++ b/apps/core/fimport/static/fimport/template/mega-import.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\Coding\MIS\misui\apps\core\fimport\static\fimport\template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{277EC948-FDD0-48A6-B1DD-A04D168B3A8A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6CBB119-1C27-41D8-A9EE-7954E538AF5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="803" firstSheet="5" activeTab="12" xr2:uid="{ABCF866D-F0C2-489F-81F3-6B45D3E3629E}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="803" firstSheet="7" activeTab="13" xr2:uid="{ABCF866D-F0C2-489F-81F3-6B45D3E3629E}"/>
   </bookViews>
   <sheets>
     <sheet name="#account.users" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="439" uniqueCount="205">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="159">
   <si>
     <t>E-Mail</t>
   </si>
@@ -553,18 +553,6 @@
 - Ví dụ: Bà</t>
   </si>
   <si>
-    <t>1</t>
-  </si>
-  <si>
-    <t>001</t>
-  </si>
-  <si>
-    <t>Mrs</t>
-  </si>
-  <si>
-    <t>Bà</t>
-  </si>
-  <si>
     <t>Tỉ lệ (*)</t>
   </si>
   <si>
@@ -585,18 +573,6 @@
 - Ví dụ: VND</t>
   </si>
   <si>
-    <t>VND</t>
-  </si>
-  <si>
-    <t>005</t>
-  </si>
-  <si>
-    <t>Đại Lý Cấp 5</t>
-  </si>
-  <si>
-    <t>Đại lý cấp 005</t>
-  </si>
-  <si>
     <t>- Bắt buộc, định danh
 - Độ dài tối đa: 100
 - Ví dụ: AT001</t>
@@ -610,21 +586,6 @@
 - Ví dụ: Khách hàng</t>
   </si>
   <si>
-    <t>AT001</t>
-  </si>
-  <si>
-    <t>Khách hàng</t>
-  </si>
-  <si>
-    <t>Đây là loại khách hàng</t>
-  </si>
-  <si>
-    <t>2</t>
-  </si>
-  <si>
-    <t>AT002</t>
-  </si>
-  <si>
     <t>- Tên của ngành
 - Ví dụ: Dịch vụ</t>
   </si>
@@ -632,21 +593,6 @@
     <t>- Bắt buộc, định danh
 - Độ dài tối đa: 100
 - Ví dụ: 001</t>
-  </si>
-  <si>
-    <t>Dịch vụ</t>
-  </si>
-  <si>
-    <t>Đây là loại dịch vụ</t>
-  </si>
-  <si>
-    <t>002</t>
-  </si>
-  <si>
-    <t>Bán lẻ</t>
-  </si>
-  <si>
-    <t>Đây là loại bán lẻ</t>
   </si>
   <si>
     <t>- Tên của chính sách
@@ -709,15 +655,6 @@
     </r>
   </si>
   <si>
-    <t>Thanh toán 30-30-40</t>
-  </si>
-  <si>
-    <t>0</t>
-  </si>
-  <si>
-    <t>[[0, 30, 1, 1, 1], [0, 30, 1, 1, 2], [0, 40, 1, 1, 3]]</t>
-  </si>
-  <si>
     <t>Người có thông tin liên hệ (*)</t>
   </si>
   <si>
@@ -761,27 +698,6 @@
   <si>
     <t>- Mã tài khoản liên kết với liên hệ này tại #saledata.accounts
 - Ví dụ: ACC0001</t>
-  </si>
-  <si>
-    <t>EMP0001</t>
-  </si>
-  <si>
-    <t>Giám Đốc</t>
-  </si>
-  <si>
-    <t>LH0001</t>
-  </si>
-  <si>
-    <t>0972403708</t>
-  </si>
-  <si>
-    <t>anv@example.com</t>
-  </si>
-  <si>
-    <t>AC0001</t>
-  </si>
-  <si>
-    <t>Nguyễn Văn A</t>
   </si>
   <si>
     <t>Di động (duy nhất)</t>
@@ -798,9 +714,6 @@
     <t>- Là duy nhất
 - Thư điện tử của người đại diện
 - Ví dụ: anv@example.com</t>
-  </si>
-  <si>
-    <t>Đây là điều khoản thanh toán cho việc bán hàng với các mốc thanh toán ký hợp đồng - giao hàng - xuất hoá đơn với giá trị thanh toán theo phần trăm 30-30-40.</t>
   </si>
   <si>
     <t>- Bắt buộc, định danh
@@ -889,30 +802,12 @@
 - Ví dụ: 2</t>
   </si>
   <si>
-    <t>CTY_MTS</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Công Ty TNHH Minh Tâm Solution</t>
-  </si>
-  <si>
-    <t>https://www.bflow.vn</t>
-  </si>
-  <si>
-    <t>0987654321</t>
-  </si>
-  <si>
-    <t>0317493763</t>
-  </si>
-  <si>
     <t>Email</t>
   </si>
   <si>
     <t>- Độ dài tối đa 150
 - Địa chỉ thư điện tử 
 - Ví dụ: support@bflow.vn</t>
-  </si>
-  <si>
-    <t>support@bflow.vn</t>
   </si>
   <si>
     <t>Tổng số nhân viên</t>
@@ -934,39 +829,6 @@
 - Ví dụ: CTY_MTS</t>
   </si>
   <si>
-    <t>3</t>
-  </si>
-  <si>
-    <t>4</t>
-  </si>
-  <si>
-    <t>5</t>
-  </si>
-  <si>
-    <t>6</t>
-  </si>
-  <si>
-    <t>7</t>
-  </si>
-  <si>
-    <t>8</t>
-  </si>
-  <si>
-    <t>9</t>
-  </si>
-  <si>
-    <t>10</t>
-  </si>
-  <si>
-    <t>11</t>
-  </si>
-  <si>
-    <t>12</t>
-  </si>
-  <si>
-    <t>EMP0001,EMP0002,EMP0003</t>
-  </si>
-  <si>
     <t>Liên hệ</t>
   </si>
   <si>
@@ -979,18 +841,18 @@
 - Ví dụ: [["001", 1], ["002", 0]]</t>
   </si>
   <si>
-    <t>[["001", 1],["002", 0]]</t>
-  </si>
-  <si>
     <t>- Định dạng ngày-tháng-năm (DD-MM-YYYY)
 - Ví dụ: 31-01-1970</t>
+  </si>
+  <si>
+    <t>Luôn giữ kiểu của ô là text để trình đọc dữ liệu có thể hiểu</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1043,8 +905,22 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="16"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1054,6 +930,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF0070C0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1108,8 +990,6 @@
   </cellStyleXfs>
   <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -1146,9 +1026,6 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -1166,6 +1043,15 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1485,63 +1371,63 @@
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.5546875" style="9" customWidth="1"/>
-    <col min="2" max="2" width="27.88671875" style="9" customWidth="1"/>
-    <col min="3" max="3" width="19.21875" style="9" customWidth="1"/>
-    <col min="4" max="5" width="15.88671875" style="9" customWidth="1"/>
-    <col min="6" max="6" width="36.6640625" style="9" customWidth="1"/>
-    <col min="7" max="7" width="22" style="9" customWidth="1"/>
-    <col min="8" max="16384" width="8.88671875" style="9"/>
+    <col min="1" max="1" width="8.5546875" style="7" customWidth="1"/>
+    <col min="2" max="2" width="27.88671875" style="7" customWidth="1"/>
+    <col min="3" max="3" width="19.21875" style="7" customWidth="1"/>
+    <col min="4" max="5" width="15.88671875" style="7" customWidth="1"/>
+    <col min="6" max="6" width="36.6640625" style="7" customWidth="1"/>
+    <col min="7" max="7" width="22" style="7" customWidth="1"/>
+    <col min="8" max="16384" width="8.88671875" style="7"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="B1" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="C1" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="10" t="s">
+      <c r="D1" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="10" t="s">
+      <c r="E1" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="10" t="s">
+      <c r="F1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="G1" s="10" t="s">
+      <c r="G1" s="8" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="111" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="9" t="s">
+      <c r="A2" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="B2" s="9" t="s">
+      <c r="B2" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="C2" s="9" t="s">
+      <c r="C2" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="D2" s="9" t="s">
+      <c r="D2" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="E2" s="9" t="s">
+      <c r="E2" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="F2" s="9" t="s">
+      <c r="F2" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="G2" s="9" t="s">
+      <c r="G2" s="7" t="s">
         <v>64</v>
       </c>
     </row>
@@ -1552,78 +1438,58 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E863D4F3-258D-41FD-90A7-5BEE0F94C0B4}">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="C5" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.88671875" style="9"/>
-    <col min="2" max="2" width="19.77734375" style="9" customWidth="1"/>
-    <col min="3" max="3" width="26" style="9" customWidth="1"/>
-    <col min="4" max="4" width="23.109375" style="9" customWidth="1"/>
-    <col min="5" max="5" width="65.6640625" style="9" customWidth="1"/>
-    <col min="6" max="6" width="48.33203125" style="9" customWidth="1"/>
-    <col min="7" max="16384" width="8.88671875" style="9"/>
+    <col min="1" max="1" width="8.88671875" style="7"/>
+    <col min="2" max="2" width="19.77734375" style="7" customWidth="1"/>
+    <col min="3" max="3" width="26" style="7" customWidth="1"/>
+    <col min="4" max="4" width="23.109375" style="7" customWidth="1"/>
+    <col min="5" max="5" width="65.6640625" style="7" customWidth="1"/>
+    <col min="6" max="6" width="48.33203125" style="7" customWidth="1"/>
+    <col min="7" max="16384" width="8.88671875" style="7"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="B1" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="C1" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="10" t="s">
-        <v>127</v>
-      </c>
-      <c r="E1" s="10" t="s">
-        <v>128</v>
-      </c>
-      <c r="F1" s="10" t="s">
+      <c r="D1" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="E1" s="8" t="s">
+        <v>110</v>
+      </c>
+      <c r="F1" s="8" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="172.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="9" t="s">
+      <c r="A2" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="B2" s="9" t="s">
-        <v>120</v>
-      </c>
-      <c r="C2" s="9" t="s">
-        <v>126</v>
-      </c>
-      <c r="D2" s="9" t="s">
-        <v>129</v>
-      </c>
-      <c r="E2" s="9" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A3" s="9" t="s">
-        <v>98</v>
-      </c>
-      <c r="B3" s="9" t="s">
-        <v>99</v>
-      </c>
-      <c r="C3" s="9" t="s">
-        <v>131</v>
-      </c>
-      <c r="D3" s="9" t="s">
-        <v>132</v>
-      </c>
-      <c r="E3" s="9" t="s">
-        <v>133</v>
-      </c>
-      <c r="F3" s="9" t="s">
-        <v>158</v>
+      <c r="B2" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>108</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>111</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>112</v>
       </c>
     </row>
   </sheetData>
@@ -1638,191 +1504,142 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A45619C8-AAF7-43DE-831A-2BED068D71D3}">
-  <dimension ref="A1:K3"/>
+  <dimension ref="A1:K2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="D9" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.33203125" style="9" customWidth="1"/>
-    <col min="2" max="2" width="21.44140625" style="9" customWidth="1"/>
-    <col min="3" max="3" width="28.77734375" style="9" customWidth="1"/>
-    <col min="4" max="4" width="28.5546875" style="9" customWidth="1"/>
-    <col min="5" max="5" width="25.21875" style="9" customWidth="1"/>
-    <col min="6" max="6" width="21.5546875" style="9" customWidth="1"/>
-    <col min="7" max="7" width="12.21875" style="9" customWidth="1"/>
-    <col min="8" max="8" width="19.109375" style="9" customWidth="1"/>
-    <col min="9" max="10" width="23.21875" style="9" customWidth="1"/>
-    <col min="11" max="11" width="23.33203125" style="9" customWidth="1"/>
-    <col min="12" max="16384" width="8.88671875" style="9"/>
+    <col min="1" max="1" width="10.33203125" style="7" customWidth="1"/>
+    <col min="2" max="2" width="21.44140625" style="7" customWidth="1"/>
+    <col min="3" max="3" width="28.77734375" style="7" customWidth="1"/>
+    <col min="4" max="4" width="28.5546875" style="7" customWidth="1"/>
+    <col min="5" max="5" width="25.21875" style="7" customWidth="1"/>
+    <col min="6" max="6" width="21.5546875" style="7" customWidth="1"/>
+    <col min="7" max="7" width="12.21875" style="7" customWidth="1"/>
+    <col min="8" max="8" width="19.109375" style="7" customWidth="1"/>
+    <col min="9" max="10" width="23.21875" style="7" customWidth="1"/>
+    <col min="11" max="11" width="23.33203125" style="7" customWidth="1"/>
+    <col min="12" max="16384" width="8.88671875" style="7"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="B1" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="C1" s="10" t="s">
-        <v>134</v>
-      </c>
-      <c r="D1" s="10" t="s">
-        <v>135</v>
-      </c>
-      <c r="E1" s="10" t="s">
-        <v>136</v>
-      </c>
-      <c r="F1" s="10" t="s">
-        <v>139</v>
-      </c>
-      <c r="G1" s="10" t="s">
-        <v>137</v>
-      </c>
-      <c r="H1" s="10" t="s">
-        <v>154</v>
-      </c>
-      <c r="I1" s="10" t="s">
-        <v>155</v>
-      </c>
-      <c r="J1" s="10" t="s">
-        <v>145</v>
-      </c>
-      <c r="K1" s="10" t="s">
-        <v>138</v>
+      <c r="C1" s="8" t="s">
+        <v>113</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>114</v>
+      </c>
+      <c r="E1" s="8" t="s">
+        <v>115</v>
+      </c>
+      <c r="F1" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="G1" s="8" t="s">
+        <v>116</v>
+      </c>
+      <c r="H1" s="8" t="s">
+        <v>126</v>
+      </c>
+      <c r="I1" s="8" t="s">
+        <v>127</v>
+      </c>
+      <c r="J1" s="8" t="s">
+        <v>124</v>
+      </c>
+      <c r="K1" s="8" t="s">
+        <v>117</v>
       </c>
     </row>
     <row r="2" spans="1:11" ht="85.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="11" t="s">
+      <c r="A2" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="B2" s="14" t="s">
+      <c r="B2" s="12" t="s">
         <v>95</v>
       </c>
-      <c r="C2" s="9" t="s">
-        <v>140</v>
-      </c>
-      <c r="D2" s="9" t="s">
-        <v>141</v>
-      </c>
-      <c r="E2" s="9" t="s">
-        <v>142</v>
-      </c>
-      <c r="F2" s="9" t="s">
-        <v>143</v>
-      </c>
-      <c r="G2" s="9" t="s">
-        <v>144</v>
-      </c>
-      <c r="H2" s="9" t="s">
-        <v>156</v>
-      </c>
-      <c r="I2" s="9" t="s">
-        <v>157</v>
-      </c>
-      <c r="J2" s="9" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A3" s="9" t="s">
-        <v>98</v>
-      </c>
-      <c r="B3" s="9" t="s">
-        <v>99</v>
-      </c>
-      <c r="C3" s="9" t="s">
-        <v>147</v>
-      </c>
-      <c r="D3" s="9" t="s">
-        <v>99</v>
-      </c>
-      <c r="E3" s="9" t="s">
-        <v>153</v>
-      </c>
-      <c r="F3" s="9" t="s">
-        <v>148</v>
-      </c>
-      <c r="G3" s="9" t="s">
-        <v>149</v>
-      </c>
-      <c r="H3" s="9" t="s">
-        <v>150</v>
-      </c>
-      <c r="I3" s="15" t="s">
-        <v>151</v>
-      </c>
-      <c r="J3" s="9" t="s">
-        <v>152</v>
+      <c r="C2" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>122</v>
+      </c>
+      <c r="G2" s="7" t="s">
+        <v>123</v>
+      </c>
+      <c r="H2" s="7" t="s">
+        <v>128</v>
+      </c>
+      <c r="I2" s="7" t="s">
+        <v>129</v>
+      </c>
+      <c r="J2" s="7" t="s">
+        <v>125</v>
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="I3" r:id="rId1" xr:uid="{A7F80CA7-55FF-4114-ABC4-D566F639A9D2}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FDBA7C1B-B0F0-4AC8-A907-82185EA45827}">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+      <selection activeCell="C10" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.109375" style="11" customWidth="1"/>
-    <col min="2" max="2" width="25.21875" style="11" customWidth="1"/>
-    <col min="3" max="3" width="38.44140625" style="11" customWidth="1"/>
-    <col min="4" max="4" width="65" style="11" customWidth="1"/>
-    <col min="5" max="16384" width="8.88671875" style="11"/>
+    <col min="1" max="1" width="11.109375" style="9" customWidth="1"/>
+    <col min="2" max="2" width="25.21875" style="9" customWidth="1"/>
+    <col min="3" max="3" width="38.44140625" style="9" customWidth="1"/>
+    <col min="4" max="4" width="65" style="9" customWidth="1"/>
+    <col min="5" max="16384" width="8.88671875" style="9"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="B1" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="C1" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="10" t="s">
+      <c r="D1" s="8" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="73.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="11" t="s">
+      <c r="A2" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="B2" s="14" t="s">
+      <c r="B2" s="12" t="s">
         <v>95</v>
       </c>
-      <c r="C2" s="9" t="s">
+      <c r="C2" s="7" t="s">
         <v>96</v>
       </c>
-      <c r="D2" s="9" t="s">
+      <c r="D2" s="7" t="s">
         <v>97</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" s="11" t="s">
-        <v>98</v>
-      </c>
-      <c r="B3" s="11" t="s">
-        <v>99</v>
-      </c>
-      <c r="C3" s="11" t="s">
-        <v>100</v>
-      </c>
-      <c r="D3" s="11" t="s">
-        <v>101</v>
       </c>
     </row>
   </sheetData>
@@ -1832,699 +1649,121 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{876A0AB4-CD70-4743-A933-50E4AFBD716C}">
-  <dimension ref="A1:O14"/>
+  <dimension ref="A1:O2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="N17" sqref="N17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.88671875" style="9"/>
-    <col min="2" max="2" width="23.109375" style="9" customWidth="1"/>
-    <col min="3" max="3" width="37" style="9" customWidth="1"/>
-    <col min="4" max="4" width="34.44140625" style="9" customWidth="1"/>
-    <col min="5" max="6" width="23.109375" style="9" customWidth="1"/>
-    <col min="7" max="7" width="32.109375" style="9" customWidth="1"/>
-    <col min="8" max="14" width="23.109375" style="9" customWidth="1"/>
-    <col min="15" max="15" width="37.44140625" style="9" customWidth="1"/>
-    <col min="16" max="16384" width="8.88671875" style="9"/>
+    <col min="1" max="1" width="8.88671875" style="7"/>
+    <col min="2" max="2" width="23.109375" style="7" customWidth="1"/>
+    <col min="3" max="3" width="37" style="7" customWidth="1"/>
+    <col min="4" max="4" width="34.44140625" style="7" customWidth="1"/>
+    <col min="5" max="6" width="23.109375" style="7" customWidth="1"/>
+    <col min="7" max="7" width="32.109375" style="7" customWidth="1"/>
+    <col min="8" max="14" width="23.109375" style="7" customWidth="1"/>
+    <col min="15" max="15" width="37.44140625" style="7" customWidth="1"/>
+    <col min="16" max="16384" width="8.88671875" style="7"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="16" t="s">
+      <c r="B1" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="C1" s="16" t="s">
-        <v>160</v>
-      </c>
-      <c r="D1" s="16" t="s">
-        <v>162</v>
-      </c>
-      <c r="E1" s="16" t="s">
-        <v>163</v>
-      </c>
-      <c r="F1" s="16" t="s">
-        <v>166</v>
-      </c>
-      <c r="G1" s="16" t="s">
-        <v>168</v>
-      </c>
-      <c r="H1" s="16" t="s">
-        <v>170</v>
-      </c>
-      <c r="I1" s="16" t="s">
-        <v>171</v>
-      </c>
-      <c r="J1" s="16" t="s">
-        <v>183</v>
-      </c>
-      <c r="K1" s="16" t="s">
-        <v>174</v>
-      </c>
-      <c r="L1" s="16" t="s">
-        <v>176</v>
-      </c>
-      <c r="M1" s="16" t="s">
-        <v>186</v>
-      </c>
-      <c r="N1" s="16" t="s">
-        <v>188</v>
-      </c>
-      <c r="O1" s="16" t="s">
-        <v>201</v>
+      <c r="C1" s="13" t="s">
+        <v>131</v>
+      </c>
+      <c r="D1" s="13" t="s">
+        <v>133</v>
+      </c>
+      <c r="E1" s="13" t="s">
+        <v>134</v>
+      </c>
+      <c r="F1" s="13" t="s">
+        <v>137</v>
+      </c>
+      <c r="G1" s="13" t="s">
+        <v>139</v>
+      </c>
+      <c r="H1" s="13" t="s">
+        <v>141</v>
+      </c>
+      <c r="I1" s="13" t="s">
+        <v>142</v>
+      </c>
+      <c r="J1" s="13" t="s">
+        <v>149</v>
+      </c>
+      <c r="K1" s="13" t="s">
+        <v>145</v>
+      </c>
+      <c r="L1" s="13" t="s">
+        <v>147</v>
+      </c>
+      <c r="M1" s="13" t="s">
+        <v>151</v>
+      </c>
+      <c r="N1" s="13" t="s">
+        <v>153</v>
+      </c>
+      <c r="O1" s="13" t="s">
+        <v>155</v>
       </c>
     </row>
     <row r="2" spans="1:15" ht="147.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="9" t="s">
+      <c r="A2" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="B2" s="9" t="s">
-        <v>159</v>
-      </c>
-      <c r="C2" s="9" t="s">
-        <v>161</v>
-      </c>
-      <c r="D2" s="9" t="s">
-        <v>164</v>
-      </c>
-      <c r="E2" s="9" t="s">
-        <v>165</v>
-      </c>
-      <c r="F2" s="9" t="s">
-        <v>167</v>
-      </c>
-      <c r="G2" s="9" t="s">
-        <v>169</v>
-      </c>
-      <c r="H2" s="9" t="s">
-        <v>173</v>
-      </c>
-      <c r="I2" s="9" t="s">
-        <v>172</v>
-      </c>
-      <c r="J2" s="9" t="s">
-        <v>184</v>
-      </c>
-      <c r="K2" s="9" t="s">
-        <v>175</v>
-      </c>
-      <c r="L2" s="9" t="s">
-        <v>177</v>
-      </c>
-      <c r="M2" s="9" t="s">
-        <v>187</v>
-      </c>
-      <c r="N2" s="9" t="s">
-        <v>189</v>
-      </c>
-      <c r="O2" s="9" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A3" s="9" t="s">
-        <v>98</v>
-      </c>
-      <c r="B3" s="9" t="s">
-        <v>178</v>
-      </c>
-      <c r="C3" s="9" t="s">
-        <v>179</v>
-      </c>
-      <c r="D3" s="9" t="s">
-        <v>114</v>
-      </c>
-      <c r="E3" s="9" t="s">
-        <v>99</v>
-      </c>
-      <c r="F3" s="9" t="s">
-        <v>99</v>
-      </c>
-      <c r="G3" s="9" t="s">
-        <v>200</v>
-      </c>
-      <c r="H3" s="15" t="s">
-        <v>180</v>
-      </c>
-      <c r="I3" s="9" t="s">
-        <v>181</v>
-      </c>
-      <c r="J3" s="9" t="s">
-        <v>185</v>
-      </c>
-      <c r="K3" s="9" t="s">
-        <v>182</v>
-      </c>
-      <c r="L3" s="9" t="s">
-        <v>98</v>
-      </c>
-      <c r="M3" s="9" t="s">
-        <v>117</v>
-      </c>
-      <c r="N3" s="9" t="s">
-        <v>178</v>
-      </c>
-      <c r="O3" s="9" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A4" s="9" t="s">
-        <v>117</v>
-      </c>
-      <c r="B4" s="9" t="s">
-        <v>178</v>
-      </c>
-      <c r="C4" s="9" t="s">
-        <v>179</v>
-      </c>
-      <c r="D4" s="9" t="s">
-        <v>114</v>
-      </c>
-      <c r="E4" s="9" t="s">
-        <v>99</v>
-      </c>
-      <c r="F4" s="9" t="s">
-        <v>99</v>
-      </c>
-      <c r="G4" s="9" t="s">
-        <v>147</v>
-      </c>
-      <c r="H4" s="15" t="s">
-        <v>180</v>
-      </c>
-      <c r="I4" s="9" t="s">
-        <v>181</v>
-      </c>
-      <c r="J4" s="9" t="s">
-        <v>185</v>
-      </c>
-      <c r="K4" s="9" t="s">
-        <v>182</v>
-      </c>
-      <c r="L4" s="9" t="s">
-        <v>117</v>
-      </c>
-      <c r="M4" s="9" t="s">
-        <v>98</v>
-      </c>
-      <c r="N4" s="9" t="s">
-        <v>178</v>
-      </c>
-      <c r="O4" s="9" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A5" s="9" t="s">
-        <v>190</v>
-      </c>
-      <c r="B5" s="9" t="s">
-        <v>178</v>
-      </c>
-      <c r="C5" s="9" t="s">
-        <v>179</v>
-      </c>
-      <c r="D5" s="9" t="s">
-        <v>114</v>
-      </c>
-      <c r="E5" s="9" t="s">
-        <v>99</v>
-      </c>
-      <c r="F5" s="9" t="s">
-        <v>99</v>
-      </c>
-      <c r="G5" s="9" t="s">
-        <v>147</v>
-      </c>
-      <c r="H5" s="15" t="s">
-        <v>180</v>
-      </c>
-      <c r="I5" s="9" t="s">
-        <v>181</v>
-      </c>
-      <c r="J5" s="9" t="s">
-        <v>185</v>
-      </c>
-      <c r="K5" s="9" t="s">
-        <v>182</v>
-      </c>
-      <c r="L5" s="9" t="s">
-        <v>190</v>
-      </c>
-      <c r="M5" s="9" t="s">
-        <v>190</v>
-      </c>
-      <c r="N5" s="9" t="s">
-        <v>178</v>
-      </c>
-      <c r="O5" s="9" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A6" s="9" t="s">
-        <v>191</v>
-      </c>
-      <c r="B6" s="9" t="s">
-        <v>178</v>
-      </c>
-      <c r="C6" s="9" t="s">
-        <v>179</v>
-      </c>
-      <c r="D6" s="9" t="s">
-        <v>114</v>
-      </c>
-      <c r="E6" s="9" t="s">
-        <v>99</v>
-      </c>
-      <c r="F6" s="9" t="s">
-        <v>99</v>
-      </c>
-      <c r="G6" s="9" t="s">
-        <v>147</v>
-      </c>
-      <c r="H6" s="15" t="s">
-        <v>180</v>
-      </c>
-      <c r="I6" s="9" t="s">
-        <v>181</v>
-      </c>
-      <c r="J6" s="9" t="s">
-        <v>185</v>
-      </c>
-      <c r="K6" s="9" t="s">
-        <v>182</v>
-      </c>
-      <c r="L6" s="9" t="s">
-        <v>191</v>
-      </c>
-      <c r="M6" s="9" t="s">
-        <v>191</v>
-      </c>
-      <c r="N6" s="9" t="s">
-        <v>178</v>
-      </c>
-      <c r="O6" s="9" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A7" s="9" t="s">
-        <v>192</v>
-      </c>
-      <c r="B7" s="9" t="s">
-        <v>178</v>
-      </c>
-      <c r="C7" s="9" t="s">
-        <v>179</v>
-      </c>
-      <c r="D7" s="9" t="s">
-        <v>114</v>
-      </c>
-      <c r="E7" s="9" t="s">
-        <v>99</v>
-      </c>
-      <c r="F7" s="9" t="s">
-        <v>99</v>
-      </c>
-      <c r="G7" s="9" t="s">
-        <v>147</v>
-      </c>
-      <c r="H7" s="15" t="s">
-        <v>180</v>
-      </c>
-      <c r="I7" s="9" t="s">
-        <v>181</v>
-      </c>
-      <c r="J7" s="9" t="s">
-        <v>185</v>
-      </c>
-      <c r="K7" s="9" t="s">
-        <v>182</v>
-      </c>
-      <c r="L7" s="9" t="s">
-        <v>192</v>
-      </c>
-      <c r="M7" s="9" t="s">
-        <v>98</v>
-      </c>
-      <c r="N7" s="9" t="s">
-        <v>178</v>
-      </c>
-      <c r="O7" s="9" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A8" s="9" t="s">
-        <v>193</v>
-      </c>
-      <c r="B8" s="9" t="s">
-        <v>178</v>
-      </c>
-      <c r="C8" s="9" t="s">
-        <v>179</v>
-      </c>
-      <c r="D8" s="9" t="s">
-        <v>114</v>
-      </c>
-      <c r="E8" s="9" t="s">
-        <v>99</v>
-      </c>
-      <c r="F8" s="9" t="s">
-        <v>99</v>
-      </c>
-      <c r="G8" s="9" t="s">
-        <v>147</v>
-      </c>
-      <c r="H8" s="15" t="s">
-        <v>180</v>
-      </c>
-      <c r="I8" s="9" t="s">
-        <v>181</v>
-      </c>
-      <c r="J8" s="9" t="s">
-        <v>185</v>
-      </c>
-      <c r="K8" s="9" t="s">
-        <v>182</v>
-      </c>
-      <c r="L8" s="9" t="s">
-        <v>193</v>
-      </c>
-      <c r="M8" s="9" t="s">
-        <v>192</v>
-      </c>
-      <c r="N8" s="9" t="s">
-        <v>178</v>
-      </c>
-      <c r="O8" s="9" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A9" s="9" t="s">
-        <v>194</v>
-      </c>
-      <c r="B9" s="9" t="s">
-        <v>178</v>
-      </c>
-      <c r="C9" s="9" t="s">
-        <v>179</v>
-      </c>
-      <c r="D9" s="9" t="s">
-        <v>114</v>
-      </c>
-      <c r="E9" s="9" t="s">
-        <v>99</v>
-      </c>
-      <c r="F9" s="9" t="s">
-        <v>99</v>
-      </c>
-      <c r="G9" s="9" t="s">
-        <v>147</v>
-      </c>
-      <c r="H9" s="15" t="s">
-        <v>180</v>
-      </c>
-      <c r="I9" s="9" t="s">
-        <v>181</v>
-      </c>
-      <c r="J9" s="9" t="s">
-        <v>185</v>
-      </c>
-      <c r="K9" s="9" t="s">
-        <v>182</v>
-      </c>
-      <c r="L9" s="9" t="s">
-        <v>98</v>
-      </c>
-      <c r="M9" s="9" t="s">
-        <v>117</v>
-      </c>
-      <c r="N9" s="9" t="s">
-        <v>178</v>
-      </c>
-      <c r="O9" s="9" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A10" s="9" t="s">
-        <v>195</v>
-      </c>
-      <c r="B10" s="9" t="s">
-        <v>178</v>
-      </c>
-      <c r="C10" s="9" t="s">
-        <v>179</v>
-      </c>
-      <c r="D10" s="9" t="s">
-        <v>114</v>
-      </c>
-      <c r="E10" s="9" t="s">
-        <v>99</v>
-      </c>
-      <c r="F10" s="9" t="s">
-        <v>99</v>
-      </c>
-      <c r="G10" s="9" t="s">
-        <v>147</v>
-      </c>
-      <c r="H10" s="15" t="s">
-        <v>180</v>
-      </c>
-      <c r="I10" s="9" t="s">
-        <v>181</v>
-      </c>
-      <c r="J10" s="9" t="s">
-        <v>185</v>
-      </c>
-      <c r="K10" s="9" t="s">
-        <v>182</v>
-      </c>
-      <c r="L10" s="9" t="s">
-        <v>117</v>
-      </c>
-      <c r="M10" s="9" t="s">
-        <v>117</v>
-      </c>
-      <c r="N10" s="9" t="s">
-        <v>178</v>
-      </c>
-      <c r="O10" s="9" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A11" s="9" t="s">
-        <v>196</v>
-      </c>
-      <c r="B11" s="9" t="s">
-        <v>178</v>
-      </c>
-      <c r="C11" s="9" t="s">
-        <v>179</v>
-      </c>
-      <c r="D11" s="9" t="s">
-        <v>114</v>
-      </c>
-      <c r="E11" s="9" t="s">
-        <v>99</v>
-      </c>
-      <c r="F11" s="9" t="s">
-        <v>99</v>
-      </c>
-      <c r="G11" s="9" t="s">
-        <v>147</v>
-      </c>
-      <c r="H11" s="15" t="s">
-        <v>180</v>
-      </c>
-      <c r="I11" s="9" t="s">
-        <v>181</v>
-      </c>
-      <c r="J11" s="9" t="s">
-        <v>185</v>
-      </c>
-      <c r="K11" s="9" t="s">
-        <v>182</v>
-      </c>
-      <c r="L11" s="9" t="s">
-        <v>191</v>
-      </c>
-      <c r="M11" s="9" t="s">
-        <v>117</v>
-      </c>
-      <c r="N11" s="9" t="s">
-        <v>178</v>
-      </c>
-      <c r="O11" s="9" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A12" s="9" t="s">
-        <v>197</v>
-      </c>
-      <c r="B12" s="9" t="s">
-        <v>178</v>
-      </c>
-      <c r="C12" s="9" t="s">
-        <v>179</v>
-      </c>
-      <c r="D12" s="9" t="s">
-        <v>114</v>
-      </c>
-      <c r="E12" s="9" t="s">
-        <v>99</v>
-      </c>
-      <c r="F12" s="9" t="s">
-        <v>99</v>
-      </c>
-      <c r="G12" s="9" t="s">
-        <v>147</v>
-      </c>
-      <c r="H12" s="15" t="s">
-        <v>180</v>
-      </c>
-      <c r="I12" s="9" t="s">
-        <v>181</v>
-      </c>
-      <c r="J12" s="9" t="s">
-        <v>185</v>
-      </c>
-      <c r="K12" s="9" t="s">
-        <v>182</v>
-      </c>
-      <c r="L12" s="9" t="s">
-        <v>193</v>
-      </c>
-      <c r="M12" s="9" t="s">
-        <v>117</v>
-      </c>
-      <c r="N12" s="9" t="s">
-        <v>178</v>
-      </c>
-      <c r="O12" s="9" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A13" s="9" t="s">
-        <v>198</v>
-      </c>
-      <c r="B13" s="9" t="s">
-        <v>178</v>
-      </c>
-      <c r="C13" s="9" t="s">
-        <v>179</v>
-      </c>
-      <c r="D13" s="9" t="s">
-        <v>114</v>
-      </c>
-      <c r="E13" s="9" t="s">
-        <v>99</v>
-      </c>
-      <c r="F13" s="9" t="s">
-        <v>99</v>
-      </c>
-      <c r="G13" s="9" t="s">
-        <v>147</v>
-      </c>
-      <c r="H13" s="15" t="s">
-        <v>180</v>
-      </c>
-      <c r="I13" s="9" t="s">
-        <v>181</v>
-      </c>
-      <c r="J13" s="9" t="s">
-        <v>185</v>
-      </c>
-      <c r="K13" s="9" t="s">
-        <v>182</v>
-      </c>
-      <c r="L13" s="9" t="s">
-        <v>192</v>
-      </c>
-      <c r="M13" s="9" t="s">
-        <v>117</v>
-      </c>
-      <c r="N13" s="9" t="s">
-        <v>178</v>
-      </c>
-      <c r="O13" s="9" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A14" s="9" t="s">
-        <v>199</v>
-      </c>
-      <c r="B14" s="9" t="s">
-        <v>178</v>
-      </c>
-      <c r="C14" s="9" t="s">
-        <v>179</v>
-      </c>
-      <c r="D14" s="9" t="s">
-        <v>114</v>
-      </c>
-      <c r="E14" s="9" t="s">
-        <v>99</v>
-      </c>
-      <c r="F14" s="9" t="s">
-        <v>99</v>
-      </c>
-      <c r="G14" s="9" t="s">
-        <v>147</v>
-      </c>
-      <c r="H14" s="15" t="s">
-        <v>180</v>
-      </c>
-      <c r="I14" s="9" t="s">
-        <v>181</v>
-      </c>
-      <c r="J14" s="9" t="s">
-        <v>185</v>
-      </c>
-      <c r="K14" s="9" t="s">
-        <v>182</v>
-      </c>
-      <c r="L14" s="9" t="s">
-        <v>117</v>
-      </c>
-      <c r="M14" s="9" t="s">
-        <v>117</v>
-      </c>
-      <c r="N14" s="9" t="s">
-        <v>178</v>
-      </c>
-      <c r="O14" s="9" t="s">
-        <v>203</v>
+      <c r="B2" s="7" t="s">
+        <v>130</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>132</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>135</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>136</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>138</v>
+      </c>
+      <c r="G2" s="7" t="s">
+        <v>140</v>
+      </c>
+      <c r="H2" s="7" t="s">
+        <v>144</v>
+      </c>
+      <c r="I2" s="7" t="s">
+        <v>143</v>
+      </c>
+      <c r="J2" s="7" t="s">
+        <v>150</v>
+      </c>
+      <c r="K2" s="7" t="s">
+        <v>146</v>
+      </c>
+      <c r="L2" s="7" t="s">
+        <v>148</v>
+      </c>
+      <c r="M2" s="7" t="s">
+        <v>152</v>
+      </c>
+      <c r="N2" s="7" t="s">
+        <v>154</v>
+      </c>
+      <c r="O2" s="7" t="s">
+        <v>156</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="6" type="noConversion"/>
-  <hyperlinks>
-    <hyperlink ref="H3" r:id="rId1" xr:uid="{DFD74E29-D273-4805-B496-72D456495F15}"/>
-    <hyperlink ref="H4" r:id="rId2" xr:uid="{913AF339-92F9-4A30-AF6D-F6F7851D4855}"/>
-    <hyperlink ref="H5" r:id="rId3" xr:uid="{FB385679-6EAF-4646-884A-0E1F6A1405D6}"/>
-    <hyperlink ref="H6" r:id="rId4" xr:uid="{201E1320-C7A6-460A-A532-DA3CD3CEFF4D}"/>
-    <hyperlink ref="H7" r:id="rId5" xr:uid="{03C0343A-487B-4774-B7D2-B39772EADD0A}"/>
-    <hyperlink ref="H8" r:id="rId6" xr:uid="{941D56E1-E801-47ED-9A22-DDE59A567A7B}"/>
-    <hyperlink ref="H9" r:id="rId7" xr:uid="{73AB2EBC-7F01-485B-82F5-DE4EB358507B}"/>
-    <hyperlink ref="H10" r:id="rId8" xr:uid="{05579D94-AE7B-450B-B1B3-BF0E4C5D83AC}"/>
-    <hyperlink ref="H11" r:id="rId9" xr:uid="{AC67AA11-A167-4FC4-9B86-5610129AE4FA}"/>
-    <hyperlink ref="H12" r:id="rId10" xr:uid="{1C817A0D-7D06-4BF0-849F-C18858065C79}"/>
-    <hyperlink ref="H13" r:id="rId11" xr:uid="{4F882C98-A634-4820-8120-E6319CF16CB9}"/>
-    <hyperlink ref="H14" r:id="rId12" xr:uid="{19074FCD-10BB-4A5E-B322-BCEABE884FB5}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -2533,132 +1772,138 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35B69A6E-98BC-434D-A419-FDB6C97F2A28}">
   <dimension ref="A1:E38"/>
   <sheetViews>
-    <sheetView topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="E30" sqref="E30"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="24.44140625" style="6" customWidth="1"/>
-    <col min="2" max="2" width="28.21875" style="6" customWidth="1"/>
-    <col min="3" max="3" width="30.33203125" style="6" customWidth="1"/>
-    <col min="4" max="4" width="32.6640625" style="7" customWidth="1"/>
-    <col min="5" max="5" width="38.88671875" style="6" customWidth="1"/>
-    <col min="6" max="16384" width="8.88671875" style="6"/>
+    <col min="1" max="1" width="24.44140625" style="4" customWidth="1"/>
+    <col min="2" max="2" width="28.21875" style="4" customWidth="1"/>
+    <col min="3" max="3" width="30.33203125" style="4" customWidth="1"/>
+    <col min="4" max="4" width="32.6640625" style="5" customWidth="1"/>
+    <col min="5" max="5" width="38.88671875" style="4" customWidth="1"/>
+    <col min="6" max="16384" width="8.88671875" style="4"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="4" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="6" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3" s="8" t="s">
+      <c r="A3" s="6" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4" s="8"/>
+      <c r="A4" s="6"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A5" s="8"/>
+      <c r="A5" s="6"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A6" s="8"/>
+      <c r="A6" s="6"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A7" s="8"/>
+      <c r="A7" s="6"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A8" s="8"/>
+      <c r="A8" s="6"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A9" s="8"/>
+      <c r="A9" s="6"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A10" s="8"/>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A11" s="8"/>
+      <c r="A10" s="6"/>
+    </row>
+    <row r="11" spans="1:5" ht="34.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="20" t="s">
+        <v>158</v>
+      </c>
+      <c r="B11" s="21"/>
+      <c r="C11" s="21"/>
+      <c r="D11" s="21"/>
+      <c r="E11" s="21"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A12" s="8"/>
+      <c r="A12" s="6"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A13" s="8"/>
+      <c r="A13" s="6"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A14" s="8"/>
+      <c r="A14" s="6"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A15" s="8"/>
+      <c r="A15" s="6"/>
     </row>
     <row r="16" spans="1:5" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="17" t="s">
+      <c r="A16" s="14" t="s">
         <v>45</v>
       </c>
-      <c r="B16" s="18"/>
-      <c r="C16" s="18"/>
-      <c r="D16" s="18"/>
-      <c r="E16" s="18"/>
+      <c r="B16" s="15"/>
+      <c r="C16" s="15"/>
+      <c r="D16" s="15"/>
+      <c r="E16" s="15"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A17" s="5" t="s">
+      <c r="A17" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="B17" s="19" t="s">
+      <c r="B17" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="C17" s="19"/>
-      <c r="D17" s="19"/>
-      <c r="E17" s="5" t="s">
+      <c r="C17" s="16"/>
+      <c r="D17" s="16"/>
+      <c r="E17" s="3" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A18" s="3" t="s">
+      <c r="A18" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="B18" s="20" t="s">
+      <c r="B18" s="17" t="s">
         <v>47</v>
       </c>
-      <c r="C18" s="20"/>
-      <c r="D18" s="20"/>
-      <c r="E18" s="3"/>
+      <c r="C18" s="17"/>
+      <c r="D18" s="17"/>
+      <c r="E18" s="1"/>
     </row>
     <row r="19" spans="1:5" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="3" t="s">
+      <c r="A19" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="B19" s="21" t="s">
+      <c r="B19" s="18" t="s">
         <v>50</v>
       </c>
-      <c r="C19" s="21"/>
-      <c r="D19" s="21"/>
-      <c r="E19" s="3"/>
+      <c r="C19" s="18"/>
+      <c r="D19" s="18"/>
+      <c r="E19" s="1"/>
     </row>
     <row r="20" spans="1:5" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="3" t="s">
+      <c r="A20" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B20" s="21" t="s">
+      <c r="B20" s="18" t="s">
         <v>51</v>
       </c>
-      <c r="C20" s="21"/>
-      <c r="D20" s="21"/>
-      <c r="E20" s="3"/>
+      <c r="C20" s="18"/>
+      <c r="D20" s="18"/>
+      <c r="E20" s="1"/>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A21" s="3"/>
-      <c r="B21" s="20"/>
-      <c r="C21" s="20"/>
-      <c r="D21" s="20"/>
-      <c r="E21" s="3"/>
+      <c r="A21" s="1"/>
+      <c r="B21" s="17"/>
+      <c r="C21" s="17"/>
+      <c r="D21" s="17"/>
+      <c r="E21" s="1"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22"/>
@@ -2673,152 +1918,153 @@
       <c r="A25"/>
     </row>
     <row r="26" spans="1:5" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="17" t="s">
+      <c r="A26" s="14" t="s">
         <v>53</v>
       </c>
-      <c r="B26" s="18"/>
-      <c r="C26" s="18"/>
-      <c r="D26" s="18"/>
-      <c r="E26" s="18"/>
+      <c r="B26" s="15"/>
+      <c r="C26" s="15"/>
+      <c r="D26" s="15"/>
+      <c r="E26" s="15"/>
     </row>
     <row r="27" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="12" t="s">
+      <c r="A27" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="B27" s="12" t="s">
+      <c r="B27" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="C27" s="12" t="s">
+      <c r="C27" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="D27" s="13" t="s">
+      <c r="D27" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="E27" s="13" t="s">
+      <c r="E27" s="11" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="28" spans="1:5" ht="36" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="3" t="s">
+      <c r="A28" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B28" s="3" t="s">
+      <c r="B28" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C28" s="3" t="s">
+      <c r="C28" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D28" s="4" t="s">
+      <c r="D28" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="E28" s="4"/>
+      <c r="E28" s="2"/>
     </row>
     <row r="29" spans="1:5" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A29" s="3" t="s">
+      <c r="A29" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="B29" s="3" t="s">
+      <c r="B29" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="C29" s="3" t="s">
+      <c r="C29" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="D29" s="4" t="s">
+      <c r="D29" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="E29" s="4" t="s">
+      <c r="E29" s="2" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="30" spans="1:5" ht="55.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="3" t="s">
+      <c r="A30" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B30" s="3" t="s">
+      <c r="B30" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="C30" s="3" t="s">
+      <c r="C30" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D30" s="4" t="s">
+      <c r="D30" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="E30" s="4"/>
+      <c r="E30" s="2"/>
     </row>
     <row r="31" spans="1:5" ht="62.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="3" t="s">
+      <c r="A31" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B31" s="3" t="s">
+      <c r="B31" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C31" s="3" t="s">
+      <c r="C31" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="D31" s="4" t="s">
+      <c r="D31" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="E31" s="4"/>
+      <c r="E31" s="2"/>
     </row>
     <row r="32" spans="1:5" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="3" t="s">
+      <c r="A32" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B32" s="3" t="s">
+      <c r="B32" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="C32" s="3" t="s">
+      <c r="C32" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="D32" s="4" t="s">
+      <c r="D32" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="E32" s="4"/>
+      <c r="E32" s="2"/>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A33" s="3"/>
-      <c r="B33" s="3"/>
-      <c r="C33" s="3"/>
-      <c r="D33" s="4"/>
-      <c r="E33" s="4"/>
+      <c r="A33" s="1"/>
+      <c r="B33" s="1"/>
+      <c r="C33" s="1"/>
+      <c r="D33" s="2"/>
+      <c r="E33" s="2"/>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A34" s="3"/>
-      <c r="B34" s="3"/>
-      <c r="C34" s="3"/>
-      <c r="D34" s="4"/>
-      <c r="E34" s="4"/>
+      <c r="A34" s="1"/>
+      <c r="B34" s="1"/>
+      <c r="C34" s="1"/>
+      <c r="D34" s="2"/>
+      <c r="E34" s="2"/>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A35" s="3"/>
-      <c r="B35" s="3"/>
-      <c r="C35" s="3"/>
-      <c r="D35" s="4"/>
-      <c r="E35" s="4"/>
+      <c r="A35" s="1"/>
+      <c r="B35" s="1"/>
+      <c r="C35" s="1"/>
+      <c r="D35" s="2"/>
+      <c r="E35" s="2"/>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A36" s="3"/>
-      <c r="B36" s="3"/>
-      <c r="C36" s="3"/>
-      <c r="D36" s="4"/>
-      <c r="E36" s="4"/>
+      <c r="A36" s="1"/>
+      <c r="B36" s="1"/>
+      <c r="C36" s="1"/>
+      <c r="D36" s="2"/>
+      <c r="E36" s="2"/>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A37" s="3"/>
-      <c r="B37" s="3"/>
-      <c r="C37" s="3"/>
-      <c r="D37" s="4"/>
-      <c r="E37" s="4"/>
+      <c r="A37" s="1"/>
+      <c r="B37" s="1"/>
+      <c r="C37" s="1"/>
+      <c r="D37" s="2"/>
+      <c r="E37" s="2"/>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A38" s="3"/>
-      <c r="B38" s="3"/>
-      <c r="C38" s="3"/>
-      <c r="D38" s="4"/>
-      <c r="E38" s="4"/>
+      <c r="A38" s="1"/>
+      <c r="B38" s="1"/>
+      <c r="C38" s="1"/>
+      <c r="D38" s="2"/>
+      <c r="E38" s="2"/>
     </row>
   </sheetData>
-  <mergeCells count="7">
+  <mergeCells count="8">
+    <mergeCell ref="A11:E11"/>
     <mergeCell ref="A16:E16"/>
     <mergeCell ref="A26:E26"/>
     <mergeCell ref="B17:D17"/>
@@ -2840,43 +2086,43 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="C10" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.88671875" style="9"/>
-    <col min="2" max="2" width="48.44140625" style="9" customWidth="1"/>
-    <col min="3" max="3" width="40" style="9" customWidth="1"/>
-    <col min="4" max="4" width="47.6640625" style="9" customWidth="1"/>
-    <col min="5" max="16384" width="8.88671875" style="9"/>
+    <col min="1" max="1" width="8.88671875" style="7"/>
+    <col min="2" max="2" width="48.44140625" style="7" customWidth="1"/>
+    <col min="3" max="3" width="40" style="7" customWidth="1"/>
+    <col min="4" max="4" width="47.6640625" style="7" customWidth="1"/>
+    <col min="5" max="16384" width="8.88671875" style="7"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="B1" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="C1" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="D1" s="10" t="s">
+      <c r="D1" s="8" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="75.599999999999994" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="9" t="s">
+      <c r="A2" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="B2" s="9" t="s">
+      <c r="B2" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="C2" s="9" t="s">
+      <c r="C2" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="D2" s="9" t="s">
+      <c r="D2" s="7" t="s">
         <v>56</v>
       </c>
     </row>
@@ -2890,91 +2136,91 @@
   <dimension ref="A1:K2"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+      <selection activeCell="D8" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.6640625" style="2" customWidth="1"/>
-    <col min="2" max="3" width="19.21875" style="2" customWidth="1"/>
-    <col min="4" max="4" width="18.77734375" style="2" customWidth="1"/>
-    <col min="5" max="5" width="28.109375" style="2" customWidth="1"/>
-    <col min="6" max="6" width="20.21875" style="2" customWidth="1"/>
-    <col min="7" max="7" width="17.44140625" style="2" customWidth="1"/>
-    <col min="8" max="8" width="18" style="2" customWidth="1"/>
-    <col min="9" max="9" width="19.109375" style="2" customWidth="1"/>
-    <col min="10" max="10" width="16.21875" style="2" customWidth="1"/>
-    <col min="11" max="11" width="18.109375" style="2" customWidth="1"/>
-    <col min="12" max="16384" width="8.88671875" style="2"/>
+    <col min="1" max="1" width="8.6640625" style="9" customWidth="1"/>
+    <col min="2" max="3" width="19.21875" style="9" customWidth="1"/>
+    <col min="4" max="4" width="18.77734375" style="9" customWidth="1"/>
+    <col min="5" max="5" width="28.109375" style="9" customWidth="1"/>
+    <col min="6" max="6" width="20.21875" style="9" customWidth="1"/>
+    <col min="7" max="7" width="17.44140625" style="9" customWidth="1"/>
+    <col min="8" max="8" width="18" style="9" customWidth="1"/>
+    <col min="9" max="9" width="19.109375" style="9" customWidth="1"/>
+    <col min="10" max="10" width="16.21875" style="9" customWidth="1"/>
+    <col min="11" max="11" width="18.109375" style="9" customWidth="1"/>
+    <col min="12" max="16384" width="8.88671875" style="9"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="19" t="s">
         <v>94</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J1" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="K1" s="19" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:11" ht="146.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="9" t="s">
+      <c r="A2" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="B2" s="9" t="s">
+      <c r="B2" s="7" t="s">
         <v>91</v>
       </c>
-      <c r="C2" s="9" t="s">
+      <c r="C2" s="7" t="s">
         <v>87</v>
       </c>
-      <c r="D2" s="9" t="s">
+      <c r="D2" s="7" t="s">
         <v>88</v>
       </c>
-      <c r="E2" s="9" t="s">
+      <c r="E2" s="7" t="s">
         <v>90</v>
       </c>
-      <c r="F2" s="9" t="s">
+      <c r="F2" s="7" t="s">
         <v>89</v>
       </c>
-      <c r="G2" s="9" t="s">
+      <c r="G2" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="H2" s="9" t="s">
-        <v>204</v>
-      </c>
-      <c r="I2" s="9" t="s">
-        <v>204</v>
-      </c>
-      <c r="J2" s="9" t="s">
+      <c r="H2" s="7" t="s">
+        <v>157</v>
+      </c>
+      <c r="I2" s="7" t="s">
+        <v>157</v>
+      </c>
+      <c r="J2" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="K2" s="9" t="s">
+      <c r="K2" s="7" t="s">
         <v>86</v>
       </c>
     </row>
@@ -2988,50 +2234,50 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.88671875" style="9" customWidth="1"/>
-    <col min="2" max="2" width="23.44140625" style="9" customWidth="1"/>
-    <col min="3" max="3" width="25.33203125" style="9" customWidth="1"/>
-    <col min="4" max="4" width="20.109375" style="9" customWidth="1"/>
-    <col min="5" max="5" width="20.21875" style="9" customWidth="1"/>
-    <col min="6" max="16384" width="8.88671875" style="11"/>
+    <col min="1" max="1" width="10.88671875" style="7" customWidth="1"/>
+    <col min="2" max="2" width="23.44140625" style="7" customWidth="1"/>
+    <col min="3" max="3" width="25.33203125" style="7" customWidth="1"/>
+    <col min="4" max="4" width="20.109375" style="7" customWidth="1"/>
+    <col min="5" max="5" width="20.21875" style="7" customWidth="1"/>
+    <col min="6" max="16384" width="8.88671875" style="9"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="B1" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="C1" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="D1" s="10" t="s">
+      <c r="D1" s="8" t="s">
         <v>83</v>
       </c>
-      <c r="E1" s="10" t="s">
+      <c r="E1" s="8" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="91.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="9" t="s">
+      <c r="A2" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="B2" s="9" t="s">
+      <c r="B2" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="C2" s="9" t="s">
+      <c r="C2" s="7" t="s">
         <v>68</v>
       </c>
-      <c r="D2" s="9" t="s">
+      <c r="D2" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="E2" s="9" t="s">
+      <c r="E2" s="7" t="s">
         <v>70</v>
       </c>
     </row>
@@ -3045,92 +2291,92 @@
   <dimension ref="A1:K2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+      <selection activeCell="E8" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.21875" style="9" customWidth="1"/>
-    <col min="2" max="2" width="30.21875" style="9" customWidth="1"/>
-    <col min="3" max="3" width="25.33203125" style="9" customWidth="1"/>
-    <col min="4" max="4" width="16.21875" style="9" customWidth="1"/>
-    <col min="5" max="5" width="17.33203125" style="9" customWidth="1"/>
-    <col min="6" max="6" width="21.109375" style="9" customWidth="1"/>
-    <col min="7" max="7" width="18.33203125" style="9" customWidth="1"/>
-    <col min="8" max="8" width="19.5546875" style="9" customWidth="1"/>
-    <col min="9" max="9" width="23.77734375" style="9" customWidth="1"/>
-    <col min="10" max="10" width="17.88671875" style="9" customWidth="1"/>
-    <col min="11" max="11" width="20.21875" style="9" customWidth="1"/>
-    <col min="12" max="16384" width="8.88671875" style="11"/>
+    <col min="1" max="1" width="10.21875" style="7" customWidth="1"/>
+    <col min="2" max="2" width="30.21875" style="7" customWidth="1"/>
+    <col min="3" max="3" width="25.33203125" style="7" customWidth="1"/>
+    <col min="4" max="4" width="16.21875" style="7" customWidth="1"/>
+    <col min="5" max="5" width="17.33203125" style="7" customWidth="1"/>
+    <col min="6" max="6" width="21.109375" style="7" customWidth="1"/>
+    <col min="7" max="7" width="18.33203125" style="7" customWidth="1"/>
+    <col min="8" max="8" width="19.5546875" style="7" customWidth="1"/>
+    <col min="9" max="9" width="23.77734375" style="7" customWidth="1"/>
+    <col min="10" max="10" width="17.88671875" style="7" customWidth="1"/>
+    <col min="11" max="11" width="20.21875" style="7" customWidth="1"/>
+    <col min="12" max="16384" width="8.88671875" style="9"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="B1" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="C1" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="D1" s="10" t="s">
+      <c r="D1" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="E1" s="10" t="s">
+      <c r="E1" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="F1" s="10" t="s">
+      <c r="F1" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="G1" s="10" t="s">
+      <c r="G1" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="H1" s="10" t="s">
+      <c r="H1" s="8" t="s">
         <v>77</v>
       </c>
-      <c r="I1" s="10" t="s">
+      <c r="I1" s="8" t="s">
         <v>78</v>
       </c>
-      <c r="J1" s="10" t="s">
+      <c r="J1" s="8" t="s">
         <v>79</v>
       </c>
-      <c r="K1" s="10" t="s">
+      <c r="K1" s="8" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="2" spans="1:11" ht="184.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="9" t="s">
+      <c r="A2" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="B2" s="9" t="s">
+      <c r="B2" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="C2" s="9" t="s">
+      <c r="C2" s="7" t="s">
         <v>72</v>
       </c>
-      <c r="D2" s="9" t="s">
+      <c r="D2" s="7" t="s">
         <v>73</v>
       </c>
-      <c r="E2" s="9" t="s">
+      <c r="E2" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="F2" s="9" t="s">
+      <c r="F2" s="7" t="s">
         <v>75</v>
       </c>
-      <c r="G2" s="9" t="s">
+      <c r="G2" s="7" t="s">
         <v>85</v>
       </c>
-      <c r="H2" s="9" t="s">
+      <c r="H2" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="I2" s="9" t="s">
+      <c r="I2" s="7" t="s">
         <v>81</v>
       </c>
-      <c r="J2" s="9" t="s">
+      <c r="J2" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="K2" s="9" t="s">
+      <c r="K2" s="7" t="s">
         <v>82</v>
       </c>
     </row>
@@ -3141,61 +2387,47 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0006E928-76FF-46D6-8C3B-F76222261BB1}">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.88671875" style="9"/>
-    <col min="2" max="2" width="27" style="9" customWidth="1"/>
-    <col min="3" max="3" width="21.77734375" style="9" customWidth="1"/>
-    <col min="4" max="4" width="42.6640625" style="9" customWidth="1"/>
-    <col min="5" max="16384" width="8.88671875" style="9"/>
+    <col min="1" max="1" width="8.88671875" style="7"/>
+    <col min="2" max="2" width="27" style="7" customWidth="1"/>
+    <col min="3" max="3" width="21.77734375" style="7" customWidth="1"/>
+    <col min="4" max="4" width="42.6640625" style="7" customWidth="1"/>
+    <col min="5" max="16384" width="8.88671875" style="7"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="B1" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="C1" s="8" t="s">
+        <v>98</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A2" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>100</v>
+      </c>
+      <c r="D2" s="7" t="s">
         <v>102</v>
-      </c>
-      <c r="D1" s="10" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A2" s="9" t="s">
-        <v>55</v>
-      </c>
-      <c r="B2" s="9" t="s">
-        <v>105</v>
-      </c>
-      <c r="C2" s="9" t="s">
-        <v>104</v>
-      </c>
-      <c r="D2" s="9" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" s="9" t="s">
-        <v>98</v>
-      </c>
-      <c r="B3" s="9" t="s">
-        <v>107</v>
-      </c>
-      <c r="C3" s="9" t="s">
-        <v>98</v>
-      </c>
-      <c r="D3" s="9" t="s">
-        <v>107</v>
       </c>
     </row>
   </sheetData>
@@ -3205,58 +2437,44 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{709BFA93-CCDF-43DC-B3BF-04DACD72B0E2}">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="C10" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.88671875" style="9"/>
-    <col min="2" max="2" width="27" style="9" customWidth="1"/>
-    <col min="3" max="3" width="37.44140625" style="9" customWidth="1"/>
-    <col min="4" max="4" width="42.6640625" style="9" customWidth="1"/>
-    <col min="5" max="16384" width="8.88671875" style="9"/>
+    <col min="1" max="1" width="8.88671875" style="7"/>
+    <col min="2" max="2" width="27" style="7" customWidth="1"/>
+    <col min="3" max="3" width="37.44140625" style="7" customWidth="1"/>
+    <col min="4" max="4" width="42.6640625" style="7" customWidth="1"/>
+    <col min="5" max="16384" width="8.88671875" style="7"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="B1" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="C1" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="10" t="s">
+      <c r="D1" s="8" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="9" t="s">
+      <c r="A2" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="B2" s="9" t="s">
-        <v>105</v>
-      </c>
-      <c r="C2" s="9" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" s="9" t="s">
-        <v>98</v>
-      </c>
-      <c r="B3" s="9" t="s">
-        <v>108</v>
-      </c>
-      <c r="C3" s="9" t="s">
-        <v>109</v>
-      </c>
-      <c r="D3" s="9" t="s">
-        <v>110</v>
+      <c r="B2" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>104</v>
       </c>
     </row>
   </sheetData>
@@ -3266,72 +2484,44 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1359912D-CDDC-4C74-BCFB-CBE40EB489F2}">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+      <selection activeCell="D8" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.88671875" style="9"/>
-    <col min="2" max="2" width="27" style="9" customWidth="1"/>
-    <col min="3" max="3" width="37.44140625" style="9" customWidth="1"/>
-    <col min="4" max="4" width="42.6640625" style="9" customWidth="1"/>
-    <col min="5" max="16384" width="8.88671875" style="9"/>
+    <col min="1" max="1" width="8.88671875" style="7"/>
+    <col min="2" max="2" width="27" style="7" customWidth="1"/>
+    <col min="3" max="3" width="37.44140625" style="7" customWidth="1"/>
+    <col min="4" max="4" width="42.6640625" style="7" customWidth="1"/>
+    <col min="5" max="16384" width="8.88671875" style="7"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="B1" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="C1" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="10" t="s">
+      <c r="D1" s="8" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="9" t="s">
+      <c r="A2" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="B2" s="9" t="s">
-        <v>111</v>
-      </c>
-      <c r="C2" s="9" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" s="9" t="s">
-        <v>98</v>
-      </c>
-      <c r="B3" s="9" t="s">
-        <v>114</v>
-      </c>
-      <c r="C3" s="9" t="s">
-        <v>115</v>
-      </c>
-      <c r="D3" s="9" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" s="9" t="s">
-        <v>117</v>
-      </c>
-      <c r="B4" s="9" t="s">
-        <v>118</v>
-      </c>
-      <c r="C4" s="9" t="s">
-        <v>115</v>
-      </c>
-      <c r="D4" s="9" t="s">
-        <v>116</v>
+      <c r="B2" s="7" t="s">
+        <v>103</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>105</v>
       </c>
     </row>
   </sheetData>
@@ -3341,72 +2531,44 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ACBC7503-D39D-4D5C-B33A-E4C15DD2E38F}">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="I17" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.88671875" style="9"/>
-    <col min="2" max="2" width="27" style="9" customWidth="1"/>
-    <col min="3" max="3" width="37.44140625" style="9" customWidth="1"/>
-    <col min="4" max="4" width="42.6640625" style="9" customWidth="1"/>
-    <col min="5" max="16384" width="8.88671875" style="9"/>
+    <col min="1" max="1" width="8.88671875" style="7"/>
+    <col min="2" max="2" width="27" style="7" customWidth="1"/>
+    <col min="3" max="3" width="37.44140625" style="7" customWidth="1"/>
+    <col min="4" max="4" width="42.6640625" style="7" customWidth="1"/>
+    <col min="5" max="16384" width="8.88671875" style="7"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="B1" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="C1" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="10" t="s">
+      <c r="D1" s="8" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="9" t="s">
+      <c r="A2" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="B2" s="9" t="s">
-        <v>120</v>
-      </c>
-      <c r="C2" s="9" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" s="9" t="s">
-        <v>98</v>
-      </c>
-      <c r="B3" s="9" t="s">
-        <v>99</v>
-      </c>
-      <c r="C3" s="9" t="s">
-        <v>121</v>
-      </c>
-      <c r="D3" s="9" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" s="9" t="s">
-        <v>117</v>
-      </c>
-      <c r="B4" s="9" t="s">
-        <v>123</v>
-      </c>
-      <c r="C4" s="9" t="s">
-        <v>124</v>
-      </c>
-      <c r="D4" s="9" t="s">
-        <v>125</v>
+      <c r="B2" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>106</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[SIT] Fix columns import employee
</commit_message>
<xml_diff>
--- a/apps/core/fimport/static/fimport/template/mega-import.xlsx
+++ b/apps/core/fimport/static/fimport/template/mega-import.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\Coding\MIS\misui\apps\core\fimport\static\fimport\template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6CBB119-1C27-41D8-A9EE-7954E538AF5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D409DE9-B636-4ACE-8CA5-3FBC9E7B03A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="803" firstSheet="7" activeTab="13" xr2:uid="{ABCF866D-F0C2-489F-81F3-6B45D3E3629E}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="803" activeTab="2" xr2:uid="{ABCF866D-F0C2-489F-81F3-6B45D3E3629E}"/>
   </bookViews>
   <sheets>
     <sheet name="#account.users" sheetId="1" r:id="rId1"/>
@@ -344,18 +344,6 @@
     <t>- Mã của vai trò tại #hr.roles
 - Danh sách mã vai trò liên kết với nhau bằng dấu phẩy.
 - Ví dụ: QL</t>
-  </si>
-  <si>
-    <t>- Bắt buộc
-- Độ dài tối đa: 100
-- Tên của nhân viên
-- Ví dụ: Nguyễn Văn</t>
-  </si>
-  <si>
-    <t>- Bắt buộc
-- Độ dài tối đa: 100
-- Họ của nhân viên
-- Ví dụ: A</t>
   </si>
   <si>
     <t>- Bắt buộc
@@ -846,6 +834,18 @@
   </si>
   <si>
     <t>Luôn giữ kiểu của ô là text để trình đọc dữ liệu có thể hiểu</t>
+  </si>
+  <si>
+    <t>- Bắt buộc
+- Độ dài tối đa: 100
+- Tên của nhân viên
+- Ví dụ: A</t>
+  </si>
+  <si>
+    <t>- Bắt buộc
+- Độ dài tối đa: 100
+- Họ của nhân viên
+- Ví dụ: Nguyễn Văn</t>
   </si>
 </sst>
 </file>
@@ -1029,6 +1029,15 @@
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1043,15 +1052,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1466,10 +1466,10 @@
         <v>4</v>
       </c>
       <c r="D1" s="8" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="E1" s="8" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="F1" s="8" t="s">
         <v>19</v>
@@ -1480,16 +1480,16 @@
         <v>55</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
   </sheetData>
@@ -1533,31 +1533,31 @@
         <v>10</v>
       </c>
       <c r="C1" s="8" t="s">
+        <v>111</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="E1" s="8" t="s">
         <v>113</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="F1" s="8" t="s">
+        <v>116</v>
+      </c>
+      <c r="G1" s="8" t="s">
         <v>114</v>
       </c>
-      <c r="E1" s="8" t="s">
+      <c r="H1" s="8" t="s">
+        <v>124</v>
+      </c>
+      <c r="I1" s="8" t="s">
+        <v>125</v>
+      </c>
+      <c r="J1" s="8" t="s">
+        <v>122</v>
+      </c>
+      <c r="K1" s="8" t="s">
         <v>115</v>
-      </c>
-      <c r="F1" s="8" t="s">
-        <v>118</v>
-      </c>
-      <c r="G1" s="8" t="s">
-        <v>116</v>
-      </c>
-      <c r="H1" s="8" t="s">
-        <v>126</v>
-      </c>
-      <c r="I1" s="8" t="s">
-        <v>127</v>
-      </c>
-      <c r="J1" s="8" t="s">
-        <v>124</v>
-      </c>
-      <c r="K1" s="8" t="s">
-        <v>117</v>
       </c>
     </row>
     <row r="2" spans="1:11" ht="85.8" customHeight="1" x14ac:dyDescent="0.3">
@@ -1565,31 +1565,31 @@
         <v>55</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C2" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="E2" s="7" t="s">
         <v>119</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="F2" s="7" t="s">
         <v>120</v>
       </c>
-      <c r="E2" s="7" t="s">
+      <c r="G2" s="7" t="s">
         <v>121</v>
       </c>
-      <c r="F2" s="7" t="s">
-        <v>122</v>
-      </c>
-      <c r="G2" s="7" t="s">
+      <c r="H2" s="7" t="s">
+        <v>126</v>
+      </c>
+      <c r="I2" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="J2" s="7" t="s">
         <v>123</v>
-      </c>
-      <c r="H2" s="7" t="s">
-        <v>128</v>
-      </c>
-      <c r="I2" s="7" t="s">
-        <v>129</v>
-      </c>
-      <c r="J2" s="7" t="s">
-        <v>125</v>
       </c>
     </row>
   </sheetData>
@@ -1633,13 +1633,13 @@
         <v>55</v>
       </c>
       <c r="B2" s="12" t="s">
+        <v>93</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="D2" s="7" t="s">
         <v>95</v>
-      </c>
-      <c r="C2" s="7" t="s">
-        <v>96</v>
-      </c>
-      <c r="D2" s="7" t="s">
-        <v>97</v>
       </c>
     </row>
   </sheetData>
@@ -1676,43 +1676,43 @@
         <v>10</v>
       </c>
       <c r="C1" s="13" t="s">
+        <v>129</v>
+      </c>
+      <c r="D1" s="13" t="s">
         <v>131</v>
       </c>
-      <c r="D1" s="13" t="s">
-        <v>133</v>
-      </c>
       <c r="E1" s="13" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="F1" s="13" t="s">
+        <v>135</v>
+      </c>
+      <c r="G1" s="13" t="s">
         <v>137</v>
       </c>
-      <c r="G1" s="13" t="s">
+      <c r="H1" s="13" t="s">
         <v>139</v>
       </c>
-      <c r="H1" s="13" t="s">
-        <v>141</v>
-      </c>
       <c r="I1" s="13" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="J1" s="13" t="s">
+        <v>147</v>
+      </c>
+      <c r="K1" s="13" t="s">
+        <v>143</v>
+      </c>
+      <c r="L1" s="13" t="s">
+        <v>145</v>
+      </c>
+      <c r="M1" s="13" t="s">
         <v>149</v>
       </c>
-      <c r="K1" s="13" t="s">
-        <v>145</v>
-      </c>
-      <c r="L1" s="13" t="s">
-        <v>147</v>
-      </c>
-      <c r="M1" s="13" t="s">
+      <c r="N1" s="13" t="s">
         <v>151</v>
       </c>
-      <c r="N1" s="13" t="s">
+      <c r="O1" s="13" t="s">
         <v>153</v>
-      </c>
-      <c r="O1" s="13" t="s">
-        <v>155</v>
       </c>
     </row>
     <row r="2" spans="1:15" ht="147.6" customHeight="1" x14ac:dyDescent="0.3">
@@ -1720,46 +1720,46 @@
         <v>55</v>
       </c>
       <c r="B2" s="7" t="s">
+        <v>128</v>
+      </c>
+      <c r="C2" s="7" t="s">
         <v>130</v>
       </c>
-      <c r="C2" s="7" t="s">
-        <v>132</v>
-      </c>
       <c r="D2" s="7" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="E2" s="7" t="s">
+        <v>134</v>
+      </c>
+      <c r="F2" s="7" t="s">
         <v>136</v>
       </c>
-      <c r="F2" s="7" t="s">
+      <c r="G2" s="7" t="s">
         <v>138</v>
       </c>
-      <c r="G2" s="7" t="s">
-        <v>140</v>
-      </c>
       <c r="H2" s="7" t="s">
+        <v>142</v>
+      </c>
+      <c r="I2" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="J2" s="7" t="s">
+        <v>148</v>
+      </c>
+      <c r="K2" s="7" t="s">
         <v>144</v>
       </c>
-      <c r="I2" s="7" t="s">
-        <v>143</v>
-      </c>
-      <c r="J2" s="7" t="s">
+      <c r="L2" s="7" t="s">
+        <v>146</v>
+      </c>
+      <c r="M2" s="7" t="s">
         <v>150</v>
       </c>
-      <c r="K2" s="7" t="s">
-        <v>146</v>
-      </c>
-      <c r="L2" s="7" t="s">
-        <v>148</v>
-      </c>
-      <c r="M2" s="7" t="s">
+      <c r="N2" s="7" t="s">
         <v>152</v>
       </c>
-      <c r="N2" s="7" t="s">
+      <c r="O2" s="7" t="s">
         <v>154</v>
-      </c>
-      <c r="O2" s="7" t="s">
-        <v>156</v>
       </c>
     </row>
   </sheetData>
@@ -1772,7 +1772,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35B69A6E-98BC-434D-A419-FDB6C97F2A28}">
   <dimension ref="A1:E38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
@@ -1823,13 +1823,13 @@
       <c r="A10" s="6"/>
     </row>
     <row r="11" spans="1:5" ht="34.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="20" t="s">
-        <v>158</v>
-      </c>
-      <c r="B11" s="21"/>
-      <c r="C11" s="21"/>
-      <c r="D11" s="21"/>
-      <c r="E11" s="21"/>
+      <c r="A11" s="15" t="s">
+        <v>156</v>
+      </c>
+      <c r="B11" s="16"/>
+      <c r="C11" s="16"/>
+      <c r="D11" s="16"/>
+      <c r="E11" s="16"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="6"/>
@@ -1844,65 +1844,65 @@
       <c r="A15" s="6"/>
     </row>
     <row r="16" spans="1:5" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="14" t="s">
+      <c r="A16" s="17" t="s">
         <v>45</v>
       </c>
-      <c r="B16" s="15"/>
-      <c r="C16" s="15"/>
-      <c r="D16" s="15"/>
-      <c r="E16" s="15"/>
+      <c r="B16" s="18"/>
+      <c r="C16" s="18"/>
+      <c r="D16" s="18"/>
+      <c r="E16" s="18"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="B17" s="16" t="s">
+      <c r="B17" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="C17" s="16"/>
-      <c r="D17" s="16"/>
+      <c r="C17" s="19"/>
+      <c r="D17" s="19"/>
       <c r="E17" s="3" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="B18" s="17" t="s">
+      <c r="B18" s="20" t="s">
         <v>47</v>
       </c>
-      <c r="C18" s="17"/>
-      <c r="D18" s="17"/>
+      <c r="C18" s="20"/>
+      <c r="D18" s="20"/>
       <c r="E18" s="1"/>
     </row>
     <row r="19" spans="1:5" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="B19" s="18" t="s">
+      <c r="B19" s="21" t="s">
         <v>50</v>
       </c>
-      <c r="C19" s="18"/>
-      <c r="D19" s="18"/>
+      <c r="C19" s="21"/>
+      <c r="D19" s="21"/>
       <c r="E19" s="1"/>
     </row>
     <row r="20" spans="1:5" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B20" s="18" t="s">
+      <c r="B20" s="21" t="s">
         <v>51</v>
       </c>
-      <c r="C20" s="18"/>
-      <c r="D20" s="18"/>
+      <c r="C20" s="21"/>
+      <c r="D20" s="21"/>
       <c r="E20" s="1"/>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" s="1"/>
-      <c r="B21" s="17"/>
-      <c r="C21" s="17"/>
-      <c r="D21" s="17"/>
+      <c r="B21" s="20"/>
+      <c r="C21" s="20"/>
+      <c r="D21" s="20"/>
       <c r="E21" s="1"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
@@ -1918,13 +1918,13 @@
       <c r="A25"/>
     </row>
     <row r="26" spans="1:5" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="14" t="s">
+      <c r="A26" s="17" t="s">
         <v>53</v>
       </c>
-      <c r="B26" s="15"/>
-      <c r="C26" s="15"/>
-      <c r="D26" s="15"/>
-      <c r="E26" s="15"/>
+      <c r="B26" s="18"/>
+      <c r="C26" s="18"/>
+      <c r="D26" s="18"/>
+      <c r="E26" s="18"/>
     </row>
     <row r="27" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="10" t="s">
@@ -1940,7 +1940,7 @@
         <v>27</v>
       </c>
       <c r="E27" s="11" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="28" spans="1:5" ht="36" customHeight="1" x14ac:dyDescent="0.3">
@@ -1972,7 +1972,7 @@
         <v>43</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="30" spans="1:5" ht="55.8" customHeight="1" x14ac:dyDescent="0.3">
@@ -2135,8 +2135,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{18F2B7B4-0119-40B2-9AE3-A031B16A0EEC}">
   <dimension ref="A1:K2"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D8" sqref="A1:XFD1048576"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2155,37 +2155,37 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="19" t="s">
+      <c r="B1" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="C1" s="19" t="s">
+      <c r="C1" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="19" t="s">
+      <c r="D1" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="19" t="s">
+      <c r="E1" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="F1" s="19" t="s">
+      <c r="F1" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="G1" s="19" t="s">
+      <c r="G1" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="H1" s="19" t="s">
+      <c r="H1" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="I1" s="19" t="s">
-        <v>94</v>
-      </c>
-      <c r="J1" s="19" t="s">
+      <c r="I1" s="14" t="s">
+        <v>92</v>
+      </c>
+      <c r="J1" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="K1" s="19" t="s">
+      <c r="K1" s="14" t="s">
         <v>16</v>
       </c>
     </row>
@@ -2194,28 +2194,28 @@
         <v>55</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C2" s="7" t="s">
+        <v>157</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>158</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="F2" s="7" t="s">
         <v>87</v>
-      </c>
-      <c r="D2" s="7" t="s">
-        <v>88</v>
-      </c>
-      <c r="E2" s="7" t="s">
-        <v>90</v>
-      </c>
-      <c r="F2" s="7" t="s">
-        <v>89</v>
       </c>
       <c r="G2" s="7" t="s">
         <v>65</v>
       </c>
       <c r="H2" s="7" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="I2" s="7" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="J2" s="7" t="s">
         <v>66</v>
@@ -2410,10 +2410,10 @@
         <v>10</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D1" s="8" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
@@ -2421,13 +2421,13 @@
         <v>55</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C2" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="D2" s="7" t="s">
         <v>100</v>
-      </c>
-      <c r="D2" s="7" t="s">
-        <v>102</v>
       </c>
     </row>
   </sheetData>
@@ -2471,10 +2471,10 @@
         <v>55</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
   </sheetData>
@@ -2518,10 +2518,10 @@
         <v>55</v>
       </c>
       <c r="B2" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="C2" s="7" t="s">
         <v>103</v>
-      </c>
-      <c r="C2" s="7" t="s">
-        <v>105</v>
       </c>
     </row>
   </sheetData>
@@ -2565,10 +2565,10 @@
         <v>55</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[hotfix/master-viet] update file mega-import, update import product
</commit_message>
<xml_diff>
--- a/apps/core/fimport/static/fimport/template/mega-import.xlsx
+++ b/apps/core/fimport/static/fimport/template/mega-import.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PCAdmin\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABEA3A8B-9BE5-4699-82A0-C78F0B2BC594}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DA6F90D-0E20-46C4-8977-6FD6ABD89992}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="803" firstSheet="10" activeTab="16" xr2:uid="{ABCF866D-F0C2-489F-81F3-6B45D3E3629E}"/>
   </bookViews>
@@ -711,10 +711,6 @@
 -Mã nhóm đơn vị tính
 tại #saledata.product.uomgroup
 -Ví dụ: 001</t>
-  </si>
-  <si>
-    <t xml:space="preserve">- 0 là theo batch/Lot
-- 1 là theo serial num </t>
   </si>
   <si>
     <t>-Bắt buộc nếu mục đích sản phẩm có chứa [0]
@@ -1743,6 +1739,11 @@
   </si>
   <si>
     <t>nva@example.com</t>
+  </si>
+  <si>
+    <t>- 1 là theo batch/Lot
+- 2 là theo serial num 
+- 0 là không có</t>
   </si>
 </sst>
 </file>
@@ -1963,7 +1964,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -2032,6 +2033,52 @@
     <xf numFmtId="0" fontId="10" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="14" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2055,64 +2102,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2687,40 +2676,40 @@
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A3" s="33">
+      <c r="A3" s="25">
         <v>1</v>
       </c>
-      <c r="B3" s="33" t="s">
+      <c r="B3" s="25" t="s">
+        <v>405</v>
+      </c>
+      <c r="C3" s="25" t="s">
         <v>406</v>
       </c>
-      <c r="C3" s="33" t="s">
+      <c r="D3" s="25"/>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A4" s="25">
+        <v>2</v>
+      </c>
+      <c r="B4" s="25" t="s">
         <v>407</v>
       </c>
-      <c r="D3" s="33"/>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A4" s="33">
-        <v>2</v>
-      </c>
-      <c r="B4" s="33" t="s">
+      <c r="C4" s="25" t="s">
         <v>408</v>
       </c>
-      <c r="C4" s="33" t="s">
+      <c r="D4" s="25"/>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A5" s="25">
+        <v>3</v>
+      </c>
+      <c r="B5" s="25" t="s">
         <v>409</v>
       </c>
-      <c r="D4" s="33"/>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A5" s="33">
-        <v>3</v>
-      </c>
-      <c r="B5" s="33" t="s">
+      <c r="C5" s="25" t="s">
         <v>410</v>
       </c>
-      <c r="C5" s="33" t="s">
-        <v>411</v>
-      </c>
-      <c r="D5" s="33"/>
+      <c r="D5" s="25"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2770,52 +2759,52 @@
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A3" s="33">
+      <c r="A3" s="25">
         <v>1</v>
       </c>
-      <c r="B3" s="33" t="s">
+      <c r="B3" s="25" t="s">
+        <v>411</v>
+      </c>
+      <c r="C3" s="25" t="s">
+        <v>121</v>
+      </c>
+      <c r="D3" s="25"/>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A4" s="25">
+        <v>2</v>
+      </c>
+      <c r="B4" s="25" t="s">
         <v>412</v>
       </c>
-      <c r="C3" s="33" t="s">
-        <v>121</v>
-      </c>
-      <c r="D3" s="33"/>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A4" s="33">
-        <v>2</v>
-      </c>
-      <c r="B4" s="33" t="s">
+      <c r="C4" s="25" t="s">
+        <v>122</v>
+      </c>
+      <c r="D4" s="25"/>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A5" s="25">
+        <v>3</v>
+      </c>
+      <c r="B5" s="25" t="s">
         <v>413</v>
       </c>
-      <c r="C4" s="33" t="s">
-        <v>122</v>
-      </c>
-      <c r="D4" s="33"/>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A5" s="33">
-        <v>3</v>
-      </c>
-      <c r="B5" s="33" t="s">
+      <c r="C5" s="25" t="s">
+        <v>123</v>
+      </c>
+      <c r="D5" s="25"/>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A6" s="25">
+        <v>4</v>
+      </c>
+      <c r="B6" s="25" t="s">
         <v>414</v>
       </c>
-      <c r="C5" s="33" t="s">
-        <v>123</v>
-      </c>
-      <c r="D5" s="33"/>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A6" s="33">
-        <v>4</v>
-      </c>
-      <c r="B6" s="33" t="s">
-        <v>415</v>
-      </c>
-      <c r="C6" s="33" t="s">
+      <c r="C6" s="25" t="s">
         <v>124</v>
       </c>
-      <c r="D6" s="33"/>
+      <c r="D6" s="25"/>
     </row>
   </sheetData>
   <phoneticPr fontId="6" type="noConversion"/>
@@ -2945,116 +2934,116 @@
       </c>
     </row>
     <row r="3" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="33">
+      <c r="A3" s="25">
         <v>1</v>
       </c>
-      <c r="B3" s="33" t="s">
+      <c r="B3" s="25" t="s">
+        <v>415</v>
+      </c>
+      <c r="C3" s="25" t="s">
+        <v>154</v>
+      </c>
+      <c r="D3" s="25" t="s">
+        <v>155</v>
+      </c>
+      <c r="E3" s="25">
+        <v>1</v>
+      </c>
+      <c r="F3" s="25" t="s">
+        <v>400</v>
+      </c>
+      <c r="G3" s="25" t="s">
+        <v>411</v>
+      </c>
+      <c r="H3" s="27" t="s">
+        <v>352</v>
+      </c>
+      <c r="I3" s="25"/>
+      <c r="J3" s="25"/>
+      <c r="K3" s="25"/>
+      <c r="L3" s="25">
+        <v>311001023</v>
+      </c>
+      <c r="M3" s="25"/>
+      <c r="N3" s="25"/>
+      <c r="O3" s="25"/>
+      <c r="P3" s="25" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="25">
+        <v>2</v>
+      </c>
+      <c r="B4" s="25" t="s">
         <v>416</v>
       </c>
-      <c r="C3" s="33" t="s">
-        <v>154</v>
-      </c>
-      <c r="D3" s="33" t="s">
+      <c r="C4" s="25" t="s">
+        <v>156</v>
+      </c>
+      <c r="D4" s="25" t="s">
         <v>155</v>
       </c>
-      <c r="E3" s="33">
+      <c r="E4" s="25">
         <v>1</v>
       </c>
-      <c r="F3" s="33" t="s">
+      <c r="F4" s="25" t="s">
         <v>401</v>
       </c>
-      <c r="G3" s="33" t="s">
+      <c r="G4" s="25" t="s">
         <v>412</v>
       </c>
-      <c r="H3" s="35" t="s">
-        <v>353</v>
-      </c>
-      <c r="I3" s="33"/>
-      <c r="J3" s="33"/>
-      <c r="K3" s="33"/>
-      <c r="L3" s="33">
-        <v>311001023</v>
-      </c>
-      <c r="M3" s="33"/>
-      <c r="N3" s="33"/>
-      <c r="O3" s="33"/>
-      <c r="P3" s="33" t="s">
+      <c r="H4" s="27" t="s">
+        <v>359</v>
+      </c>
+      <c r="I4" s="25"/>
+      <c r="J4" s="25"/>
+      <c r="K4" s="25"/>
+      <c r="L4" s="25">
+        <v>311001014</v>
+      </c>
+      <c r="M4" s="25"/>
+      <c r="N4" s="25"/>
+      <c r="O4" s="25"/>
+      <c r="P4" s="25" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="4" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="33">
-        <v>2</v>
-      </c>
-      <c r="B4" s="33" t="s">
+    <row r="5" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="25">
+        <v>3</v>
+      </c>
+      <c r="B5" s="25" t="s">
         <v>417</v>
       </c>
-      <c r="C4" s="33" t="s">
-        <v>156</v>
-      </c>
-      <c r="D4" s="33" t="s">
-        <v>155</v>
-      </c>
-      <c r="E4" s="33">
+      <c r="C5" s="25" t="s">
+        <v>158</v>
+      </c>
+      <c r="D5" s="25" t="s">
+        <v>159</v>
+      </c>
+      <c r="E5" s="25">
         <v>1</v>
       </c>
-      <c r="F4" s="33" t="s">
+      <c r="F5" s="25" t="s">
         <v>402</v>
       </c>
-      <c r="G4" s="33" t="s">
+      <c r="G5" s="25" t="s">
         <v>413</v>
       </c>
-      <c r="H4" s="35" t="s">
-        <v>360</v>
-      </c>
-      <c r="I4" s="33"/>
-      <c r="J4" s="33"/>
-      <c r="K4" s="33"/>
-      <c r="L4" s="33">
-        <v>311001014</v>
-      </c>
-      <c r="M4" s="33"/>
-      <c r="N4" s="33"/>
-      <c r="O4" s="33"/>
-      <c r="P4" s="33" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="5" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="33">
-        <v>3</v>
-      </c>
-      <c r="B5" s="33" t="s">
-        <v>418</v>
-      </c>
-      <c r="C5" s="33" t="s">
-        <v>158</v>
-      </c>
-      <c r="D5" s="33" t="s">
-        <v>159</v>
-      </c>
-      <c r="E5" s="33">
-        <v>1</v>
-      </c>
-      <c r="F5" s="33" t="s">
-        <v>403</v>
-      </c>
-      <c r="G5" s="33" t="s">
-        <v>414</v>
-      </c>
-      <c r="H5" s="35" t="s">
-        <v>366</v>
-      </c>
-      <c r="I5" s="33"/>
-      <c r="J5" s="33"/>
-      <c r="K5" s="33"/>
-      <c r="L5" s="33">
+      <c r="H5" s="27" t="s">
+        <v>365</v>
+      </c>
+      <c r="I5" s="25"/>
+      <c r="J5" s="25"/>
+      <c r="K5" s="25"/>
+      <c r="L5" s="25">
         <v>311001015</v>
       </c>
-      <c r="M5" s="33"/>
-      <c r="N5" s="33"/>
-      <c r="O5" s="33"/>
-      <c r="P5" s="33" t="s">
+      <c r="M5" s="25"/>
+      <c r="N5" s="25"/>
+      <c r="O5" s="25"/>
+      <c r="P5" s="25" t="s">
         <v>157</v>
       </c>
     </row>
@@ -3101,29 +3090,29 @@
         <v>177</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="D2" s="7"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A3" s="34">
+      <c r="A3" s="26">
         <v>1</v>
       </c>
-      <c r="B3" s="34" t="s">
-        <v>201</v>
-      </c>
-      <c r="C3" s="34" t="s">
+      <c r="B3" s="26" t="s">
+        <v>200</v>
+      </c>
+      <c r="C3" s="26" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A4" s="26">
+        <v>2</v>
+      </c>
+      <c r="B4" s="26" t="s">
         <v>419</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A4" s="34">
-        <v>2</v>
-      </c>
-      <c r="B4" s="34" t="s">
-        <v>420</v>
-      </c>
-      <c r="C4" s="34" t="s">
+      <c r="C4" s="26" t="s">
         <v>170</v>
       </c>
     </row>
@@ -3165,13 +3154,13 @@
         <v>164</v>
       </c>
       <c r="E1" s="8" t="s">
+        <v>194</v>
+      </c>
+      <c r="F1" s="8" t="s">
         <v>195</v>
       </c>
-      <c r="F1" s="8" t="s">
+      <c r="G1" s="8" t="s">
         <v>196</v>
-      </c>
-      <c r="G1" s="8" t="s">
-        <v>197</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="58" x14ac:dyDescent="0.35">
@@ -3179,156 +3168,156 @@
         <v>7</v>
       </c>
       <c r="B2" s="7" t="s">
+        <v>197</v>
+      </c>
+      <c r="C2" s="7" t="s">
         <v>198</v>
-      </c>
-      <c r="C2" s="7" t="s">
-        <v>199</v>
       </c>
       <c r="D2" s="7" t="s">
         <v>182</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A3" s="34">
+      <c r="A3" s="26">
         <v>1</v>
       </c>
-      <c r="B3" s="34" t="s">
+      <c r="B3" s="26" t="s">
+        <v>199</v>
+      </c>
+      <c r="C3" s="26" t="s">
+        <v>420</v>
+      </c>
+      <c r="D3" s="15" t="s">
         <v>200</v>
       </c>
-      <c r="C3" s="34" t="s">
+      <c r="E3" s="25">
+        <v>1</v>
+      </c>
+      <c r="F3" s="26">
+        <v>1</v>
+      </c>
+      <c r="G3" s="26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A4" s="26">
+        <v>2</v>
+      </c>
+      <c r="B4" s="26" t="s">
+        <v>201</v>
+      </c>
+      <c r="C4" s="26" t="s">
         <v>421</v>
       </c>
-      <c r="D3" s="15" t="s">
-        <v>201</v>
-      </c>
-      <c r="E3" s="33">
+      <c r="D4" s="15" t="s">
+        <v>200</v>
+      </c>
+      <c r="E4" s="25">
+        <v>0</v>
+      </c>
+      <c r="F4" s="26">
         <v>1</v>
       </c>
-      <c r="F3" s="34">
+      <c r="G4" s="26">
         <v>1</v>
       </c>
-      <c r="G3" s="34">
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A5" s="26">
+        <v>3</v>
+      </c>
+      <c r="B5" s="26" t="s">
+        <v>202</v>
+      </c>
+      <c r="C5" s="26" t="s">
+        <v>422</v>
+      </c>
+      <c r="D5" s="15" t="s">
+        <v>200</v>
+      </c>
+      <c r="E5" s="25">
+        <v>0</v>
+      </c>
+      <c r="F5" s="26">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A4" s="34">
-        <v>2</v>
-      </c>
-      <c r="B4" s="34" t="s">
-        <v>202</v>
-      </c>
-      <c r="C4" s="34" t="s">
-        <v>422</v>
-      </c>
-      <c r="D4" s="15" t="s">
-        <v>201</v>
-      </c>
-      <c r="E4" s="33">
+      <c r="G5" s="26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A6" s="26">
+        <v>4</v>
+      </c>
+      <c r="B6" s="26" t="s">
+        <v>203</v>
+      </c>
+      <c r="C6" s="26" t="s">
+        <v>423</v>
+      </c>
+      <c r="D6" s="15" t="s">
+        <v>200</v>
+      </c>
+      <c r="E6" s="25">
         <v>0</v>
       </c>
-      <c r="F4" s="34">
+      <c r="F6" s="26">
         <v>1</v>
       </c>
-      <c r="G4" s="34">
+      <c r="G6" s="26">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A5" s="34">
-        <v>3</v>
-      </c>
-      <c r="B5" s="34" t="s">
-        <v>203</v>
-      </c>
-      <c r="C5" s="34" t="s">
-        <v>423</v>
-      </c>
-      <c r="D5" s="15" t="s">
-        <v>201</v>
-      </c>
-      <c r="E5" s="33">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A7" s="26">
+        <v>5</v>
+      </c>
+      <c r="B7" s="26" t="s">
+        <v>204</v>
+      </c>
+      <c r="C7" s="26" t="s">
+        <v>424</v>
+      </c>
+      <c r="D7" s="15" t="s">
+        <v>200</v>
+      </c>
+      <c r="E7" s="25">
         <v>0</v>
       </c>
-      <c r="F5" s="34">
+      <c r="F7" s="26">
         <v>1</v>
       </c>
-      <c r="G5" s="34">
+      <c r="G7" s="26">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A6" s="34">
-        <v>4</v>
-      </c>
-      <c r="B6" s="34" t="s">
-        <v>204</v>
-      </c>
-      <c r="C6" s="34" t="s">
-        <v>424</v>
-      </c>
-      <c r="D6" s="15" t="s">
-        <v>201</v>
-      </c>
-      <c r="E6" s="33">
-        <v>0</v>
-      </c>
-      <c r="F6" s="34">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A8" s="26">
+        <v>6</v>
+      </c>
+      <c r="B8" s="26" t="s">
+        <v>425</v>
+      </c>
+      <c r="C8" s="26" t="s">
+        <v>426</v>
+      </c>
+      <c r="D8" s="15" t="s">
+        <v>419</v>
+      </c>
+      <c r="E8" s="32">
         <v>1</v>
       </c>
-      <c r="G6" s="34">
+      <c r="F8" s="26">
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A7" s="34">
-        <v>5</v>
-      </c>
-      <c r="B7" s="34" t="s">
-        <v>205</v>
-      </c>
-      <c r="C7" s="34" t="s">
-        <v>425</v>
-      </c>
-      <c r="D7" s="15" t="s">
-        <v>201</v>
-      </c>
-      <c r="E7" s="33">
-        <v>0</v>
-      </c>
-      <c r="F7" s="34">
-        <v>1</v>
-      </c>
-      <c r="G7" s="34">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A8" s="34">
-        <v>6</v>
-      </c>
-      <c r="B8" s="34" t="s">
-        <v>426</v>
-      </c>
-      <c r="C8" s="34" t="s">
-        <v>427</v>
-      </c>
-      <c r="D8" s="15" t="s">
-        <v>420</v>
-      </c>
-      <c r="E8" s="44">
-        <v>1</v>
-      </c>
-      <c r="F8" s="34">
-        <v>1</v>
-      </c>
-      <c r="G8" s="34"/>
+      <c r="G8" s="26"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="E9" s="43"/>
+      <c r="E9" s="31"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3372,7 +3361,7 @@
         <v>177</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D2" s="7"/>
     </row>
@@ -3418,50 +3407,50 @@
         <v>177</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D2" s="7"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A3" s="34">
+      <c r="A3" s="26">
         <v>1</v>
       </c>
-      <c r="B3" s="34" t="s">
+      <c r="B3" s="26" t="s">
+        <v>428</v>
+      </c>
+      <c r="C3" s="26" t="s">
         <v>429</v>
       </c>
-      <c r="C3" s="34" t="s">
+      <c r="D3" s="26" t="s">
         <v>430</v>
       </c>
-      <c r="D3" s="34" t="s">
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A4" s="26">
+        <v>2</v>
+      </c>
+      <c r="B4" s="26" t="s">
         <v>431</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A4" s="34">
-        <v>2</v>
-      </c>
-      <c r="B4" s="34" t="s">
+      <c r="C4" s="26" t="s">
         <v>432</v>
       </c>
-      <c r="C4" s="34" t="s">
+      <c r="D4" s="26" t="s">
         <v>433</v>
       </c>
-      <c r="D4" s="34" t="s">
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A5" s="26">
+        <v>3</v>
+      </c>
+      <c r="B5" s="26" t="s">
         <v>434</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A5" s="34">
-        <v>3</v>
-      </c>
-      <c r="B5" s="34" t="s">
+      <c r="C5" s="26" t="s">
         <v>435</v>
       </c>
-      <c r="C5" s="34" t="s">
+      <c r="D5" s="26" t="s">
         <v>436</v>
-      </c>
-      <c r="D5" s="34" t="s">
-        <v>437</v>
       </c>
     </row>
   </sheetData>
@@ -3474,7 +3463,7 @@
   <dimension ref="A1:U5"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="L2" sqref="L2"/>
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3588,7 +3577,7 @@
         <v>182</v>
       </c>
       <c r="J2" s="16" t="s">
-        <v>183</v>
+        <v>449</v>
       </c>
       <c r="K2" s="16"/>
       <c r="L2" s="16"/>
@@ -3596,182 +3585,182 @@
       <c r="N2" s="16"/>
       <c r="O2" s="16"/>
       <c r="P2" s="16" t="s">
+        <v>183</v>
+      </c>
+      <c r="Q2" s="16" t="s">
         <v>184</v>
       </c>
-      <c r="Q2" s="16" t="s">
+      <c r="R2" s="16" t="s">
         <v>185</v>
       </c>
-      <c r="R2" s="16" t="s">
+      <c r="S2" s="16" t="s">
         <v>186</v>
       </c>
-      <c r="S2" s="16" t="s">
+      <c r="T2" s="16" t="s">
         <v>187</v>
       </c>
-      <c r="T2" s="16" t="s">
+      <c r="U2" s="16" t="s">
         <v>188</v>
       </c>
-      <c r="U2" s="16" t="s">
+    </row>
+    <row r="3" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A3" s="33">
+        <v>1</v>
+      </c>
+      <c r="B3" s="33" t="s">
+        <v>437</v>
+      </c>
+      <c r="C3" s="33" t="s">
+        <v>438</v>
+      </c>
+      <c r="D3" s="33">
+        <v>123</v>
+      </c>
+      <c r="E3" s="33" t="s">
+        <v>430</v>
+      </c>
+      <c r="F3" s="33" t="s">
         <v>189</v>
       </c>
-    </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.35">
-      <c r="A3" s="45">
+      <c r="G3" s="33" t="s">
+        <v>439</v>
+      </c>
+      <c r="H3" s="33" t="s">
+        <v>428</v>
+      </c>
+      <c r="I3" s="26" t="s">
+        <v>200</v>
+      </c>
+      <c r="J3" s="33">
         <v>1</v>
       </c>
-      <c r="B3" s="45" t="s">
-        <v>438</v>
-      </c>
-      <c r="C3" s="45" t="s">
+      <c r="K3" s="33"/>
+      <c r="L3" s="33"/>
+      <c r="M3" s="33"/>
+      <c r="N3" s="33"/>
+      <c r="O3" s="33"/>
+      <c r="P3" s="26" t="s">
+        <v>199</v>
+      </c>
+      <c r="Q3" s="33" t="s">
+        <v>398</v>
+      </c>
+      <c r="R3" s="26" t="s">
+        <v>199</v>
+      </c>
+      <c r="S3" s="26" t="s">
+        <v>199</v>
+      </c>
+      <c r="T3" s="33" t="s">
+        <v>398</v>
+      </c>
+      <c r="U3" s="33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A4" s="33">
+        <v>2</v>
+      </c>
+      <c r="B4" s="33" t="s">
+        <v>440</v>
+      </c>
+      <c r="C4" s="33" t="s">
+        <v>441</v>
+      </c>
+      <c r="D4" s="33"/>
+      <c r="E4" s="33" t="s">
+        <v>433</v>
+      </c>
+      <c r="F4" s="33" t="s">
+        <v>442</v>
+      </c>
+      <c r="G4" s="33" t="s">
         <v>439</v>
       </c>
-      <c r="D3" s="45">
-        <v>123</v>
-      </c>
-      <c r="E3" s="45" t="s">
+      <c r="H4" s="33" t="s">
         <v>431</v>
       </c>
-      <c r="F3" s="45" t="s">
-        <v>190</v>
-      </c>
-      <c r="G3" s="45" t="s">
-        <v>440</v>
-      </c>
-      <c r="H3" s="45" t="s">
-        <v>429</v>
-      </c>
-      <c r="I3" s="34" t="s">
-        <v>201</v>
-      </c>
-      <c r="J3" s="45">
-        <v>1</v>
-      </c>
-      <c r="K3" s="45"/>
-      <c r="L3" s="45"/>
-      <c r="M3" s="45"/>
-      <c r="N3" s="45"/>
-      <c r="O3" s="45"/>
-      <c r="P3" s="34" t="s">
+      <c r="I4" s="26" t="s">
         <v>200</v>
       </c>
-      <c r="Q3" s="45" t="s">
-        <v>399</v>
-      </c>
-      <c r="R3" s="34" t="s">
+      <c r="J4" s="33">
+        <v>0</v>
+      </c>
+      <c r="K4" s="33"/>
+      <c r="L4" s="33"/>
+      <c r="M4" s="33"/>
+      <c r="N4" s="33"/>
+      <c r="O4" s="33"/>
+      <c r="P4" s="26" t="s">
+        <v>199</v>
+      </c>
+      <c r="Q4" s="33" t="s">
+        <v>398</v>
+      </c>
+      <c r="R4" s="26" t="s">
+        <v>199</v>
+      </c>
+      <c r="S4" s="26" t="s">
+        <v>199</v>
+      </c>
+      <c r="T4" s="33" t="s">
+        <v>398</v>
+      </c>
+      <c r="U4" s="33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A5" s="33">
+        <v>3</v>
+      </c>
+      <c r="B5" s="33" t="s">
+        <v>443</v>
+      </c>
+      <c r="C5" s="33" t="s">
+        <v>444</v>
+      </c>
+      <c r="D5" s="33"/>
+      <c r="E5" s="33" t="s">
+        <v>436</v>
+      </c>
+      <c r="F5" s="33" t="s">
+        <v>442</v>
+      </c>
+      <c r="G5" s="33" t="s">
+        <v>445</v>
+      </c>
+      <c r="H5" s="33" t="s">
+        <v>434</v>
+      </c>
+      <c r="I5" s="26" t="s">
         <v>200</v>
       </c>
-      <c r="S3" s="34" t="s">
-        <v>200</v>
-      </c>
-      <c r="T3" s="45" t="s">
-        <v>399</v>
-      </c>
-      <c r="U3" s="45">
+      <c r="J5" s="33">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.35">
-      <c r="A4" s="45">
-        <v>2</v>
-      </c>
-      <c r="B4" s="45" t="s">
-        <v>441</v>
-      </c>
-      <c r="C4" s="45" t="s">
-        <v>442</v>
-      </c>
-      <c r="D4" s="45"/>
-      <c r="E4" s="45" t="s">
-        <v>434</v>
-      </c>
-      <c r="F4" s="45" t="s">
-        <v>443</v>
-      </c>
-      <c r="G4" s="45" t="s">
-        <v>440</v>
-      </c>
-      <c r="H4" s="45" t="s">
-        <v>432</v>
-      </c>
-      <c r="I4" s="34" t="s">
-        <v>201</v>
-      </c>
-      <c r="J4" s="45">
-        <v>0</v>
-      </c>
-      <c r="K4" s="45"/>
-      <c r="L4" s="45"/>
-      <c r="M4" s="45"/>
-      <c r="N4" s="45"/>
-      <c r="O4" s="45"/>
-      <c r="P4" s="34" t="s">
-        <v>200</v>
-      </c>
-      <c r="Q4" s="45" t="s">
-        <v>399</v>
-      </c>
-      <c r="R4" s="34" t="s">
-        <v>200</v>
-      </c>
-      <c r="S4" s="34" t="s">
-        <v>200</v>
-      </c>
-      <c r="T4" s="45" t="s">
-        <v>399</v>
-      </c>
-      <c r="U4" s="45">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.35">
-      <c r="A5" s="45">
-        <v>3</v>
-      </c>
-      <c r="B5" s="45" t="s">
-        <v>444</v>
-      </c>
-      <c r="C5" s="45" t="s">
-        <v>445</v>
-      </c>
-      <c r="D5" s="45"/>
-      <c r="E5" s="45" t="s">
-        <v>437</v>
-      </c>
-      <c r="F5" s="45" t="s">
-        <v>443</v>
-      </c>
-      <c r="G5" s="45" t="s">
-        <v>446</v>
-      </c>
-      <c r="H5" s="45" t="s">
-        <v>435</v>
-      </c>
-      <c r="I5" s="34" t="s">
-        <v>201</v>
-      </c>
-      <c r="J5" s="45">
-        <v>0</v>
-      </c>
-      <c r="K5" s="45"/>
-      <c r="L5" s="45"/>
-      <c r="M5" s="45"/>
-      <c r="N5" s="45"/>
-      <c r="O5" s="45"/>
-      <c r="P5" s="34" t="s">
-        <v>200</v>
-      </c>
-      <c r="Q5" s="45" t="s">
-        <v>399</v>
-      </c>
-      <c r="R5" s="34" t="s">
-        <v>200</v>
-      </c>
-      <c r="S5" s="34" t="s">
-        <v>200</v>
-      </c>
-      <c r="T5" s="45" t="s">
-        <v>399</v>
-      </c>
-      <c r="U5" s="45">
+      <c r="K5" s="33"/>
+      <c r="L5" s="33"/>
+      <c r="M5" s="33"/>
+      <c r="N5" s="33"/>
+      <c r="O5" s="33"/>
+      <c r="P5" s="26" t="s">
+        <v>199</v>
+      </c>
+      <c r="Q5" s="33" t="s">
+        <v>398</v>
+      </c>
+      <c r="R5" s="26" t="s">
+        <v>199</v>
+      </c>
+      <c r="S5" s="26" t="s">
+        <v>199</v>
+      </c>
+      <c r="T5" s="33" t="s">
+        <v>398</v>
+      </c>
+      <c r="U5" s="33">
         <v>0</v>
       </c>
     </row>
@@ -3816,13 +3805,13 @@
         <v>7</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C2" s="7" t="s">
+        <v>229</v>
+      </c>
+      <c r="D2" s="7" t="s">
         <v>230</v>
-      </c>
-      <c r="D2" s="7" t="s">
-        <v>231</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
@@ -3833,7 +3822,7 @@
         <v>110</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
@@ -3844,7 +3833,7 @@
         <v>112</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
   </sheetData>
@@ -3882,31 +3871,31 @@
         <v>55</v>
       </c>
       <c r="C1" s="8" t="s">
+        <v>210</v>
+      </c>
+      <c r="D1" s="8" t="s">
         <v>211</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="E1" s="8" t="s">
         <v>212</v>
       </c>
-      <c r="E1" s="8" t="s">
+      <c r="F1" s="8" t="s">
         <v>213</v>
       </c>
-      <c r="F1" s="8" t="s">
+      <c r="G1" s="8" t="s">
         <v>214</v>
       </c>
-      <c r="G1" s="8" t="s">
+      <c r="H1" s="8" t="s">
         <v>215</v>
       </c>
-      <c r="H1" s="8" t="s">
+      <c r="I1" s="8" t="s">
         <v>216</v>
       </c>
-      <c r="I1" s="8" t="s">
+      <c r="J1" s="8" t="s">
         <v>217</v>
       </c>
-      <c r="J1" s="8" t="s">
+      <c r="K1" s="8" t="s">
         <v>218</v>
-      </c>
-      <c r="K1" s="8" t="s">
-        <v>219</v>
       </c>
     </row>
     <row r="2" spans="1:11" ht="85.9" customHeight="1" x14ac:dyDescent="0.35">
@@ -3914,61 +3903,61 @@
         <v>7</v>
       </c>
       <c r="B2" s="10" t="s">
+        <v>219</v>
+      </c>
+      <c r="C2" s="7" t="s">
         <v>220</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="D2" s="7" t="s">
         <v>221</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="E2" s="7" t="s">
         <v>222</v>
       </c>
-      <c r="E2" s="7" t="s">
+      <c r="F2" s="7" t="s">
         <v>223</v>
       </c>
-      <c r="F2" s="7" t="s">
+      <c r="G2" s="7" t="s">
         <v>224</v>
       </c>
-      <c r="G2" s="7" t="s">
+      <c r="H2" s="7" t="s">
         <v>225</v>
       </c>
-      <c r="H2" s="7" t="s">
+      <c r="I2" s="7" t="s">
         <v>226</v>
       </c>
-      <c r="I2" s="7" t="s">
+      <c r="J2" s="7" t="s">
         <v>227</v>
       </c>
-      <c r="J2" s="7" t="s">
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A3" s="25">
+        <v>1</v>
+      </c>
+      <c r="B3" s="25" t="s">
+        <v>446</v>
+      </c>
+      <c r="C3" s="27" t="s">
+        <v>377</v>
+      </c>
+      <c r="D3" s="25">
+        <v>1</v>
+      </c>
+      <c r="E3" s="25" t="s">
+        <v>447</v>
+      </c>
+      <c r="F3" s="25" t="s">
         <v>228</v>
       </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A3" s="33">
-        <v>1</v>
-      </c>
-      <c r="B3" s="33" t="s">
-        <v>447</v>
-      </c>
-      <c r="C3" s="35" t="s">
-        <v>378</v>
-      </c>
-      <c r="D3" s="33">
-        <v>1</v>
-      </c>
-      <c r="E3" s="33" t="s">
+      <c r="G3" s="25"/>
+      <c r="H3" s="25">
+        <v>903331332</v>
+      </c>
+      <c r="I3" s="34" t="s">
         <v>448</v>
       </c>
-      <c r="F3" s="33" t="s">
-        <v>229</v>
-      </c>
-      <c r="G3" s="33"/>
-      <c r="H3" s="33">
-        <v>903331332</v>
-      </c>
-      <c r="I3" s="46" t="s">
-        <v>449</v>
-      </c>
-      <c r="J3" s="33"/>
-      <c r="K3" s="33"/>
+      <c r="J3" s="25"/>
+      <c r="K3" s="25"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.35">
       <c r="I4" s="12"/>
@@ -4021,140 +4010,140 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A1" s="32" t="s">
+      <c r="A1" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="32" t="s">
+      <c r="B1" s="24" t="s">
         <v>45</v>
       </c>
-      <c r="C1" s="32" t="s">
+      <c r="C1" s="24" t="s">
         <v>46</v>
       </c>
-      <c r="D1" s="32" t="s">
+      <c r="D1" s="24" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="75.650000000000006" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="37" t="s">
+      <c r="A2" s="38" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="33" t="s">
+      <c r="B2" s="25" t="s">
+        <v>309</v>
+      </c>
+      <c r="C2" s="25" t="s">
+        <v>312</v>
+      </c>
+      <c r="D2" s="25" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+      <c r="A3" s="39"/>
+      <c r="B3" s="25" t="s">
         <v>310</v>
       </c>
-      <c r="C2" s="33" t="s">
+      <c r="C3" s="25" t="s">
         <v>313</v>
       </c>
-      <c r="D2" s="33" t="s">
+      <c r="D3" s="25" t="s">
         <v>316</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="29" x14ac:dyDescent="0.35">
-      <c r="A3" s="36"/>
-      <c r="B3" s="33" t="s">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A4" s="39"/>
+      <c r="B4" s="25" t="s">
         <v>311</v>
       </c>
-      <c r="C3" s="33" t="s">
+      <c r="C4" s="25" t="s">
         <v>314</v>
       </c>
-      <c r="D3" s="33" t="s">
+      <c r="D4" s="25" t="s">
         <v>317</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A4" s="36"/>
-      <c r="B4" s="33" t="s">
-        <v>312</v>
-      </c>
-      <c r="C4" s="33" t="s">
-        <v>315</v>
-      </c>
-      <c r="D4" s="33" t="s">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A5" s="25">
+        <v>1</v>
+      </c>
+      <c r="B5" s="25" t="s">
         <v>318</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A5" s="33">
-        <v>1</v>
-      </c>
-      <c r="B5" s="33" t="s">
+      <c r="C5" s="25" t="s">
+        <v>48</v>
+      </c>
+      <c r="D5" s="25"/>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A6" s="25">
+        <v>2</v>
+      </c>
+      <c r="B6" s="25" t="s">
         <v>319</v>
       </c>
-      <c r="C5" s="33" t="s">
-        <v>48</v>
-      </c>
-      <c r="D5" s="33"/>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A6" s="33">
-        <v>2</v>
-      </c>
-      <c r="B6" s="33" t="s">
+      <c r="C6" s="25" t="s">
+        <v>49</v>
+      </c>
+      <c r="D6" s="25"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A7" s="25">
+        <v>3</v>
+      </c>
+      <c r="B7" s="25" t="s">
+        <v>50</v>
+      </c>
+      <c r="C7" s="25" t="s">
+        <v>51</v>
+      </c>
+      <c r="D7" s="27"/>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A8" s="25">
+        <v>4</v>
+      </c>
+      <c r="B8" s="25" t="s">
         <v>320</v>
       </c>
-      <c r="C6" s="33" t="s">
-        <v>49</v>
-      </c>
-      <c r="D6" s="33"/>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A7" s="33">
-        <v>3</v>
-      </c>
-      <c r="B7" s="33" t="s">
-        <v>50</v>
-      </c>
-      <c r="C7" s="33" t="s">
-        <v>51</v>
-      </c>
-      <c r="D7" s="35"/>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A8" s="33">
-        <v>4</v>
-      </c>
-      <c r="B8" s="33" t="s">
+      <c r="C8" s="25" t="s">
         <v>321</v>
       </c>
-      <c r="C8" s="33" t="s">
+      <c r="D8" s="25"/>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A9" s="25">
+        <v>5</v>
+      </c>
+      <c r="B9" s="25" t="s">
         <v>322</v>
       </c>
-      <c r="D8" s="33"/>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A9" s="33">
-        <v>5</v>
-      </c>
-      <c r="B9" s="33" t="s">
+      <c r="C9" s="25" t="s">
+        <v>52</v>
+      </c>
+      <c r="D9" s="25"/>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A10" s="25">
+        <v>6</v>
+      </c>
+      <c r="B10" s="25" t="s">
+        <v>53</v>
+      </c>
+      <c r="C10" s="25" t="s">
+        <v>54</v>
+      </c>
+      <c r="D10" s="25"/>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A11" s="25">
+        <v>7</v>
+      </c>
+      <c r="B11" s="25" t="s">
         <v>323</v>
       </c>
-      <c r="C9" s="33" t="s">
-        <v>52</v>
-      </c>
-      <c r="D9" s="33"/>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A10" s="33">
-        <v>6</v>
-      </c>
-      <c r="B10" s="33" t="s">
-        <v>53</v>
-      </c>
-      <c r="C10" s="33" t="s">
-        <v>54</v>
-      </c>
-      <c r="D10" s="33"/>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A11" s="33">
-        <v>7</v>
-      </c>
-      <c r="B11" s="33" t="s">
+      <c r="C11" s="25" t="s">
         <v>324</v>
       </c>
-      <c r="C11" s="33" t="s">
-        <v>325</v>
-      </c>
-      <c r="D11" s="33"/>
+      <c r="D11" s="25"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -4194,10 +4183,10 @@
         <v>3</v>
       </c>
       <c r="D1" s="8" t="s">
+        <v>205</v>
+      </c>
+      <c r="E1" s="8" t="s">
         <v>206</v>
-      </c>
-      <c r="E1" s="8" t="s">
-        <v>207</v>
       </c>
       <c r="F1" s="8" t="s">
         <v>80</v>
@@ -4211,13 +4200,13 @@
         <v>119</v>
       </c>
       <c r="C2" s="7" t="s">
+        <v>207</v>
+      </c>
+      <c r="D2" s="7" t="s">
         <v>208</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="E2" s="7" t="s">
         <v>209</v>
-      </c>
-      <c r="E2" s="7" t="s">
-        <v>210</v>
       </c>
     </row>
   </sheetData>
@@ -4250,17 +4239,17 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="4" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="6" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="6" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
@@ -4285,13 +4274,13 @@
       <c r="A10" s="6"/>
     </row>
     <row r="11" spans="1:5" ht="34.9" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="24" t="s">
-        <v>237</v>
-      </c>
-      <c r="B11" s="25"/>
-      <c r="C11" s="25"/>
-      <c r="D11" s="25"/>
-      <c r="E11" s="25"/>
+      <c r="A11" s="40" t="s">
+        <v>236</v>
+      </c>
+      <c r="B11" s="41"/>
+      <c r="C11" s="41"/>
+      <c r="D11" s="41"/>
+      <c r="E11" s="41"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" s="6"/>
@@ -4306,65 +4295,65 @@
       <c r="A15" s="6"/>
     </row>
     <row r="16" spans="1:5" ht="28.9" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="26" t="s">
-        <v>238</v>
-      </c>
-      <c r="B16" s="27"/>
-      <c r="C16" s="27"/>
-      <c r="D16" s="27"/>
-      <c r="E16" s="27"/>
+      <c r="A16" s="42" t="s">
+        <v>237</v>
+      </c>
+      <c r="B16" s="43"/>
+      <c r="C16" s="43"/>
+      <c r="D16" s="43"/>
+      <c r="E16" s="43"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17" s="3" t="s">
+        <v>238</v>
+      </c>
+      <c r="B17" s="45" t="s">
+        <v>80</v>
+      </c>
+      <c r="C17" s="45"/>
+      <c r="D17" s="45"/>
+      <c r="E17" s="3" t="s">
         <v>239</v>
-      </c>
-      <c r="B17" s="29" t="s">
-        <v>80</v>
-      </c>
-      <c r="C17" s="29"/>
-      <c r="D17" s="29"/>
-      <c r="E17" s="3" t="s">
-        <v>240</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="B18" s="46" t="s">
         <v>241</v>
       </c>
-      <c r="B18" s="30" t="s">
-        <v>242</v>
-      </c>
-      <c r="C18" s="30"/>
-      <c r="D18" s="30"/>
+      <c r="C18" s="46"/>
+      <c r="D18" s="46"/>
       <c r="E18" s="1"/>
     </row>
     <row r="19" spans="1:5" ht="29.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="B19" s="47" t="s">
         <v>243</v>
       </c>
-      <c r="B19" s="31" t="s">
-        <v>244</v>
-      </c>
-      <c r="C19" s="31"/>
-      <c r="D19" s="31"/>
+      <c r="C19" s="47"/>
+      <c r="D19" s="47"/>
       <c r="E19" s="1"/>
     </row>
     <row r="20" spans="1:5" ht="34.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B20" s="31" t="s">
-        <v>245</v>
-      </c>
-      <c r="C20" s="31"/>
-      <c r="D20" s="31"/>
+      <c r="B20" s="47" t="s">
+        <v>244</v>
+      </c>
+      <c r="C20" s="47"/>
+      <c r="D20" s="47"/>
       <c r="E20" s="1"/>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A21" s="1"/>
-      <c r="B21" s="30"/>
-      <c r="C21" s="30"/>
-      <c r="D21" s="30"/>
+      <c r="B21" s="46"/>
+      <c r="C21" s="46"/>
+      <c r="D21" s="46"/>
       <c r="E21" s="1"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.35">
@@ -4380,283 +4369,283 @@
       <c r="A25"/>
     </row>
     <row r="26" spans="1:5" ht="28.9" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="28" t="s">
-        <v>246</v>
-      </c>
-      <c r="B26" s="28"/>
-      <c r="C26" s="28"/>
-      <c r="D26" s="28"/>
-      <c r="E26" s="28"/>
+      <c r="A26" s="44" t="s">
+        <v>245</v>
+      </c>
+      <c r="B26" s="44"/>
+      <c r="C26" s="44"/>
+      <c r="D26" s="44"/>
+      <c r="E26" s="44"/>
     </row>
     <row r="27" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A27" s="20" t="s">
+        <v>246</v>
+      </c>
+      <c r="B27" s="20" t="s">
         <v>247</v>
       </c>
-      <c r="B27" s="20" t="s">
+      <c r="C27" s="20" t="s">
         <v>248</v>
       </c>
-      <c r="C27" s="20" t="s">
+      <c r="D27" s="21" t="s">
         <v>249</v>
       </c>
-      <c r="D27" s="21" t="s">
-        <v>250</v>
-      </c>
       <c r="E27" s="21" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="28" spans="1:5" ht="87" x14ac:dyDescent="0.35">
       <c r="A28" s="22" t="s">
+        <v>250</v>
+      </c>
+      <c r="B28" s="22" t="s">
         <v>251</v>
-      </c>
-      <c r="B28" s="22" t="s">
-        <v>252</v>
       </c>
       <c r="C28" s="17" t="s">
         <v>58</v>
       </c>
       <c r="D28" s="19" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="E28" s="18" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="29" spans="1:5" ht="55.9" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A29" s="22" t="s">
+        <v>257</v>
+      </c>
+      <c r="B29" s="22" t="s">
         <v>258</v>
-      </c>
-      <c r="B29" s="22" t="s">
-        <v>259</v>
       </c>
       <c r="C29" s="17" t="s">
         <v>62</v>
       </c>
       <c r="D29" s="19" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="E29" s="18"/>
     </row>
     <row r="30" spans="1:5" ht="62.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A30" s="22" t="s">
+        <v>253</v>
+      </c>
+      <c r="B30" s="22" t="s">
         <v>254</v>
-      </c>
-      <c r="B30" s="22" t="s">
-        <v>255</v>
       </c>
       <c r="C30" s="17" t="s">
         <v>54</v>
       </c>
       <c r="D30" s="18" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E30" s="18"/>
     </row>
     <row r="31" spans="1:5" ht="42.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A31" s="22" t="s">
+        <v>260</v>
+      </c>
+      <c r="B31" s="22" t="s">
         <v>261</v>
       </c>
-      <c r="B31" s="22" t="s">
+      <c r="C31" s="17" t="s">
         <v>262</v>
       </c>
-      <c r="C31" s="17" t="s">
+      <c r="D31" s="19" t="s">
         <v>263</v>
-      </c>
-      <c r="D31" s="19" t="s">
-        <v>264</v>
       </c>
       <c r="E31" s="18"/>
     </row>
     <row r="32" spans="1:5" ht="36" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A32" s="22" t="s">
+        <v>264</v>
+      </c>
+      <c r="B32" s="22" t="s">
         <v>265</v>
-      </c>
-      <c r="B32" s="22" t="s">
-        <v>266</v>
       </c>
       <c r="C32" s="17" t="s">
         <v>76</v>
       </c>
       <c r="D32" s="19" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="E32" s="18"/>
     </row>
     <row r="33" spans="1:5" ht="36.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A33" s="23" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="B33" s="23" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="C33" s="17" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="D33" s="18"/>
       <c r="E33" s="18"/>
     </row>
     <row r="34" spans="1:5" ht="38.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A34" s="23" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="B34" s="23" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="C34" s="17" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="D34" s="18"/>
       <c r="E34" s="18"/>
     </row>
     <row r="35" spans="1:5" ht="39.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A35" s="22" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B35" s="22" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="C35" s="17" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="D35" s="18"/>
       <c r="E35" s="18"/>
     </row>
     <row r="36" spans="1:5" ht="32.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A36" s="22" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="B36" s="22" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C36" s="17" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="D36" s="18"/>
       <c r="E36" s="18"/>
     </row>
     <row r="37" spans="1:5" ht="42.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A37" s="22" t="s">
+        <v>269</v>
+      </c>
+      <c r="B37" s="22" t="s">
+        <v>299</v>
+      </c>
+      <c r="C37" s="17" t="s">
         <v>270</v>
-      </c>
-      <c r="B37" s="22" t="s">
-        <v>300</v>
-      </c>
-      <c r="C37" s="17" t="s">
-        <v>271</v>
       </c>
       <c r="D37" s="18"/>
       <c r="E37" s="18"/>
     </row>
     <row r="38" spans="1:5" ht="42.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A38" s="22" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="B38" s="22" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="C38" s="17" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="D38" s="18"/>
       <c r="E38" s="18"/>
     </row>
     <row r="39" spans="1:5" ht="42.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A39" s="22" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="B39" s="22" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="C39" s="17" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D39" s="18"/>
       <c r="E39" s="18"/>
     </row>
     <row r="40" spans="1:5" ht="42.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A40" s="22" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="B40" s="22" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="C40" s="17" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="D40" s="18"/>
       <c r="E40" s="18"/>
     </row>
     <row r="41" spans="1:5" ht="42.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A41" s="22" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="B41" s="22" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="C41" s="17" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="D41" s="18"/>
       <c r="E41" s="18"/>
     </row>
     <row r="42" spans="1:5" ht="42.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A42" s="23" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="B42" s="23" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C42" s="17" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="D42" s="18"/>
       <c r="E42" s="18"/>
     </row>
     <row r="43" spans="1:5" ht="42.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A43" s="22" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="B43" s="22" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="C43" s="17" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="D43" s="18"/>
       <c r="E43" s="18"/>
     </row>
     <row r="44" spans="1:5" ht="42.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A44" s="23" t="s">
+        <v>284</v>
+      </c>
+      <c r="B44" s="23" t="s">
         <v>285</v>
       </c>
-      <c r="B44" s="23" t="s">
+      <c r="C44" s="17" t="s">
         <v>286</v>
-      </c>
-      <c r="C44" s="17" t="s">
-        <v>287</v>
       </c>
       <c r="D44" s="18"/>
       <c r="E44" s="18"/>
     </row>
     <row r="45" spans="1:5" ht="42.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A45" s="22" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="B45" s="22" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="C45" s="17" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="D45" s="18"/>
       <c r="E45" s="18"/>
     </row>
     <row r="46" spans="1:5" ht="42.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A46" s="22" t="s">
+        <v>274</v>
+      </c>
+      <c r="B46" s="22" t="s">
         <v>275</v>
-      </c>
-      <c r="B46" s="22" t="s">
-        <v>276</v>
       </c>
       <c r="C46" s="17" t="s">
         <v>138</v>
@@ -4666,10 +4655,10 @@
     </row>
     <row r="47" spans="1:5" ht="42.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A47" s="1" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="C47" s="1"/>
       <c r="D47" s="2"/>
@@ -4697,7 +4686,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{18F2B7B4-0119-40B2-9AE3-A031B16A0EEC}">
-  <dimension ref="A1:K21"/>
+  <dimension ref="A1:K20"/>
   <sheetViews>
     <sheetView topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="F4" sqref="F4"/>
@@ -4719,37 +4708,37 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A1" s="50" t="s">
+      <c r="A1" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="50" t="s">
+      <c r="B1" s="37" t="s">
         <v>55</v>
       </c>
-      <c r="C1" s="50" t="s">
+      <c r="C1" s="37" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="50" t="s">
+      <c r="D1" s="37" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="50" t="s">
+      <c r="E1" s="37" t="s">
         <v>56</v>
       </c>
-      <c r="F1" s="50" t="s">
+      <c r="F1" s="37" t="s">
         <v>57</v>
       </c>
-      <c r="G1" s="50" t="s">
+      <c r="G1" s="37" t="s">
         <v>58</v>
       </c>
-      <c r="H1" s="50" t="s">
+      <c r="H1" s="37" t="s">
         <v>59</v>
       </c>
-      <c r="I1" s="50" t="s">
+      <c r="I1" s="37" t="s">
         <v>60</v>
       </c>
-      <c r="J1" s="50" t="s">
+      <c r="J1" s="37" t="s">
         <v>61</v>
       </c>
-      <c r="K1" s="50" t="s">
+      <c r="K1" s="37" t="s">
         <v>62</v>
       </c>
     </row>
@@ -4757,395 +4746,392 @@
       <c r="A2" s="39" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="40" t="s">
-        <v>310</v>
-      </c>
-      <c r="C2" s="40" t="s">
-        <v>313</v>
-      </c>
-      <c r="D2" s="40" t="s">
-        <v>313</v>
-      </c>
-      <c r="E2" s="40" t="s">
-        <v>313</v>
-      </c>
-      <c r="F2" s="40" t="s">
-        <v>313</v>
-      </c>
-      <c r="G2" s="40" t="s">
-        <v>342</v>
-      </c>
-      <c r="H2" s="40" t="s">
-        <v>345</v>
-      </c>
-      <c r="I2" s="40" t="s">
-        <v>345</v>
-      </c>
-      <c r="J2" s="40" t="s">
-        <v>347</v>
-      </c>
-      <c r="K2" s="40" t="s">
-        <v>350</v>
+      <c r="B2" s="25" t="s">
+        <v>309</v>
+      </c>
+      <c r="C2" s="25" t="s">
+        <v>312</v>
+      </c>
+      <c r="D2" s="25" t="s">
+        <v>312</v>
+      </c>
+      <c r="E2" s="25" t="s">
+        <v>312</v>
+      </c>
+      <c r="F2" s="25" t="s">
+        <v>312</v>
+      </c>
+      <c r="G2" s="25" t="s">
+        <v>341</v>
+      </c>
+      <c r="H2" s="25" t="s">
+        <v>344</v>
+      </c>
+      <c r="I2" s="25" t="s">
+        <v>344</v>
+      </c>
+      <c r="J2" s="25" t="s">
+        <v>346</v>
+      </c>
+      <c r="K2" s="25" t="s">
+        <v>349</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A3" s="39"/>
-      <c r="B3" s="40" t="s">
-        <v>326</v>
-      </c>
-      <c r="C3" s="40" t="s">
-        <v>330</v>
-      </c>
-      <c r="D3" s="40" t="s">
-        <v>330</v>
-      </c>
-      <c r="E3" s="40" t="s">
-        <v>335</v>
-      </c>
-      <c r="F3" s="40" t="s">
-        <v>338</v>
-      </c>
-      <c r="G3" s="40" t="s">
-        <v>343</v>
-      </c>
-      <c r="H3" s="40" t="s">
-        <v>346</v>
-      </c>
-      <c r="I3" s="40" t="s">
-        <v>346</v>
-      </c>
-      <c r="J3" s="40" t="s">
-        <v>348</v>
-      </c>
-      <c r="K3" s="40" t="s">
-        <v>351</v>
+      <c r="B3" s="25" t="s">
+        <v>325</v>
+      </c>
+      <c r="C3" s="25" t="s">
+        <v>329</v>
+      </c>
+      <c r="D3" s="25" t="s">
+        <v>329</v>
+      </c>
+      <c r="E3" s="25" t="s">
+        <v>334</v>
+      </c>
+      <c r="F3" s="25" t="s">
+        <v>337</v>
+      </c>
+      <c r="G3" s="25" t="s">
+        <v>342</v>
+      </c>
+      <c r="H3" s="25" t="s">
+        <v>345</v>
+      </c>
+      <c r="I3" s="25" t="s">
+        <v>345</v>
+      </c>
+      <c r="J3" s="25" t="s">
+        <v>347</v>
+      </c>
+      <c r="K3" s="25" t="s">
+        <v>350</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A4" s="39"/>
-      <c r="B4" s="40" t="s">
-        <v>327</v>
-      </c>
-      <c r="C4" s="40" t="s">
-        <v>331</v>
-      </c>
-      <c r="D4" s="40" t="s">
-        <v>333</v>
-      </c>
-      <c r="E4" s="40" t="s">
-        <v>336</v>
-      </c>
-      <c r="F4" s="40" t="s">
-        <v>339</v>
-      </c>
-      <c r="G4" s="40" t="s">
-        <v>344</v>
-      </c>
-      <c r="H4" s="40"/>
-      <c r="I4" s="40"/>
-      <c r="J4" s="40" t="s">
-        <v>349</v>
-      </c>
-      <c r="K4" s="40" t="s">
-        <v>352</v>
+      <c r="B4" s="25" t="s">
+        <v>326</v>
+      </c>
+      <c r="C4" s="25" t="s">
+        <v>330</v>
+      </c>
+      <c r="D4" s="25" t="s">
+        <v>332</v>
+      </c>
+      <c r="E4" s="25" t="s">
+        <v>335</v>
+      </c>
+      <c r="F4" s="25" t="s">
+        <v>338</v>
+      </c>
+      <c r="G4" s="25" t="s">
+        <v>343</v>
+      </c>
+      <c r="H4" s="25"/>
+      <c r="I4" s="25"/>
+      <c r="J4" s="25" t="s">
+        <v>348</v>
+      </c>
+      <c r="K4" s="25" t="s">
+        <v>351</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A5" s="39"/>
-      <c r="B5" s="40" t="s">
-        <v>328</v>
-      </c>
-      <c r="C5" s="40" t="s">
-        <v>332</v>
-      </c>
-      <c r="D5" s="40" t="s">
-        <v>334</v>
-      </c>
-      <c r="E5" s="40" t="s">
-        <v>337</v>
-      </c>
-      <c r="F5" s="40" t="s">
-        <v>340</v>
-      </c>
-      <c r="G5" s="40"/>
-      <c r="H5" s="40"/>
-      <c r="I5" s="40"/>
-      <c r="J5" s="40"/>
-      <c r="K5" s="40"/>
+      <c r="B5" s="25" t="s">
+        <v>327</v>
+      </c>
+      <c r="C5" s="25" t="s">
+        <v>331</v>
+      </c>
+      <c r="D5" s="25" t="s">
+        <v>333</v>
+      </c>
+      <c r="E5" s="25" t="s">
+        <v>336</v>
+      </c>
+      <c r="F5" s="25" t="s">
+        <v>339</v>
+      </c>
+      <c r="G5" s="25"/>
+      <c r="H5" s="25"/>
+      <c r="I5" s="25"/>
+      <c r="J5" s="25"/>
+      <c r="K5" s="25"/>
     </row>
     <row r="6" spans="1:11" ht="32.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="39"/>
-      <c r="B6" s="40" t="s">
-        <v>329</v>
-      </c>
-      <c r="C6" s="40"/>
-      <c r="D6" s="40"/>
-      <c r="E6" s="40"/>
-      <c r="F6" s="40" t="s">
-        <v>341</v>
-      </c>
-      <c r="G6" s="40"/>
-      <c r="H6" s="40"/>
-      <c r="I6" s="40"/>
-      <c r="J6" s="40"/>
-      <c r="K6" s="40"/>
+      <c r="B6" s="25" t="s">
+        <v>328</v>
+      </c>
+      <c r="C6" s="25"/>
+      <c r="D6" s="25"/>
+      <c r="E6" s="25"/>
+      <c r="F6" s="25" t="s">
+        <v>340</v>
+      </c>
+      <c r="G6" s="25"/>
+      <c r="H6" s="25"/>
+      <c r="I6" s="25"/>
+      <c r="J6" s="25"/>
+      <c r="K6" s="25"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A7" s="51">
+      <c r="A7" s="27">
         <v>1</v>
       </c>
-      <c r="B7" s="51" t="s">
+      <c r="B7" s="27" t="s">
+        <v>352</v>
+      </c>
+      <c r="C7" s="25" t="s">
         <v>353</v>
       </c>
-      <c r="C7" s="40" t="s">
+      <c r="D7" s="25" t="s">
         <v>354</v>
       </c>
-      <c r="D7" s="40" t="s">
+      <c r="E7" s="35" t="s">
         <v>355</v>
       </c>
-      <c r="E7" s="47" t="s">
+      <c r="F7" s="25">
+        <v>901123121</v>
+      </c>
+      <c r="G7" s="36" t="s">
         <v>356</v>
       </c>
-      <c r="F7" s="40">
-        <v>901123121</v>
-      </c>
-      <c r="G7" s="49" t="s">
+      <c r="H7" s="27" t="s">
         <v>357</v>
       </c>
-      <c r="H7" s="51" t="s">
+      <c r="I7" s="27" t="s">
         <v>358</v>
       </c>
-      <c r="I7" s="51" t="s">
+      <c r="J7" s="27"/>
+      <c r="K7" s="27"/>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A8" s="27">
+        <v>2</v>
+      </c>
+      <c r="B8" s="27" t="s">
         <v>359</v>
       </c>
-      <c r="J7" s="51"/>
-      <c r="K7" s="51"/>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A8" s="51">
-        <v>2</v>
-      </c>
-      <c r="B8" s="51" t="s">
+      <c r="C8" s="25" t="s">
         <v>360</v>
       </c>
-      <c r="C8" s="40" t="s">
+      <c r="D8" s="25" t="s">
         <v>361</v>
       </c>
-      <c r="D8" s="40" t="s">
+      <c r="E8" s="35" t="s">
         <v>362</v>
       </c>
-      <c r="E8" s="47" t="s">
+      <c r="F8" s="25">
+        <v>901123122</v>
+      </c>
+      <c r="G8" s="36" t="s">
         <v>363</v>
       </c>
-      <c r="F8" s="40">
-        <v>901123122</v>
-      </c>
-      <c r="G8" s="49" t="s">
+      <c r="H8" s="27" t="s">
+        <v>357</v>
+      </c>
+      <c r="I8" s="27" t="s">
         <v>364</v>
       </c>
-      <c r="H8" s="51" t="s">
-        <v>358</v>
-      </c>
-      <c r="I8" s="51" t="s">
+      <c r="J8" s="27"/>
+      <c r="K8" s="27"/>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A9" s="27">
+        <v>3</v>
+      </c>
+      <c r="B9" s="27" t="s">
         <v>365</v>
       </c>
-      <c r="J8" s="51"/>
-      <c r="K8" s="51"/>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A9" s="51">
-        <v>3</v>
-      </c>
-      <c r="B9" s="51" t="s">
+      <c r="C9" s="25" t="s">
         <v>366</v>
       </c>
-      <c r="C9" s="40" t="s">
+      <c r="D9" s="25" t="s">
         <v>367</v>
       </c>
-      <c r="D9" s="40" t="s">
+      <c r="E9" s="35" t="s">
         <v>368</v>
       </c>
-      <c r="E9" s="47" t="s">
+      <c r="F9" s="25">
+        <v>901123123</v>
+      </c>
+      <c r="G9" s="36" t="s">
         <v>369</v>
       </c>
-      <c r="F9" s="40">
-        <v>901123123</v>
-      </c>
-      <c r="G9" s="49" t="s">
+      <c r="H9" s="27" t="s">
+        <v>357</v>
+      </c>
+      <c r="I9" s="27" t="s">
         <v>370</v>
       </c>
-      <c r="H9" s="51" t="s">
-        <v>358</v>
-      </c>
-      <c r="I9" s="51" t="s">
+      <c r="J9" s="27"/>
+      <c r="K9" s="27"/>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A10" s="27">
+        <v>4</v>
+      </c>
+      <c r="B10" s="27" t="s">
         <v>371</v>
       </c>
-      <c r="J9" s="51"/>
-      <c r="K9" s="51"/>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A10" s="51">
-        <v>4</v>
-      </c>
-      <c r="B10" s="51" t="s">
+      <c r="C10" s="25" t="s">
         <v>372</v>
       </c>
-      <c r="C10" s="40" t="s">
+      <c r="D10" s="25" t="s">
         <v>373</v>
       </c>
-      <c r="D10" s="40" t="s">
+      <c r="E10" s="35" t="s">
         <v>374</v>
       </c>
-      <c r="E10" s="47" t="s">
+      <c r="F10" s="25">
+        <v>901123124</v>
+      </c>
+      <c r="G10" s="36" t="s">
         <v>375</v>
       </c>
-      <c r="F10" s="40">
-        <v>901123124</v>
-      </c>
-      <c r="G10" s="49" t="s">
+      <c r="H10" s="27" t="s">
+        <v>357</v>
+      </c>
+      <c r="I10" s="27" t="s">
         <v>376</v>
       </c>
-      <c r="H10" s="51" t="s">
-        <v>358</v>
-      </c>
-      <c r="I10" s="51" t="s">
-        <v>377</v>
-      </c>
-      <c r="J10" s="51"/>
-      <c r="K10" s="51"/>
+      <c r="J10" s="27"/>
+      <c r="K10" s="27"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A11" s="35"/>
-      <c r="B11" s="35"/>
-      <c r="C11" s="33"/>
-      <c r="D11" s="33"/>
-      <c r="E11" s="47"/>
-      <c r="F11" s="33"/>
-      <c r="G11" s="49"/>
-      <c r="H11" s="35"/>
-      <c r="I11" s="35"/>
-      <c r="J11" s="35"/>
-      <c r="K11" s="35"/>
+      <c r="A11" s="27"/>
+      <c r="B11" s="27"/>
+      <c r="C11" s="25"/>
+      <c r="D11" s="25"/>
+      <c r="E11" s="35"/>
+      <c r="F11" s="25"/>
+      <c r="G11" s="36"/>
+      <c r="H11" s="27"/>
+      <c r="I11" s="27"/>
+      <c r="J11" s="27"/>
+      <c r="K11" s="27"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A12" s="35"/>
-      <c r="B12" s="35"/>
-      <c r="C12" s="33"/>
-      <c r="D12" s="33"/>
-      <c r="E12" s="47"/>
-      <c r="F12" s="33"/>
-      <c r="G12" s="49"/>
-      <c r="H12" s="35"/>
-      <c r="I12" s="35"/>
-      <c r="J12" s="35"/>
-      <c r="K12" s="35"/>
+      <c r="A12" s="27"/>
+      <c r="B12" s="27"/>
+      <c r="C12" s="25"/>
+      <c r="D12" s="25"/>
+      <c r="E12" s="35"/>
+      <c r="F12" s="25"/>
+      <c r="G12" s="36"/>
+      <c r="H12" s="27"/>
+      <c r="I12" s="27"/>
+      <c r="J12" s="27"/>
+      <c r="K12" s="27"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A13" s="35"/>
-      <c r="B13" s="35"/>
-      <c r="C13" s="33"/>
-      <c r="D13" s="33"/>
-      <c r="E13" s="47"/>
-      <c r="F13" s="33"/>
-      <c r="G13" s="49"/>
-      <c r="H13" s="35"/>
-      <c r="I13" s="35"/>
-      <c r="J13" s="35"/>
-      <c r="K13" s="35"/>
+      <c r="A13" s="27"/>
+      <c r="B13" s="27"/>
+      <c r="C13" s="25"/>
+      <c r="D13" s="25"/>
+      <c r="E13" s="35"/>
+      <c r="F13" s="25"/>
+      <c r="G13" s="36"/>
+      <c r="H13" s="27"/>
+      <c r="I13" s="27"/>
+      <c r="J13" s="27"/>
+      <c r="K13" s="27"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A14" s="35"/>
-      <c r="B14" s="35"/>
-      <c r="C14" s="33"/>
-      <c r="D14" s="33"/>
-      <c r="E14" s="47"/>
-      <c r="F14" s="33"/>
-      <c r="G14" s="49"/>
-      <c r="H14" s="35"/>
-      <c r="I14" s="38"/>
-      <c r="J14" s="35"/>
-      <c r="K14" s="35"/>
+      <c r="A14" s="27"/>
+      <c r="B14" s="27"/>
+      <c r="C14" s="25"/>
+      <c r="D14" s="25"/>
+      <c r="E14" s="35"/>
+      <c r="F14" s="25"/>
+      <c r="G14" s="36"/>
+      <c r="H14" s="27"/>
+      <c r="I14" s="28"/>
+      <c r="J14" s="27"/>
+      <c r="K14" s="27"/>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A15" s="35"/>
-      <c r="B15" s="35"/>
-      <c r="C15" s="33"/>
-      <c r="D15" s="33"/>
-      <c r="E15" s="47"/>
-      <c r="F15" s="33"/>
-      <c r="G15" s="49"/>
-      <c r="H15" s="35"/>
-      <c r="I15" s="38"/>
-      <c r="J15" s="35"/>
-      <c r="K15" s="35"/>
+      <c r="A15" s="27"/>
+      <c r="B15" s="27"/>
+      <c r="C15" s="25"/>
+      <c r="D15" s="25"/>
+      <c r="E15" s="35"/>
+      <c r="F15" s="25"/>
+      <c r="G15" s="36"/>
+      <c r="H15" s="27"/>
+      <c r="I15" s="28"/>
+      <c r="J15" s="27"/>
+      <c r="K15" s="27"/>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A16" s="35"/>
-      <c r="B16" s="35"/>
-      <c r="C16" s="33"/>
-      <c r="D16" s="33"/>
-      <c r="E16" s="47"/>
-      <c r="F16" s="33"/>
-      <c r="G16" s="49"/>
-      <c r="H16" s="35"/>
-      <c r="I16" s="38"/>
-      <c r="J16" s="35"/>
-      <c r="K16" s="35"/>
+      <c r="A16" s="27"/>
+      <c r="B16" s="27"/>
+      <c r="C16" s="25"/>
+      <c r="D16" s="25"/>
+      <c r="E16" s="35"/>
+      <c r="F16" s="25"/>
+      <c r="G16" s="36"/>
+      <c r="H16" s="27"/>
+      <c r="I16" s="28"/>
+      <c r="J16" s="27"/>
+      <c r="K16" s="27"/>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A17" s="35"/>
-      <c r="B17" s="35"/>
-      <c r="C17" s="33"/>
-      <c r="D17" s="33"/>
-      <c r="E17" s="47"/>
-      <c r="F17" s="33"/>
-      <c r="G17" s="49"/>
-      <c r="H17" s="35"/>
-      <c r="I17" s="38"/>
-      <c r="J17" s="35"/>
-      <c r="K17" s="35"/>
+      <c r="A17" s="27"/>
+      <c r="B17" s="27"/>
+      <c r="C17" s="25"/>
+      <c r="D17" s="25"/>
+      <c r="E17" s="35"/>
+      <c r="F17" s="25"/>
+      <c r="G17" s="36"/>
+      <c r="H17" s="27"/>
+      <c r="I17" s="28"/>
+      <c r="J17" s="27"/>
+      <c r="K17" s="27"/>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A18" s="35"/>
-      <c r="B18" s="35"/>
-      <c r="C18" s="33"/>
-      <c r="D18" s="33"/>
-      <c r="E18" s="47"/>
-      <c r="F18" s="33"/>
-      <c r="G18" s="49"/>
-      <c r="H18" s="35"/>
-      <c r="I18" s="35"/>
-      <c r="J18" s="35"/>
-      <c r="K18" s="35"/>
+      <c r="A18" s="27"/>
+      <c r="B18" s="27"/>
+      <c r="C18" s="25"/>
+      <c r="D18" s="25"/>
+      <c r="E18" s="35"/>
+      <c r="F18" s="25"/>
+      <c r="G18" s="36"/>
+      <c r="H18" s="27"/>
+      <c r="I18" s="27"/>
+      <c r="J18" s="27"/>
+      <c r="K18" s="27"/>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A19" s="35"/>
-      <c r="B19" s="35"/>
-      <c r="C19" s="33"/>
-      <c r="D19" s="33"/>
-      <c r="E19" s="47"/>
-      <c r="F19" s="33"/>
-      <c r="G19" s="49"/>
-      <c r="H19" s="35"/>
-      <c r="I19" s="35"/>
-      <c r="J19" s="35"/>
-      <c r="K19" s="35"/>
+      <c r="A19" s="27"/>
+      <c r="B19" s="27"/>
+      <c r="C19" s="25"/>
+      <c r="D19" s="25"/>
+      <c r="E19" s="35"/>
+      <c r="F19" s="25"/>
+      <c r="G19" s="36"/>
+      <c r="H19" s="27"/>
+      <c r="I19" s="27"/>
+      <c r="J19" s="27"/>
+      <c r="K19" s="27"/>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A20" s="35"/>
-      <c r="B20" s="35"/>
-      <c r="C20" s="33"/>
-      <c r="D20" s="33"/>
-      <c r="E20" s="47"/>
-      <c r="F20" s="33"/>
-      <c r="G20" s="49"/>
-      <c r="H20" s="35"/>
-      <c r="I20" s="35"/>
-      <c r="J20" s="35"/>
-      <c r="K20" s="35"/>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="E21" s="48"/>
+      <c r="A20" s="27"/>
+      <c r="B20" s="27"/>
+      <c r="C20" s="25"/>
+      <c r="D20" s="25"/>
+      <c r="E20" s="35"/>
+      <c r="F20" s="25"/>
+      <c r="G20" s="36"/>
+      <c r="H20" s="27"/>
+      <c r="I20" s="27"/>
+      <c r="J20" s="27"/>
+      <c r="K20" s="27"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -5292,249 +5278,249 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A1" s="32" t="s">
+      <c r="A1" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="32" t="s">
+      <c r="B1" s="24" t="s">
         <v>55</v>
       </c>
-      <c r="C1" s="32" t="s">
+      <c r="C1" s="24" t="s">
         <v>46</v>
       </c>
-      <c r="D1" s="32" t="s">
+      <c r="D1" s="24" t="s">
         <v>78</v>
       </c>
-      <c r="E1" s="32" t="s">
+      <c r="E1" s="24" t="s">
         <v>79</v>
       </c>
-      <c r="F1" s="32" t="s">
+      <c r="F1" s="24" t="s">
         <v>80</v>
       </c>
-      <c r="G1" s="32" t="s">
+      <c r="G1" s="24" t="s">
         <v>47</v>
       </c>
-      <c r="H1" s="32" t="s">
+      <c r="H1" s="24" t="s">
         <v>81</v>
       </c>
-      <c r="I1" s="32" t="s">
+      <c r="I1" s="24" t="s">
         <v>82</v>
       </c>
-      <c r="J1" s="32" t="s">
+      <c r="J1" s="24" t="s">
         <v>83</v>
       </c>
-      <c r="K1" s="32" t="s">
+      <c r="K1" s="24" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="2" spans="1:11" ht="92" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="37" t="s">
+      <c r="A2" s="38" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="33" t="s">
-        <v>310</v>
-      </c>
-      <c r="C2" s="33" t="s">
-        <v>313</v>
-      </c>
-      <c r="D2" s="33" t="s">
-        <v>313</v>
-      </c>
-      <c r="E2" s="33" t="s">
+      <c r="B2" s="25" t="s">
+        <v>309</v>
+      </c>
+      <c r="C2" s="25" t="s">
+        <v>312</v>
+      </c>
+      <c r="D2" s="25" t="s">
+        <v>312</v>
+      </c>
+      <c r="E2" s="25" t="s">
+        <v>385</v>
+      </c>
+      <c r="F2" s="38" t="s">
+        <v>85</v>
+      </c>
+      <c r="G2" s="25" t="s">
+        <v>315</v>
+      </c>
+      <c r="H2" s="25" t="s">
+        <v>388</v>
+      </c>
+      <c r="I2" s="25" t="s">
+        <v>389</v>
+      </c>
+      <c r="J2" s="25" t="s">
+        <v>388</v>
+      </c>
+      <c r="K2" s="25" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" ht="87" x14ac:dyDescent="0.35">
+      <c r="A3" s="39"/>
+      <c r="B3" s="25" t="s">
+        <v>378</v>
+      </c>
+      <c r="C3" s="25" t="s">
+        <v>381</v>
+      </c>
+      <c r="D3" s="25" t="s">
+        <v>383</v>
+      </c>
+      <c r="E3" s="25" t="s">
         <v>386</v>
       </c>
-      <c r="F2" s="37" t="s">
-        <v>85</v>
-      </c>
-      <c r="G2" s="33" t="s">
+      <c r="F3" s="39"/>
+      <c r="G3" s="25" t="s">
         <v>316</v>
       </c>
-      <c r="H2" s="33" t="s">
-        <v>389</v>
-      </c>
-      <c r="I2" s="33" t="s">
+      <c r="H3" s="25" t="s">
+        <v>328</v>
+      </c>
+      <c r="I3" s="25" t="s">
         <v>390</v>
       </c>
-      <c r="J2" s="33" t="s">
-        <v>389</v>
-      </c>
-      <c r="K2" s="33" t="s">
+      <c r="J3" s="25" t="s">
+        <v>328</v>
+      </c>
+      <c r="K3" s="25" t="s">
         <v>392</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="87" x14ac:dyDescent="0.35">
-      <c r="A3" s="36"/>
-      <c r="B3" s="33" t="s">
+    <row r="4" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A4" s="39"/>
+      <c r="B4" s="25" t="s">
         <v>379</v>
       </c>
-      <c r="C3" s="33" t="s">
+      <c r="C4" s="25" t="s">
         <v>382</v>
       </c>
-      <c r="D3" s="33" t="s">
+      <c r="D4" s="25" t="s">
         <v>384</v>
       </c>
-      <c r="E3" s="33" t="s">
+      <c r="E4" s="25" t="s">
+        <v>348</v>
+      </c>
+      <c r="F4" s="39"/>
+      <c r="G4" s="25" t="s">
         <v>387</v>
       </c>
-      <c r="F3" s="36"/>
-      <c r="G3" s="33" t="s">
+      <c r="H4" s="25"/>
+      <c r="I4" s="25"/>
+      <c r="J4" s="25"/>
+      <c r="K4" s="25"/>
+    </row>
+    <row r="5" spans="1:11" ht="29" x14ac:dyDescent="0.35">
+      <c r="A5" s="39"/>
+      <c r="B5" s="25" t="s">
+        <v>380</v>
+      </c>
+      <c r="C5" s="25"/>
+      <c r="D5" s="25"/>
+      <c r="E5" s="25"/>
+      <c r="F5" s="39"/>
+      <c r="G5" s="25" t="s">
         <v>317</v>
       </c>
-      <c r="H3" s="33" t="s">
-        <v>329</v>
-      </c>
-      <c r="I3" s="33" t="s">
-        <v>391</v>
-      </c>
-      <c r="J3" s="33" t="s">
-        <v>329</v>
-      </c>
-      <c r="K3" s="33" t="s">
+      <c r="H5" s="25"/>
+      <c r="I5" s="25"/>
+      <c r="J5" s="25"/>
+      <c r="K5" s="25"/>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A6" s="25">
+        <v>1</v>
+      </c>
+      <c r="B6" s="25" t="s">
+        <v>86</v>
+      </c>
+      <c r="C6" s="25" t="s">
+        <v>71</v>
+      </c>
+      <c r="D6" s="25">
+        <v>1</v>
+      </c>
+      <c r="E6" s="25"/>
+      <c r="F6" s="25"/>
+      <c r="G6" s="25"/>
+      <c r="H6" s="25"/>
+      <c r="I6" s="25" t="s">
+        <v>52</v>
+      </c>
+      <c r="J6" s="25"/>
+      <c r="K6" s="25"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A7" s="25">
+        <v>2</v>
+      </c>
+      <c r="B7" s="25" t="s">
+        <v>87</v>
+      </c>
+      <c r="C7" s="25" t="s">
+        <v>88</v>
+      </c>
+      <c r="D7" s="25">
+        <v>2</v>
+      </c>
+      <c r="E7" s="25" t="s">
+        <v>86</v>
+      </c>
+      <c r="F7" s="25"/>
+      <c r="G7" s="27" t="s">
+        <v>352</v>
+      </c>
+      <c r="H7" s="25"/>
+      <c r="I7" s="25" t="s">
         <v>393</v>
       </c>
-    </row>
-    <row r="4" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A4" s="36"/>
-      <c r="B4" s="33" t="s">
-        <v>380</v>
-      </c>
-      <c r="C4" s="33" t="s">
-        <v>383</v>
-      </c>
-      <c r="D4" s="33" t="s">
-        <v>385</v>
-      </c>
-      <c r="E4" s="33" t="s">
-        <v>349</v>
-      </c>
-      <c r="F4" s="36"/>
-      <c r="G4" s="33" t="s">
-        <v>388</v>
-      </c>
-      <c r="H4" s="33"/>
-      <c r="I4" s="33"/>
-      <c r="J4" s="33"/>
-      <c r="K4" s="33"/>
-    </row>
-    <row r="5" spans="1:11" ht="29" x14ac:dyDescent="0.35">
-      <c r="A5" s="36"/>
-      <c r="B5" s="33" t="s">
-        <v>381</v>
-      </c>
-      <c r="C5" s="33"/>
-      <c r="D5" s="33"/>
-      <c r="E5" s="33"/>
-      <c r="F5" s="36"/>
-      <c r="G5" s="33" t="s">
-        <v>318</v>
-      </c>
-      <c r="H5" s="33"/>
-      <c r="I5" s="33"/>
-      <c r="J5" s="33"/>
-      <c r="K5" s="33"/>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A6" s="33">
-        <v>1</v>
-      </c>
-      <c r="B6" s="33" t="s">
+      <c r="J7" s="25"/>
+      <c r="K7" s="25"/>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A8" s="25">
+        <v>3</v>
+      </c>
+      <c r="B8" s="25" t="s">
+        <v>50</v>
+      </c>
+      <c r="C8" s="25" t="s">
+        <v>89</v>
+      </c>
+      <c r="D8" s="25">
+        <v>2</v>
+      </c>
+      <c r="E8" s="25" t="s">
         <v>86</v>
       </c>
-      <c r="C6" s="33" t="s">
-        <v>71</v>
-      </c>
-      <c r="D6" s="33">
-        <v>1</v>
-      </c>
-      <c r="E6" s="33"/>
-      <c r="F6" s="33"/>
-      <c r="G6" s="33"/>
-      <c r="H6" s="33"/>
-      <c r="I6" s="33" t="s">
-        <v>52</v>
-      </c>
-      <c r="J6" s="33"/>
-      <c r="K6" s="33"/>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A7" s="33">
+      <c r="F8" s="25"/>
+      <c r="G8" s="25" t="s">
+        <v>394</v>
+      </c>
+      <c r="H8" s="25"/>
+      <c r="I8" s="25" t="s">
+        <v>90</v>
+      </c>
+      <c r="J8" s="25"/>
+      <c r="K8" s="25"/>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A9" s="25">
+        <v>4</v>
+      </c>
+      <c r="B9" s="25" t="s">
+        <v>91</v>
+      </c>
+      <c r="C9" s="25" t="s">
+        <v>92</v>
+      </c>
+      <c r="D9" s="25">
         <v>2</v>
       </c>
-      <c r="B7" s="33" t="s">
-        <v>87</v>
-      </c>
-      <c r="C7" s="33" t="s">
-        <v>88</v>
-      </c>
-      <c r="D7" s="33">
-        <v>2</v>
-      </c>
-      <c r="E7" s="33" t="s">
+      <c r="E9" s="25" t="s">
         <v>86</v>
       </c>
-      <c r="F7" s="33"/>
-      <c r="G7" s="35" t="s">
-        <v>353</v>
-      </c>
-      <c r="H7" s="33"/>
-      <c r="I7" s="33" t="s">
-        <v>394</v>
-      </c>
-      <c r="J7" s="33"/>
-      <c r="K7" s="33"/>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A8" s="33">
-        <v>3</v>
-      </c>
-      <c r="B8" s="33" t="s">
-        <v>50</v>
-      </c>
-      <c r="C8" s="33" t="s">
-        <v>89</v>
-      </c>
-      <c r="D8" s="33">
-        <v>2</v>
-      </c>
-      <c r="E8" s="33" t="s">
-        <v>86</v>
-      </c>
-      <c r="F8" s="33"/>
-      <c r="G8" s="33" t="s">
+      <c r="F9" s="25"/>
+      <c r="G9" s="25" t="s">
         <v>395</v>
       </c>
-      <c r="H8" s="33"/>
-      <c r="I8" s="33" t="s">
-        <v>90</v>
-      </c>
-      <c r="J8" s="33"/>
-      <c r="K8" s="33"/>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A9" s="33">
-        <v>4</v>
-      </c>
-      <c r="B9" s="33" t="s">
-        <v>91</v>
-      </c>
-      <c r="C9" s="33" t="s">
-        <v>92</v>
-      </c>
-      <c r="D9" s="33">
-        <v>2</v>
-      </c>
-      <c r="E9" s="33" t="s">
-        <v>86</v>
-      </c>
-      <c r="F9" s="33"/>
-      <c r="G9" s="33" t="s">
-        <v>396</v>
-      </c>
-      <c r="H9" s="33"/>
-      <c r="I9" s="33" t="s">
+      <c r="H9" s="25"/>
+      <c r="I9" s="25" t="s">
         <v>93</v>
       </c>
-      <c r="J9" s="33"/>
-      <c r="K9" s="33"/>
+      <c r="J9" s="25"/>
+      <c r="K9" s="25"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -5624,16 +5610,16 @@
       </c>
     </row>
     <row r="2" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A2" s="41" t="s">
+      <c r="A2" s="29" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="41" t="s">
+      <c r="B2" s="29" t="s">
         <v>99</v>
       </c>
-      <c r="C2" s="41" t="s">
+      <c r="C2" s="29" t="s">
         <v>100</v>
       </c>
-      <c r="D2" s="41"/>
+      <c r="D2" s="29"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5678,102 +5664,102 @@
       </c>
     </row>
     <row r="2" spans="1:6" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="A2" s="41" t="s">
+      <c r="A2" s="29" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="41" t="s">
+      <c r="B2" s="29" t="s">
         <v>105</v>
       </c>
-      <c r="C2" s="41" t="s">
+      <c r="C2" s="29" t="s">
         <v>106</v>
       </c>
-      <c r="D2" s="41" t="s">
+      <c r="D2" s="29" t="s">
+        <v>396</v>
+      </c>
+      <c r="E2" s="29" t="s">
+        <v>107</v>
+      </c>
+      <c r="F2" s="30" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A3" s="26">
+        <v>1</v>
+      </c>
+      <c r="B3" s="26" t="s">
         <v>397</v>
       </c>
-      <c r="E2" s="41" t="s">
-        <v>107</v>
-      </c>
-      <c r="F2" s="42" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A3" s="34">
+      <c r="C3" s="26" t="s">
+        <v>397</v>
+      </c>
+      <c r="D3" s="26">
         <v>1</v>
       </c>
-      <c r="B3" s="34" t="s">
+      <c r="E3" s="26" t="s">
+        <v>101</v>
+      </c>
+      <c r="F3" s="26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A4" s="26">
+        <v>2</v>
+      </c>
+      <c r="B4" s="26" t="s">
+        <v>190</v>
+      </c>
+      <c r="C4" s="26" t="s">
+        <v>190</v>
+      </c>
+      <c r="D4" s="26">
+        <v>1</v>
+      </c>
+      <c r="E4" s="26" t="s">
+        <v>101</v>
+      </c>
+      <c r="F4" s="26">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A5" s="26">
+        <v>3</v>
+      </c>
+      <c r="B5" s="26" t="s">
         <v>398</v>
       </c>
-      <c r="C3" s="34" t="s">
+      <c r="C5" s="26" t="s">
         <v>398</v>
       </c>
-      <c r="D3" s="34">
+      <c r="D5" s="26">
         <v>1</v>
       </c>
-      <c r="E3" s="34" t="s">
+      <c r="E5" s="26" t="s">
         <v>101</v>
       </c>
-      <c r="F3" s="34">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A4" s="34">
-        <v>2</v>
-      </c>
-      <c r="B4" s="34" t="s">
-        <v>191</v>
-      </c>
-      <c r="C4" s="34" t="s">
-        <v>191</v>
-      </c>
-      <c r="D4" s="34">
+      <c r="F5" s="26">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A6" s="26">
+        <v>4</v>
+      </c>
+      <c r="B6" s="26" t="s">
+        <v>399</v>
+      </c>
+      <c r="C6" s="26" t="s">
+        <v>399</v>
+      </c>
+      <c r="D6" s="26">
         <v>1</v>
       </c>
-      <c r="E4" s="34" t="s">
+      <c r="E6" s="26" t="s">
         <v>101</v>
       </c>
-      <c r="F4" s="34">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A5" s="34">
-        <v>3</v>
-      </c>
-      <c r="B5" s="34" t="s">
-        <v>399</v>
-      </c>
-      <c r="C5" s="34" t="s">
-        <v>399</v>
-      </c>
-      <c r="D5" s="34">
-        <v>1</v>
-      </c>
-      <c r="E5" s="34" t="s">
-        <v>101</v>
-      </c>
-      <c r="F5" s="34">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A6" s="34">
-        <v>4</v>
-      </c>
-      <c r="B6" s="34" t="s">
-        <v>400</v>
-      </c>
-      <c r="C6" s="34" t="s">
-        <v>400</v>
-      </c>
-      <c r="D6" s="34">
-        <v>1</v>
-      </c>
-      <c r="E6" s="34" t="s">
-        <v>101</v>
-      </c>
-      <c r="F6" s="34">
+      <c r="F6" s="26">
         <v>10</v>
       </c>
     </row>
@@ -5825,64 +5811,64 @@
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A3" s="33">
+      <c r="A3" s="25">
         <v>1</v>
       </c>
-      <c r="B3" s="33" t="s">
+      <c r="B3" s="25" t="s">
+        <v>400</v>
+      </c>
+      <c r="C3" s="25" t="s">
+        <v>111</v>
+      </c>
+      <c r="D3" s="25"/>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A4" s="25">
+        <v>2</v>
+      </c>
+      <c r="B4" s="25" t="s">
         <v>401</v>
       </c>
-      <c r="C3" s="33" t="s">
-        <v>111</v>
-      </c>
-      <c r="D3" s="33"/>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A4" s="33">
-        <v>2</v>
-      </c>
-      <c r="B4" s="33" t="s">
+      <c r="C4" s="25" t="s">
+        <v>113</v>
+      </c>
+      <c r="D4" s="25"/>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A5" s="25">
+        <v>3</v>
+      </c>
+      <c r="B5" s="25" t="s">
         <v>402</v>
       </c>
-      <c r="C4" s="33" t="s">
-        <v>113</v>
-      </c>
-      <c r="D4" s="33"/>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A5" s="33">
-        <v>3</v>
-      </c>
-      <c r="B5" s="33" t="s">
+      <c r="C5" s="25" t="s">
+        <v>114</v>
+      </c>
+      <c r="D5" s="25"/>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A6" s="25">
+        <v>4</v>
+      </c>
+      <c r="B6" s="25" t="s">
         <v>403</v>
       </c>
-      <c r="C5" s="33" t="s">
-        <v>114</v>
-      </c>
-      <c r="D5" s="33"/>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A6" s="33">
-        <v>4</v>
-      </c>
-      <c r="B6" s="33" t="s">
+      <c r="C6" s="25" t="s">
+        <v>115</v>
+      </c>
+      <c r="D6" s="25"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A7" s="25">
+        <v>5</v>
+      </c>
+      <c r="B7" s="25" t="s">
         <v>404</v>
       </c>
-      <c r="C6" s="33" t="s">
-        <v>115</v>
-      </c>
-      <c r="D6" s="33"/>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A7" s="33">
-        <v>5</v>
-      </c>
-      <c r="B7" s="33" t="s">
-        <v>405</v>
-      </c>
-      <c r="C7" s="33" t="s">
+      <c r="C7" s="25" t="s">
         <v>116</v>
       </c>
-      <c r="D7" s="33"/>
+      <c r="D7" s="25"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
[hotfix/master-viet] update file mega-import
</commit_message>
<xml_diff>
--- a/apps/core/fimport/static/fimport/template/mega-import.xlsx
+++ b/apps/core/fimport/static/fimport/template/mega-import.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PCAdmin\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DA6F90D-0E20-46C4-8977-6FD6ABD89992}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C70BC7A-A749-4AB1-82A1-73226D7A2C08}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="803" firstSheet="10" activeTab="16" xr2:uid="{ABCF866D-F0C2-489F-81F3-6B45D3E3629E}"/>
   </bookViews>
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="639" uniqueCount="450">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="644" uniqueCount="455">
   <si>
     <t>STT</t>
   </si>
@@ -1744,6 +1744,24 @@
     <t>- 1 là theo batch/Lot
 - 2 là theo serial num 
 - 0 là không có</t>
+  </si>
+  <si>
+    <t>Giá chung</t>
+  </si>
+  <si>
+    <t>-General price của sản phẩm</t>
+  </si>
+  <si>
+    <t>Phương thức định giá</t>
+  </si>
+  <si>
+    <t>Giá tiêu chuẩn</t>
+  </si>
+  <si>
+    <t>-0 là nhập trước xuất trước
+-1 là bình quân gia quyền
+-2 là thực tế đích danh
+- Bắt buộc nếu sản phẩm lưu kho</t>
   </si>
 </sst>
 </file>
@@ -3460,10 +3478,10 @@
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA1C2273-23CD-4D05-8CA4-F0EB0A365E8D}">
-  <dimension ref="A1:U5"/>
+  <dimension ref="A1:X5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
+      <selection activeCell="T9" sqref="T9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3480,14 +3498,16 @@
     <col min="10" max="10" width="24.453125" customWidth="1"/>
     <col min="11" max="11" width="11.1796875" customWidth="1"/>
     <col min="16" max="16" width="27.1796875" customWidth="1"/>
-    <col min="17" max="17" width="26.54296875" customWidth="1"/>
-    <col min="18" max="18" width="20" customWidth="1"/>
-    <col min="19" max="19" width="26" customWidth="1"/>
-    <col min="20" max="20" width="15.1796875" customWidth="1"/>
-    <col min="21" max="21" width="28.81640625" customWidth="1"/>
+    <col min="17" max="18" width="26.54296875" customWidth="1"/>
+    <col min="19" max="19" width="20" customWidth="1"/>
+    <col min="20" max="20" width="26.54296875" customWidth="1"/>
+    <col min="21" max="21" width="20" customWidth="1"/>
+    <col min="22" max="22" width="26" customWidth="1"/>
+    <col min="23" max="23" width="15.1796875" customWidth="1"/>
+    <col min="24" max="24" width="28.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" ht="29" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:24" ht="29" x14ac:dyDescent="0.35">
       <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
@@ -3540,19 +3560,28 @@
         <v>172</v>
       </c>
       <c r="R1" s="14" t="s">
+        <v>450</v>
+      </c>
+      <c r="S1" s="14" t="s">
         <v>173</v>
       </c>
-      <c r="S1" s="14" t="s">
+      <c r="T1" s="14" t="s">
+        <v>452</v>
+      </c>
+      <c r="U1" s="14" t="s">
+        <v>453</v>
+      </c>
+      <c r="V1" s="14" t="s">
         <v>174</v>
       </c>
-      <c r="T1" s="14" t="s">
+      <c r="W1" s="14" t="s">
         <v>175</v>
       </c>
-      <c r="U1" s="14" t="s">
+      <c r="X1" s="14" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="2" spans="1:21" ht="116" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:24" ht="116" x14ac:dyDescent="0.35">
       <c r="A2" s="7" t="s">
         <v>7</v>
       </c>
@@ -3591,19 +3620,26 @@
         <v>184</v>
       </c>
       <c r="R2" s="16" t="s">
+        <v>451</v>
+      </c>
+      <c r="S2" s="16" t="s">
         <v>185</v>
       </c>
-      <c r="S2" s="16" t="s">
+      <c r="T2" s="16" t="s">
+        <v>454</v>
+      </c>
+      <c r="U2" s="16"/>
+      <c r="V2" s="16" t="s">
         <v>186</v>
       </c>
-      <c r="T2" s="16" t="s">
+      <c r="W2" s="16" t="s">
         <v>187</v>
       </c>
-      <c r="U2" s="16" t="s">
+      <c r="X2" s="16" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A3" s="33">
         <v>1</v>
       </c>
@@ -3645,20 +3681,29 @@
       <c r="Q3" s="33" t="s">
         <v>398</v>
       </c>
-      <c r="R3" s="26" t="s">
-        <v>199</v>
+      <c r="R3" s="33">
+        <v>100000</v>
       </c>
       <c r="S3" s="26" t="s">
         <v>199</v>
       </c>
-      <c r="T3" s="33" t="s">
+      <c r="T3" s="33">
+        <v>0</v>
+      </c>
+      <c r="U3" s="26">
+        <v>100000</v>
+      </c>
+      <c r="V3" s="26" t="s">
+        <v>199</v>
+      </c>
+      <c r="W3" s="33" t="s">
         <v>398</v>
       </c>
-      <c r="U3" s="33">
+      <c r="X3" s="33">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A4" s="33">
         <v>2</v>
       </c>
@@ -3698,20 +3743,29 @@
       <c r="Q4" s="33" t="s">
         <v>398</v>
       </c>
-      <c r="R4" s="26" t="s">
-        <v>199</v>
+      <c r="R4" s="33">
+        <v>200000</v>
       </c>
       <c r="S4" s="26" t="s">
         <v>199</v>
       </c>
-      <c r="T4" s="33" t="s">
+      <c r="T4" s="33">
+        <v>0</v>
+      </c>
+      <c r="U4" s="26">
+        <v>200000</v>
+      </c>
+      <c r="V4" s="26" t="s">
+        <v>199</v>
+      </c>
+      <c r="W4" s="33" t="s">
         <v>398</v>
       </c>
-      <c r="U4" s="33">
+      <c r="X4" s="33">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A5" s="33">
         <v>3</v>
       </c>
@@ -3751,16 +3805,25 @@
       <c r="Q5" s="33" t="s">
         <v>398</v>
       </c>
-      <c r="R5" s="26" t="s">
-        <v>199</v>
+      <c r="R5" s="33">
+        <v>300000</v>
       </c>
       <c r="S5" s="26" t="s">
         <v>199</v>
       </c>
-      <c r="T5" s="33" t="s">
+      <c r="T5" s="33">
+        <v>0</v>
+      </c>
+      <c r="U5" s="26">
+        <v>300000</v>
+      </c>
+      <c r="V5" s="26" t="s">
+        <v>199</v>
+      </c>
+      <c r="W5" s="33" t="s">
         <v>398</v>
       </c>
-      <c r="U5" s="33">
+      <c r="X5" s="33">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
[hotfix/master-viet] update import product
</commit_message>
<xml_diff>
--- a/apps/core/fimport/static/fimport/template/mega-import.xlsx
+++ b/apps/core/fimport/static/fimport/template/mega-import.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PCAdmin\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C8E58F9-411C-4419-80E2-EF7E50B6D7F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6772712-56DC-4006-A84A-00F5591DA584}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="803" firstSheet="10" activeTab="16" xr2:uid="{ABCF866D-F0C2-489F-81F3-6B45D3E3629E}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="803" firstSheet="11" activeTab="17" xr2:uid="{ABCF866D-F0C2-489F-81F3-6B45D3E3629E}"/>
   </bookViews>
   <sheets>
     <sheet name="#account.users" sheetId="1" r:id="rId1"/>
@@ -29,11 +29,12 @@
     <sheet name="#saledata.product.uom" sheetId="20" r:id="rId14"/>
     <sheet name="#saledata.product.producttype" sheetId="17" r:id="rId15"/>
     <sheet name="#saledata.product.prodcategory" sheetId="18" r:id="rId16"/>
-    <sheet name="#saledata.product" sheetId="22" r:id="rId17"/>
-    <sheet name="#saledata.salutation" sheetId="8" r:id="rId18"/>
-    <sheet name="#saledata.contact" sheetId="9" r:id="rId19"/>
-    <sheet name="#saledata.payment-term" sheetId="14" r:id="rId20"/>
-    <sheet name="Guidelines - Chỉ dẫn" sheetId="6" r:id="rId21"/>
+    <sheet name="#saledata.product.manufacturer" sheetId="23" r:id="rId17"/>
+    <sheet name="#saledata.product" sheetId="22" r:id="rId18"/>
+    <sheet name="#saledata.salutation" sheetId="8" r:id="rId19"/>
+    <sheet name="#saledata.contact" sheetId="9" r:id="rId20"/>
+    <sheet name="#saledata.payment-term" sheetId="14" r:id="rId21"/>
+    <sheet name="Guidelines - Chỉ dẫn" sheetId="6" r:id="rId22"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -56,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="644" uniqueCount="455">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="656" uniqueCount="459">
   <si>
     <t>STT</t>
   </si>
@@ -1763,6 +1764,21 @@
 - Bắt buộc nếu sản phẩm lưu kho
 - Lưu ý: Khi import sản phẩm, trường hợp có cách ghi nhận khác các phương pháp này, sau khi hoàn tất cập nhập hệ thống, vui lòng vào chi tiết sản phẩm để điều chỉnh</t>
   </si>
+  <si>
+    <t>Hãng sản xuất</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - Mã hãng sản xuất tại #saledata.product.manufacturer</t>
+  </si>
+  <si>
+    <t>- Bắt buộc, định danh
+- Độ dài tối đa: 100
+- Ví dụ: manu001</t>
+  </si>
+  <si>
+    <t>- Tên của hãng
+- Ví dụ: Hãng 01</t>
+  </si>
 </sst>
 </file>
 
@@ -1839,7 +1855,7 @@
       <sz val="11"/>
       <color rgb="FF242424"/>
       <name val="Aptos Narrow"/>
-      <charset val="1"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
@@ -3393,7 +3409,7 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="I26" sqref="I26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3477,11 +3493,93 @@
 </file>
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E783ACB7-D919-4F74-AC1A-D54D8522C4AB}">
+  <dimension ref="A1:D5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="2" width="23.81640625" customWidth="1"/>
+    <col min="3" max="3" width="36" customWidth="1"/>
+    <col min="4" max="4" width="35.81640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A1" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A2" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>457</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>458</v>
+      </c>
+      <c r="D2" s="7"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A3" s="26">
+        <v>1</v>
+      </c>
+      <c r="B3" s="26">
+        <v>1</v>
+      </c>
+      <c r="C3" s="26" t="s">
+        <v>429</v>
+      </c>
+      <c r="D3" s="26"/>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A4" s="26">
+        <v>2</v>
+      </c>
+      <c r="B4" s="26">
+        <v>2</v>
+      </c>
+      <c r="C4" s="26" t="s">
+        <v>432</v>
+      </c>
+      <c r="D4" s="26"/>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A5" s="26">
+        <v>3</v>
+      </c>
+      <c r="B5" s="26">
+        <v>3</v>
+      </c>
+      <c r="C5" s="26" t="s">
+        <v>435</v>
+      </c>
+      <c r="D5" s="26"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA1C2273-23CD-4D05-8CA4-F0EB0A365E8D}">
-  <dimension ref="A1:X5"/>
+  <dimension ref="A1:Y5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="O1" workbookViewId="0">
-      <selection activeCell="T3" sqref="T3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3494,20 +3592,21 @@
     <col min="6" max="6" width="21.453125" customWidth="1"/>
     <col min="7" max="7" width="21.1796875" customWidth="1"/>
     <col min="8" max="8" width="24.453125" customWidth="1"/>
-    <col min="9" max="9" width="28.453125" customWidth="1"/>
-    <col min="10" max="10" width="24.453125" customWidth="1"/>
-    <col min="11" max="11" width="11.1796875" customWidth="1"/>
-    <col min="16" max="16" width="27.1796875" customWidth="1"/>
-    <col min="17" max="18" width="26.54296875" customWidth="1"/>
-    <col min="19" max="19" width="20" customWidth="1"/>
-    <col min="20" max="20" width="26.54296875" customWidth="1"/>
-    <col min="21" max="21" width="20" customWidth="1"/>
-    <col min="22" max="22" width="26" customWidth="1"/>
-    <col min="23" max="23" width="15.1796875" customWidth="1"/>
-    <col min="24" max="24" width="28.81640625" customWidth="1"/>
+    <col min="9" max="9" width="32.90625" customWidth="1"/>
+    <col min="10" max="10" width="28.453125" customWidth="1"/>
+    <col min="11" max="11" width="24.453125" customWidth="1"/>
+    <col min="12" max="12" width="11.1796875" customWidth="1"/>
+    <col min="17" max="17" width="27.1796875" customWidth="1"/>
+    <col min="18" max="19" width="26.54296875" customWidth="1"/>
+    <col min="20" max="20" width="20" customWidth="1"/>
+    <col min="21" max="21" width="26.54296875" customWidth="1"/>
+    <col min="22" max="22" width="20" customWidth="1"/>
+    <col min="23" max="23" width="26" customWidth="1"/>
+    <col min="24" max="24" width="15.1796875" customWidth="1"/>
+    <col min="25" max="25" width="28.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" ht="29" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:25" ht="29" x14ac:dyDescent="0.35">
       <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
@@ -3533,55 +3632,58 @@
         <v>163</v>
       </c>
       <c r="I1" s="14" t="s">
+        <v>455</v>
+      </c>
+      <c r="J1" s="14" t="s">
         <v>164</v>
       </c>
-      <c r="J1" s="14" t="s">
+      <c r="K1" s="14" t="s">
         <v>165</v>
       </c>
-      <c r="K1" s="14" t="s">
+      <c r="L1" s="14" t="s">
         <v>166</v>
       </c>
-      <c r="L1" s="14" t="s">
+      <c r="M1" s="14" t="s">
         <v>167</v>
       </c>
-      <c r="M1" s="14" t="s">
+      <c r="N1" s="14" t="s">
         <v>168</v>
       </c>
-      <c r="N1" s="14" t="s">
+      <c r="O1" s="14" t="s">
         <v>169</v>
       </c>
-      <c r="O1" s="14" t="s">
+      <c r="P1" s="14" t="s">
         <v>170</v>
       </c>
-      <c r="P1" s="14" t="s">
+      <c r="Q1" s="14" t="s">
         <v>171</v>
       </c>
-      <c r="Q1" s="14" t="s">
+      <c r="R1" s="14" t="s">
         <v>172</v>
       </c>
-      <c r="R1" s="14" t="s">
+      <c r="S1" s="14" t="s">
         <v>450</v>
       </c>
-      <c r="S1" s="14" t="s">
+      <c r="T1" s="14" t="s">
         <v>173</v>
       </c>
-      <c r="T1" s="14" t="s">
+      <c r="U1" s="14" t="s">
         <v>452</v>
       </c>
-      <c r="U1" s="14" t="s">
+      <c r="V1" s="14" t="s">
         <v>453</v>
       </c>
-      <c r="V1" s="14" t="s">
+      <c r="W1" s="14" t="s">
         <v>174</v>
       </c>
-      <c r="W1" s="14" t="s">
+      <c r="X1" s="14" t="s">
         <v>175</v>
       </c>
-      <c r="X1" s="14" t="s">
+      <c r="Y1" s="14" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="2" spans="1:24" ht="145" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:25" ht="145" x14ac:dyDescent="0.35">
       <c r="A2" s="7" t="s">
         <v>7</v>
       </c>
@@ -3602,44 +3704,47 @@
       <c r="H2" s="16" t="s">
         <v>181</v>
       </c>
-      <c r="I2" s="7" t="s">
+      <c r="I2" s="16" t="s">
+        <v>456</v>
+      </c>
+      <c r="J2" s="7" t="s">
         <v>182</v>
       </c>
-      <c r="J2" s="16" t="s">
+      <c r="K2" s="16" t="s">
         <v>449</v>
       </c>
-      <c r="K2" s="16"/>
       <c r="L2" s="16"/>
       <c r="M2" s="16"/>
       <c r="N2" s="16"/>
       <c r="O2" s="16"/>
-      <c r="P2" s="16" t="s">
+      <c r="P2" s="16"/>
+      <c r="Q2" s="16" t="s">
         <v>183</v>
       </c>
-      <c r="Q2" s="16" t="s">
+      <c r="R2" s="16" t="s">
         <v>184</v>
       </c>
-      <c r="R2" s="16" t="s">
+      <c r="S2" s="16" t="s">
         <v>451</v>
       </c>
-      <c r="S2" s="16" t="s">
+      <c r="T2" s="16" t="s">
         <v>185</v>
       </c>
-      <c r="T2" s="16" t="s">
+      <c r="U2" s="16" t="s">
         <v>454</v>
       </c>
-      <c r="U2" s="16"/>
-      <c r="V2" s="16" t="s">
+      <c r="V2" s="16"/>
+      <c r="W2" s="16" t="s">
         <v>186</v>
       </c>
-      <c r="W2" s="16" t="s">
+      <c r="X2" s="16" t="s">
         <v>187</v>
       </c>
-      <c r="X2" s="16" t="s">
+      <c r="Y2" s="16" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A3" s="33">
         <v>1</v>
       </c>
@@ -3664,46 +3769,45 @@
       <c r="H3" s="33" t="s">
         <v>428</v>
       </c>
-      <c r="I3" s="26" t="s">
+      <c r="I3" s="33"/>
+      <c r="J3" s="26" t="s">
         <v>200</v>
       </c>
-      <c r="J3" s="33">
+      <c r="K3" s="33">
         <v>1</v>
       </c>
-      <c r="K3" s="33"/>
       <c r="L3" s="33"/>
       <c r="M3" s="33"/>
       <c r="N3" s="33"/>
       <c r="O3" s="33"/>
-      <c r="P3" s="26" t="s">
+      <c r="P3" s="33"/>
+      <c r="Q3" s="26" t="s">
         <v>199</v>
       </c>
-      <c r="Q3" s="33" t="s">
+      <c r="R3" s="33" t="s">
         <v>398</v>
       </c>
-      <c r="R3" s="33">
+      <c r="S3" s="33"/>
+      <c r="T3" s="26" t="s">
+        <v>199</v>
+      </c>
+      <c r="U3" s="33">
+        <v>0</v>
+      </c>
+      <c r="V3" s="26">
         <v>100000</v>
       </c>
-      <c r="S3" s="26" t="s">
+      <c r="W3" s="26" t="s">
         <v>199</v>
       </c>
-      <c r="T3" s="33">
+      <c r="X3" s="33" t="s">
+        <v>398</v>
+      </c>
+      <c r="Y3" s="33">
         <v>0</v>
       </c>
-      <c r="U3" s="26">
-        <v>100000</v>
-      </c>
-      <c r="V3" s="26" t="s">
-        <v>199</v>
-      </c>
-      <c r="W3" s="33" t="s">
-        <v>398</v>
-      </c>
-      <c r="X3" s="33">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.35">
+    </row>
+    <row r="4" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A4" s="33">
         <v>2</v>
       </c>
@@ -3726,46 +3830,47 @@
       <c r="H4" s="33" t="s">
         <v>431</v>
       </c>
-      <c r="I4" s="26" t="s">
+      <c r="I4" s="33"/>
+      <c r="J4" s="26" t="s">
         <v>200</v>
       </c>
-      <c r="J4" s="33">
+      <c r="K4" s="33">
         <v>0</v>
       </c>
-      <c r="K4" s="33"/>
       <c r="L4" s="33"/>
       <c r="M4" s="33"/>
       <c r="N4" s="33"/>
       <c r="O4" s="33"/>
-      <c r="P4" s="26" t="s">
+      <c r="P4" s="33"/>
+      <c r="Q4" s="26" t="s">
         <v>199</v>
       </c>
-      <c r="Q4" s="33" t="s">
+      <c r="R4" s="33" t="s">
         <v>398</v>
       </c>
-      <c r="R4" s="33">
+      <c r="S4" s="33">
         <v>200000</v>
       </c>
-      <c r="S4" s="26" t="s">
+      <c r="T4" s="26" t="s">
         <v>199</v>
       </c>
-      <c r="T4" s="33">
+      <c r="U4" s="33">
         <v>0</v>
       </c>
-      <c r="U4" s="26">
+      <c r="V4" s="26">
         <v>200000</v>
       </c>
-      <c r="V4" s="26" t="s">
+      <c r="W4" s="26" t="s">
         <v>199</v>
       </c>
-      <c r="W4" s="33" t="s">
+      <c r="X4" s="33" t="s">
         <v>398</v>
       </c>
-      <c r="X4" s="33">
+      <c r="Y4" s="33">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A5" s="33">
         <v>3</v>
       </c>
@@ -3788,42 +3893,43 @@
       <c r="H5" s="33" t="s">
         <v>434</v>
       </c>
-      <c r="I5" s="26" t="s">
+      <c r="I5" s="33"/>
+      <c r="J5" s="26" t="s">
         <v>200</v>
       </c>
-      <c r="J5" s="33">
+      <c r="K5" s="33">
         <v>0</v>
       </c>
-      <c r="K5" s="33"/>
       <c r="L5" s="33"/>
       <c r="M5" s="33"/>
       <c r="N5" s="33"/>
       <c r="O5" s="33"/>
-      <c r="P5" s="26" t="s">
+      <c r="P5" s="33"/>
+      <c r="Q5" s="26" t="s">
         <v>199</v>
       </c>
-      <c r="Q5" s="33" t="s">
+      <c r="R5" s="33" t="s">
         <v>398</v>
       </c>
-      <c r="R5" s="33">
+      <c r="S5" s="33">
         <v>300000</v>
       </c>
-      <c r="S5" s="26" t="s">
+      <c r="T5" s="26" t="s">
         <v>199</v>
       </c>
-      <c r="T5" s="33">
+      <c r="U5" s="33">
         <v>0</v>
       </c>
-      <c r="U5" s="26">
+      <c r="V5" s="26">
         <v>300000</v>
       </c>
-      <c r="V5" s="26" t="s">
+      <c r="W5" s="26" t="s">
         <v>199</v>
       </c>
-      <c r="W5" s="33" t="s">
+      <c r="X5" s="33" t="s">
         <v>398</v>
       </c>
-      <c r="X5" s="33">
+      <c r="Y5" s="33">
         <v>0</v>
       </c>
     </row>
@@ -3832,7 +3938,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FDBA7C1B-B0F0-4AC8-A907-82185EA45827}">
   <dimension ref="A1:D4"/>
   <sheetViews>
@@ -3904,7 +4010,168 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C373C485-720B-481D-9EE6-F43D8158DF65}">
+  <dimension ref="A1:D11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="8.81640625" style="7"/>
+    <col min="2" max="2" width="48.453125" style="7" customWidth="1"/>
+    <col min="3" max="3" width="40" style="7" customWidth="1"/>
+    <col min="4" max="4" width="47.7265625" style="7" customWidth="1"/>
+    <col min="5" max="16384" width="8.81640625" style="7"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A1" s="24" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="24" t="s">
+        <v>45</v>
+      </c>
+      <c r="C1" s="24" t="s">
+        <v>46</v>
+      </c>
+      <c r="D1" s="24" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="75.650000000000006" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="38" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="25" t="s">
+        <v>309</v>
+      </c>
+      <c r="C2" s="25" t="s">
+        <v>312</v>
+      </c>
+      <c r="D2" s="25" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+      <c r="A3" s="39"/>
+      <c r="B3" s="25" t="s">
+        <v>310</v>
+      </c>
+      <c r="C3" s="25" t="s">
+        <v>313</v>
+      </c>
+      <c r="D3" s="25" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A4" s="39"/>
+      <c r="B4" s="25" t="s">
+        <v>311</v>
+      </c>
+      <c r="C4" s="25" t="s">
+        <v>314</v>
+      </c>
+      <c r="D4" s="25" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A5" s="25">
+        <v>1</v>
+      </c>
+      <c r="B5" s="25" t="s">
+        <v>318</v>
+      </c>
+      <c r="C5" s="25" t="s">
+        <v>48</v>
+      </c>
+      <c r="D5" s="25"/>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A6" s="25">
+        <v>2</v>
+      </c>
+      <c r="B6" s="25" t="s">
+        <v>319</v>
+      </c>
+      <c r="C6" s="25" t="s">
+        <v>49</v>
+      </c>
+      <c r="D6" s="25"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A7" s="25">
+        <v>3</v>
+      </c>
+      <c r="B7" s="25" t="s">
+        <v>50</v>
+      </c>
+      <c r="C7" s="25" t="s">
+        <v>51</v>
+      </c>
+      <c r="D7" s="27"/>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A8" s="25">
+        <v>4</v>
+      </c>
+      <c r="B8" s="25" t="s">
+        <v>320</v>
+      </c>
+      <c r="C8" s="25" t="s">
+        <v>321</v>
+      </c>
+      <c r="D8" s="25"/>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A9" s="25">
+        <v>5</v>
+      </c>
+      <c r="B9" s="25" t="s">
+        <v>322</v>
+      </c>
+      <c r="C9" s="25" t="s">
+        <v>52</v>
+      </c>
+      <c r="D9" s="25"/>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A10" s="25">
+        <v>6</v>
+      </c>
+      <c r="B10" s="25" t="s">
+        <v>53</v>
+      </c>
+      <c r="C10" s="25" t="s">
+        <v>54</v>
+      </c>
+      <c r="D10" s="25"/>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A11" s="25">
+        <v>7</v>
+      </c>
+      <c r="B11" s="25" t="s">
+        <v>323</v>
+      </c>
+      <c r="C11" s="25" t="s">
+        <v>324</v>
+      </c>
+      <c r="D11" s="25"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A2:A4"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A45619C8-AAF7-43DE-831A-2BED068D71D3}">
   <dimension ref="A1:K11"/>
   <sheetViews>
@@ -4055,168 +4322,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C373C485-720B-481D-9EE6-F43D8158DF65}">
-  <dimension ref="A1:D11"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="8.81640625" style="7"/>
-    <col min="2" max="2" width="48.453125" style="7" customWidth="1"/>
-    <col min="3" max="3" width="40" style="7" customWidth="1"/>
-    <col min="4" max="4" width="47.7265625" style="7" customWidth="1"/>
-    <col min="5" max="16384" width="8.81640625" style="7"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A1" s="24" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="24" t="s">
-        <v>45</v>
-      </c>
-      <c r="C1" s="24" t="s">
-        <v>46</v>
-      </c>
-      <c r="D1" s="24" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" ht="75.650000000000006" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="38" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2" s="25" t="s">
-        <v>309</v>
-      </c>
-      <c r="C2" s="25" t="s">
-        <v>312</v>
-      </c>
-      <c r="D2" s="25" t="s">
-        <v>315</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="29" x14ac:dyDescent="0.35">
-      <c r="A3" s="39"/>
-      <c r="B3" s="25" t="s">
-        <v>310</v>
-      </c>
-      <c r="C3" s="25" t="s">
-        <v>313</v>
-      </c>
-      <c r="D3" s="25" t="s">
-        <v>316</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A4" s="39"/>
-      <c r="B4" s="25" t="s">
-        <v>311</v>
-      </c>
-      <c r="C4" s="25" t="s">
-        <v>314</v>
-      </c>
-      <c r="D4" s="25" t="s">
-        <v>317</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A5" s="25">
-        <v>1</v>
-      </c>
-      <c r="B5" s="25" t="s">
-        <v>318</v>
-      </c>
-      <c r="C5" s="25" t="s">
-        <v>48</v>
-      </c>
-      <c r="D5" s="25"/>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A6" s="25">
-        <v>2</v>
-      </c>
-      <c r="B6" s="25" t="s">
-        <v>319</v>
-      </c>
-      <c r="C6" s="25" t="s">
-        <v>49</v>
-      </c>
-      <c r="D6" s="25"/>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A7" s="25">
-        <v>3</v>
-      </c>
-      <c r="B7" s="25" t="s">
-        <v>50</v>
-      </c>
-      <c r="C7" s="25" t="s">
-        <v>51</v>
-      </c>
-      <c r="D7" s="27"/>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A8" s="25">
-        <v>4</v>
-      </c>
-      <c r="B8" s="25" t="s">
-        <v>320</v>
-      </c>
-      <c r="C8" s="25" t="s">
-        <v>321</v>
-      </c>
-      <c r="D8" s="25"/>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A9" s="25">
-        <v>5</v>
-      </c>
-      <c r="B9" s="25" t="s">
-        <v>322</v>
-      </c>
-      <c r="C9" s="25" t="s">
-        <v>52</v>
-      </c>
-      <c r="D9" s="25"/>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A10" s="25">
-        <v>6</v>
-      </c>
-      <c r="B10" s="25" t="s">
-        <v>53</v>
-      </c>
-      <c r="C10" s="25" t="s">
-        <v>54</v>
-      </c>
-      <c r="D10" s="25"/>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A11" s="25">
-        <v>7</v>
-      </c>
-      <c r="B11" s="25" t="s">
-        <v>323</v>
-      </c>
-      <c r="C11" s="25" t="s">
-        <v>324</v>
-      </c>
-      <c r="D11" s="25"/>
-    </row>
-  </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A2:A4"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E863D4F3-258D-41FD-90A7-5BEE0F94C0B4}">
   <dimension ref="A1:F2"/>
   <sheetViews>
@@ -4282,7 +4388,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35B69A6E-98BC-434D-A419-FDB6C97F2A28}">
   <dimension ref="A1:E47"/>
   <sheetViews>

</xml_diff>

<commit_message>
[hotfix/master-viet] update file template import
</commit_message>
<xml_diff>
--- a/apps/core/fimport/static/fimport/template/mega-import.xlsx
+++ b/apps/core/fimport/static/fimport/template/mega-import.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PCAdmin\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6772712-56DC-4006-A84A-00F5591DA584}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0327FB89-AC43-4547-B79A-497DE098AF23}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="803" firstSheet="11" activeTab="17" xr2:uid="{ABCF866D-F0C2-489F-81F3-6B45D3E3629E}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="803" firstSheet="10" activeTab="10" xr2:uid="{ABCF866D-F0C2-489F-81F3-6B45D3E3629E}"/>
   </bookViews>
   <sheets>
     <sheet name="#account.users" sheetId="1" r:id="rId1"/>
@@ -27,14 +27,13 @@
     <sheet name="#saledata.account" sheetId="15" r:id="rId12"/>
     <sheet name="#saledata.product.uomgroup" sheetId="16" r:id="rId13"/>
     <sheet name="#saledata.product.uom" sheetId="20" r:id="rId14"/>
-    <sheet name="#saledata.product.producttype" sheetId="17" r:id="rId15"/>
-    <sheet name="#saledata.product.prodcategory" sheetId="18" r:id="rId16"/>
-    <sheet name="#saledata.product.manufacturer" sheetId="23" r:id="rId17"/>
-    <sheet name="#saledata.product" sheetId="22" r:id="rId18"/>
-    <sheet name="#saledata.salutation" sheetId="8" r:id="rId19"/>
-    <sheet name="#saledata.contact" sheetId="9" r:id="rId20"/>
-    <sheet name="#saledata.payment-term" sheetId="14" r:id="rId21"/>
-    <sheet name="Guidelines - Chỉ dẫn" sheetId="6" r:id="rId22"/>
+    <sheet name="#saledata.product.prodcategory" sheetId="18" r:id="rId15"/>
+    <sheet name="#saledata.product.manufacturer" sheetId="23" r:id="rId16"/>
+    <sheet name="#saledata.product" sheetId="22" r:id="rId17"/>
+    <sheet name="#saledata.salutation" sheetId="8" r:id="rId18"/>
+    <sheet name="#saledata.contact" sheetId="9" r:id="rId19"/>
+    <sheet name="#saledata.payment-term" sheetId="14" r:id="rId20"/>
+    <sheet name="Guidelines - Chỉ dẫn" sheetId="6" r:id="rId21"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -57,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="656" uniqueCount="459">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="646" uniqueCount="455">
   <si>
     <t>STT</t>
   </si>
@@ -699,11 +698,6 @@
   </si>
   <si>
     <t>- Bắt buộc
-- Mã loại sản phẩm tại #saledata.product.producttype
-- Ví dụ: finished_goods</t>
-  </si>
-  <si>
-    <t>- Bắt buộc
 - Mã danh mục sản phẩm tại #saledata.product.prodcategory
 - Ví dụ: 001</t>
   </si>
@@ -747,10 +741,6 @@
   <si>
     <t>- Tên của nhóm đơn vị tính
 - Ví dụ: Unit</t>
-  </si>
-  <si>
-    <t>- Tên của loại sản phẩm
-- Ví dụ: Thành phẩm</t>
   </si>
   <si>
     <t>- Tên của danh mục sản phẩm
@@ -1228,9 +1218,6 @@
     <t>#saledata.price.taxcategory</t>
   </si>
   <si>
-    <t>#saledata.product.producttype</t>
-  </si>
-  <si>
     <t>#saledata.product.prodcategory</t>
   </si>
   <si>
@@ -1264,9 +1251,6 @@
     <t>Danh xưng</t>
   </si>
   <si>
-    <t>Loại sản phẩm</t>
-  </si>
-  <si>
     <t>Danh mục sản phẩm</t>
   </si>
   <si>
@@ -1298,9 +1282,6 @@
   </si>
   <si>
     <t>Unit Of Measure</t>
-  </si>
-  <si>
-    <t>Product Type</t>
   </si>
   <si>
     <t>Product Category</t>
@@ -1778,6 +1759,11 @@
   <si>
     <t>- Tên của hãng
 - Ví dụ: Hãng 01</t>
+  </si>
+  <si>
+    <t>- Bắt buộc
+- Mã loại sản phẩm tại tính năng master data config/ item/ product types
+- Ví dụ: finished_goods</t>
   </si>
 </sst>
 </file>
@@ -2714,10 +2700,10 @@
         <v>1</v>
       </c>
       <c r="B3" s="25" t="s">
-        <v>405</v>
+        <v>400</v>
       </c>
       <c r="C3" s="25" t="s">
-        <v>406</v>
+        <v>401</v>
       </c>
       <c r="D3" s="25"/>
     </row>
@@ -2726,10 +2712,10 @@
         <v>2</v>
       </c>
       <c r="B4" s="25" t="s">
-        <v>407</v>
+        <v>402</v>
       </c>
       <c r="C4" s="25" t="s">
-        <v>408</v>
+        <v>403</v>
       </c>
       <c r="D4" s="25"/>
     </row>
@@ -2738,10 +2724,10 @@
         <v>3</v>
       </c>
       <c r="B5" s="25" t="s">
-        <v>409</v>
+        <v>404</v>
       </c>
       <c r="C5" s="25" t="s">
-        <v>410</v>
+        <v>405</v>
       </c>
       <c r="D5" s="25"/>
     </row>
@@ -2754,8 +2740,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ACBC7503-D39D-4D5C-B33A-E4C15DD2E38F}">
   <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2797,7 +2783,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="25" t="s">
-        <v>411</v>
+        <v>406</v>
       </c>
       <c r="C3" s="25" t="s">
         <v>121</v>
@@ -2809,7 +2795,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="25" t="s">
-        <v>412</v>
+        <v>407</v>
       </c>
       <c r="C4" s="25" t="s">
         <v>122</v>
@@ -2821,7 +2807,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="25" t="s">
-        <v>413</v>
+        <v>408</v>
       </c>
       <c r="C5" s="25" t="s">
         <v>123</v>
@@ -2833,7 +2819,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="25" t="s">
-        <v>414</v>
+        <v>409</v>
       </c>
       <c r="C6" s="25" t="s">
         <v>124</v>
@@ -2972,7 +2958,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="25" t="s">
-        <v>415</v>
+        <v>410</v>
       </c>
       <c r="C3" s="25" t="s">
         <v>154</v>
@@ -2984,13 +2970,13 @@
         <v>1</v>
       </c>
       <c r="F3" s="25" t="s">
-        <v>400</v>
+        <v>395</v>
       </c>
       <c r="G3" s="25" t="s">
-        <v>411</v>
+        <v>406</v>
       </c>
       <c r="H3" s="27" t="s">
-        <v>352</v>
+        <v>347</v>
       </c>
       <c r="I3" s="25"/>
       <c r="J3" s="25"/>
@@ -3010,7 +2996,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="25" t="s">
-        <v>416</v>
+        <v>411</v>
       </c>
       <c r="C4" s="25" t="s">
         <v>156</v>
@@ -3022,13 +3008,13 @@
         <v>1</v>
       </c>
       <c r="F4" s="25" t="s">
-        <v>401</v>
+        <v>396</v>
       </c>
       <c r="G4" s="25" t="s">
-        <v>412</v>
+        <v>407</v>
       </c>
       <c r="H4" s="27" t="s">
-        <v>359</v>
+        <v>354</v>
       </c>
       <c r="I4" s="25"/>
       <c r="J4" s="25"/>
@@ -3048,7 +3034,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="25" t="s">
-        <v>417</v>
+        <v>412</v>
       </c>
       <c r="C5" s="25" t="s">
         <v>158</v>
@@ -3060,13 +3046,13 @@
         <v>1</v>
       </c>
       <c r="F5" s="25" t="s">
-        <v>402</v>
+        <v>397</v>
       </c>
       <c r="G5" s="25" t="s">
-        <v>413</v>
+        <v>408</v>
       </c>
       <c r="H5" s="27" t="s">
-        <v>365</v>
+        <v>360</v>
       </c>
       <c r="I5" s="25"/>
       <c r="J5" s="25"/>
@@ -3124,7 +3110,7 @@
         <v>177</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="D2" s="7"/>
     </row>
@@ -3133,10 +3119,10 @@
         <v>1</v>
       </c>
       <c r="B3" s="26" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="C3" s="26" t="s">
-        <v>418</v>
+        <v>413</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
@@ -3144,7 +3130,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="26" t="s">
-        <v>419</v>
+        <v>414</v>
       </c>
       <c r="C4" s="26" t="s">
         <v>170</v>
@@ -3188,13 +3174,13 @@
         <v>164</v>
       </c>
       <c r="E1" s="8" t="s">
+        <v>192</v>
+      </c>
+      <c r="F1" s="8" t="s">
+        <v>193</v>
+      </c>
+      <c r="G1" s="8" t="s">
         <v>194</v>
-      </c>
-      <c r="F1" s="8" t="s">
-        <v>195</v>
-      </c>
-      <c r="G1" s="8" t="s">
-        <v>196</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="58" x14ac:dyDescent="0.35">
@@ -3202,16 +3188,16 @@
         <v>7</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>427</v>
+        <v>422</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.35">
@@ -3219,13 +3205,13 @@
         <v>1</v>
       </c>
       <c r="B3" s="26" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="C3" s="26" t="s">
-        <v>420</v>
+        <v>415</v>
       </c>
       <c r="D3" s="15" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="E3" s="25">
         <v>1</v>
@@ -3242,13 +3228,13 @@
         <v>2</v>
       </c>
       <c r="B4" s="26" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="C4" s="26" t="s">
-        <v>421</v>
+        <v>416</v>
       </c>
       <c r="D4" s="15" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="E4" s="25">
         <v>0</v>
@@ -3265,13 +3251,13 @@
         <v>3</v>
       </c>
       <c r="B5" s="26" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="C5" s="26" t="s">
-        <v>422</v>
+        <v>417</v>
       </c>
       <c r="D5" s="15" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="E5" s="25">
         <v>0</v>
@@ -3288,13 +3274,13 @@
         <v>4</v>
       </c>
       <c r="B6" s="26" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="C6" s="26" t="s">
-        <v>423</v>
+        <v>418</v>
       </c>
       <c r="D6" s="15" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="E6" s="25">
         <v>0</v>
@@ -3311,13 +3297,13 @@
         <v>5</v>
       </c>
       <c r="B7" s="26" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="C7" s="26" t="s">
-        <v>424</v>
+        <v>419</v>
       </c>
       <c r="D7" s="15" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="E7" s="25">
         <v>0</v>
@@ -3334,13 +3320,13 @@
         <v>6</v>
       </c>
       <c r="B8" s="26" t="s">
-        <v>425</v>
+        <v>420</v>
       </c>
       <c r="C8" s="26" t="s">
-        <v>426</v>
+        <v>421</v>
       </c>
       <c r="D8" s="15" t="s">
-        <v>419</v>
+        <v>414</v>
       </c>
       <c r="E8" s="32">
         <v>1</v>
@@ -3359,52 +3345,6 @@
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C93ACA88-1D16-403D-BA6F-0FEB58847BDF}">
-  <dimension ref="A1:D2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="2" max="2" width="30.1796875" customWidth="1"/>
-    <col min="3" max="3" width="28.26953125" customWidth="1"/>
-    <col min="4" max="4" width="23.1796875" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A1" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="8" t="s">
-        <v>55</v>
-      </c>
-      <c r="C1" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="D1" s="8" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A2" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2" s="7" t="s">
-        <v>177</v>
-      </c>
-      <c r="C2" s="7" t="s">
-        <v>192</v>
-      </c>
-      <c r="D2" s="7"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{103DB413-C452-4A76-9162-EF01DE565453}">
   <dimension ref="A1:D5"/>
   <sheetViews>
@@ -3441,7 +3381,7 @@
         <v>177</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="D2" s="7"/>
     </row>
@@ -3450,13 +3390,13 @@
         <v>1</v>
       </c>
       <c r="B3" s="26" t="s">
-        <v>428</v>
+        <v>423</v>
       </c>
       <c r="C3" s="26" t="s">
-        <v>429</v>
+        <v>424</v>
       </c>
       <c r="D3" s="26" t="s">
-        <v>430</v>
+        <v>425</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
@@ -3464,13 +3404,13 @@
         <v>2</v>
       </c>
       <c r="B4" s="26" t="s">
-        <v>431</v>
+        <v>426</v>
       </c>
       <c r="C4" s="26" t="s">
-        <v>432</v>
+        <v>427</v>
       </c>
       <c r="D4" s="26" t="s">
-        <v>433</v>
+        <v>428</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.35">
@@ -3478,13 +3418,13 @@
         <v>3</v>
       </c>
       <c r="B5" s="26" t="s">
-        <v>434</v>
+        <v>429</v>
       </c>
       <c r="C5" s="26" t="s">
-        <v>435</v>
+        <v>430</v>
       </c>
       <c r="D5" s="26" t="s">
-        <v>436</v>
+        <v>431</v>
       </c>
     </row>
   </sheetData>
@@ -3492,7 +3432,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E783ACB7-D919-4F74-AC1A-D54D8522C4AB}">
   <dimension ref="A1:D5"/>
   <sheetViews>
@@ -3526,10 +3466,10 @@
         <v>7</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>457</v>
+        <v>452</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>458</v>
+        <v>453</v>
       </c>
       <c r="D2" s="7"/>
     </row>
@@ -3541,7 +3481,7 @@
         <v>1</v>
       </c>
       <c r="C3" s="26" t="s">
-        <v>429</v>
+        <v>424</v>
       </c>
       <c r="D3" s="26"/>
     </row>
@@ -3553,7 +3493,7 @@
         <v>2</v>
       </c>
       <c r="C4" s="26" t="s">
-        <v>432</v>
+        <v>427</v>
       </c>
       <c r="D4" s="26"/>
     </row>
@@ -3565,7 +3505,7 @@
         <v>3</v>
       </c>
       <c r="C5" s="26" t="s">
-        <v>435</v>
+        <v>430</v>
       </c>
       <c r="D5" s="26"/>
     </row>
@@ -3574,12 +3514,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA1C2273-23CD-4D05-8CA4-F0EB0A365E8D}">
   <dimension ref="A1:Y5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3632,7 +3572,7 @@
         <v>163</v>
       </c>
       <c r="I1" s="14" t="s">
-        <v>455</v>
+        <v>450</v>
       </c>
       <c r="J1" s="14" t="s">
         <v>164</v>
@@ -3662,16 +3602,16 @@
         <v>172</v>
       </c>
       <c r="S1" s="14" t="s">
-        <v>450</v>
+        <v>445</v>
       </c>
       <c r="T1" s="14" t="s">
         <v>173</v>
       </c>
       <c r="U1" s="14" t="s">
-        <v>452</v>
+        <v>447</v>
       </c>
       <c r="V1" s="14" t="s">
-        <v>453</v>
+        <v>448</v>
       </c>
       <c r="W1" s="14" t="s">
         <v>174</v>
@@ -3699,19 +3639,19 @@
         <v>179</v>
       </c>
       <c r="G2" s="16" t="s">
+        <v>454</v>
+      </c>
+      <c r="H2" s="16" t="s">
         <v>180</v>
       </c>
-      <c r="H2" s="16" t="s">
+      <c r="I2" s="16" t="s">
+        <v>451</v>
+      </c>
+      <c r="J2" s="7" t="s">
         <v>181</v>
       </c>
-      <c r="I2" s="16" t="s">
-        <v>456</v>
-      </c>
-      <c r="J2" s="7" t="s">
-        <v>182</v>
-      </c>
       <c r="K2" s="16" t="s">
-        <v>449</v>
+        <v>444</v>
       </c>
       <c r="L2" s="16"/>
       <c r="M2" s="16"/>
@@ -3719,29 +3659,29 @@
       <c r="O2" s="16"/>
       <c r="P2" s="16"/>
       <c r="Q2" s="16" t="s">
+        <v>182</v>
+      </c>
+      <c r="R2" s="16" t="s">
         <v>183</v>
       </c>
-      <c r="R2" s="16" t="s">
+      <c r="S2" s="16" t="s">
+        <v>446</v>
+      </c>
+      <c r="T2" s="16" t="s">
         <v>184</v>
       </c>
-      <c r="S2" s="16" t="s">
-        <v>451</v>
-      </c>
-      <c r="T2" s="16" t="s">
-        <v>185</v>
-      </c>
       <c r="U2" s="16" t="s">
-        <v>454</v>
+        <v>449</v>
       </c>
       <c r="V2" s="16"/>
       <c r="W2" s="16" t="s">
+        <v>185</v>
+      </c>
+      <c r="X2" s="16" t="s">
         <v>186</v>
       </c>
-      <c r="X2" s="16" t="s">
+      <c r="Y2" s="16" t="s">
         <v>187</v>
-      </c>
-      <c r="Y2" s="16" t="s">
-        <v>188</v>
       </c>
     </row>
     <row r="3" spans="1:25" x14ac:dyDescent="0.35">
@@ -3749,29 +3689,29 @@
         <v>1</v>
       </c>
       <c r="B3" s="33" t="s">
-        <v>437</v>
+        <v>432</v>
       </c>
       <c r="C3" s="33" t="s">
-        <v>438</v>
+        <v>433</v>
       </c>
       <c r="D3" s="33">
         <v>123</v>
       </c>
       <c r="E3" s="33" t="s">
-        <v>430</v>
+        <v>425</v>
       </c>
       <c r="F3" s="33" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="G3" s="33" t="s">
-        <v>439</v>
+        <v>434</v>
       </c>
       <c r="H3" s="33" t="s">
-        <v>428</v>
+        <v>423</v>
       </c>
       <c r="I3" s="33"/>
       <c r="J3" s="26" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="K3" s="33">
         <v>1</v>
@@ -3782,14 +3722,14 @@
       <c r="O3" s="33"/>
       <c r="P3" s="33"/>
       <c r="Q3" s="26" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="R3" s="33" t="s">
-        <v>398</v>
+        <v>393</v>
       </c>
       <c r="S3" s="33"/>
       <c r="T3" s="26" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="U3" s="33">
         <v>0</v>
@@ -3798,10 +3738,10 @@
         <v>100000</v>
       </c>
       <c r="W3" s="26" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="X3" s="33" t="s">
-        <v>398</v>
+        <v>393</v>
       </c>
       <c r="Y3" s="33">
         <v>0</v>
@@ -3812,27 +3752,27 @@
         <v>2</v>
       </c>
       <c r="B4" s="33" t="s">
-        <v>440</v>
+        <v>435</v>
       </c>
       <c r="C4" s="33" t="s">
-        <v>441</v>
+        <v>436</v>
       </c>
       <c r="D4" s="33"/>
       <c r="E4" s="33" t="s">
-        <v>433</v>
+        <v>428</v>
       </c>
       <c r="F4" s="33" t="s">
-        <v>442</v>
+        <v>437</v>
       </c>
       <c r="G4" s="33" t="s">
-        <v>439</v>
+        <v>434</v>
       </c>
       <c r="H4" s="33" t="s">
-        <v>431</v>
+        <v>426</v>
       </c>
       <c r="I4" s="33"/>
       <c r="J4" s="26" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="K4" s="33">
         <v>0</v>
@@ -3843,16 +3783,16 @@
       <c r="O4" s="33"/>
       <c r="P4" s="33"/>
       <c r="Q4" s="26" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="R4" s="33" t="s">
-        <v>398</v>
+        <v>393</v>
       </c>
       <c r="S4" s="33">
         <v>200000</v>
       </c>
       <c r="T4" s="26" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="U4" s="33">
         <v>0</v>
@@ -3861,10 +3801,10 @@
         <v>200000</v>
       </c>
       <c r="W4" s="26" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="X4" s="33" t="s">
-        <v>398</v>
+        <v>393</v>
       </c>
       <c r="Y4" s="33">
         <v>0</v>
@@ -3875,27 +3815,27 @@
         <v>3</v>
       </c>
       <c r="B5" s="33" t="s">
-        <v>443</v>
+        <v>438</v>
       </c>
       <c r="C5" s="33" t="s">
-        <v>444</v>
+        <v>439</v>
       </c>
       <c r="D5" s="33"/>
       <c r="E5" s="33" t="s">
-        <v>436</v>
+        <v>431</v>
       </c>
       <c r="F5" s="33" t="s">
-        <v>442</v>
+        <v>437</v>
       </c>
       <c r="G5" s="33" t="s">
-        <v>445</v>
+        <v>440</v>
       </c>
       <c r="H5" s="33" t="s">
-        <v>434</v>
+        <v>429</v>
       </c>
       <c r="I5" s="33"/>
       <c r="J5" s="26" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="K5" s="33">
         <v>0</v>
@@ -3906,16 +3846,16 @@
       <c r="O5" s="33"/>
       <c r="P5" s="33"/>
       <c r="Q5" s="26" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="R5" s="33" t="s">
-        <v>398</v>
+        <v>393</v>
       </c>
       <c r="S5" s="33">
         <v>300000</v>
       </c>
       <c r="T5" s="26" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="U5" s="33">
         <v>0</v>
@@ -3924,10 +3864,10 @@
         <v>300000</v>
       </c>
       <c r="W5" s="26" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="X5" s="33" t="s">
-        <v>398</v>
+        <v>393</v>
       </c>
       <c r="Y5" s="33">
         <v>0</v>
@@ -3938,7 +3878,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FDBA7C1B-B0F0-4AC8-A907-82185EA45827}">
   <dimension ref="A1:D4"/>
   <sheetViews>
@@ -3974,13 +3914,13 @@
         <v>7</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
@@ -3991,7 +3931,7 @@
         <v>110</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
@@ -4002,10 +3942,161 @@
         <v>112</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
     </row>
   </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A45619C8-AAF7-43DE-831A-2BED068D71D3}">
+  <dimension ref="A1:K11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="10.26953125" style="7" customWidth="1"/>
+    <col min="2" max="2" width="21.453125" style="7" customWidth="1"/>
+    <col min="3" max="3" width="28.7265625" style="7" customWidth="1"/>
+    <col min="4" max="4" width="28.54296875" style="7" customWidth="1"/>
+    <col min="5" max="5" width="25.26953125" style="7" customWidth="1"/>
+    <col min="6" max="6" width="21.54296875" style="7" customWidth="1"/>
+    <col min="7" max="7" width="12.26953125" style="7" customWidth="1"/>
+    <col min="8" max="8" width="19.1796875" style="7" customWidth="1"/>
+    <col min="9" max="11" width="23.26953125" style="7" customWidth="1"/>
+    <col min="12" max="16384" width="8.81640625" style="7"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A1" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>208</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>209</v>
+      </c>
+      <c r="E1" s="8" t="s">
+        <v>210</v>
+      </c>
+      <c r="F1" s="8" t="s">
+        <v>211</v>
+      </c>
+      <c r="G1" s="8" t="s">
+        <v>212</v>
+      </c>
+      <c r="H1" s="8" t="s">
+        <v>213</v>
+      </c>
+      <c r="I1" s="8" t="s">
+        <v>214</v>
+      </c>
+      <c r="J1" s="8" t="s">
+        <v>215</v>
+      </c>
+      <c r="K1" s="8" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" ht="85.9" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>217</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>218</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>219</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>220</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>221</v>
+      </c>
+      <c r="G2" s="7" t="s">
+        <v>222</v>
+      </c>
+      <c r="H2" s="7" t="s">
+        <v>223</v>
+      </c>
+      <c r="I2" s="7" t="s">
+        <v>224</v>
+      </c>
+      <c r="J2" s="7" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A3" s="25">
+        <v>1</v>
+      </c>
+      <c r="B3" s="25" t="s">
+        <v>441</v>
+      </c>
+      <c r="C3" s="27" t="s">
+        <v>372</v>
+      </c>
+      <c r="D3" s="25">
+        <v>1</v>
+      </c>
+      <c r="E3" s="25" t="s">
+        <v>442</v>
+      </c>
+      <c r="F3" s="25" t="s">
+        <v>226</v>
+      </c>
+      <c r="G3" s="25"/>
+      <c r="H3" s="25">
+        <v>903331332</v>
+      </c>
+      <c r="I3" s="34" t="s">
+        <v>443</v>
+      </c>
+      <c r="J3" s="25"/>
+      <c r="K3" s="25"/>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="I4" s="12"/>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="I5" s="12"/>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="I6" s="12"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="I7" s="12"/>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="I8" s="12"/>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="I9" s="12"/>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="I10" s="12"/>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="I11" s="12"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="6" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="I3" r:id="rId1" display="mailto:nva@example.com" xr:uid="{F6D89C5D-FF1D-47B0-919B-E0B60A9F5428}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -4046,37 +4137,37 @@
         <v>7</v>
       </c>
       <c r="B2" s="25" t="s">
-        <v>309</v>
+        <v>304</v>
       </c>
       <c r="C2" s="25" t="s">
-        <v>312</v>
+        <v>307</v>
       </c>
       <c r="D2" s="25" t="s">
-        <v>315</v>
+        <v>310</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A3" s="39"/>
       <c r="B3" s="25" t="s">
-        <v>310</v>
+        <v>305</v>
       </c>
       <c r="C3" s="25" t="s">
-        <v>313</v>
+        <v>308</v>
       </c>
       <c r="D3" s="25" t="s">
-        <v>316</v>
+        <v>311</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" s="39"/>
       <c r="B4" s="25" t="s">
-        <v>311</v>
+        <v>306</v>
       </c>
       <c r="C4" s="25" t="s">
-        <v>314</v>
+        <v>309</v>
       </c>
       <c r="D4" s="25" t="s">
-        <v>317</v>
+        <v>312</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.35">
@@ -4084,7 +4175,7 @@
         <v>1</v>
       </c>
       <c r="B5" s="25" t="s">
-        <v>318</v>
+        <v>313</v>
       </c>
       <c r="C5" s="25" t="s">
         <v>48</v>
@@ -4096,7 +4187,7 @@
         <v>2</v>
       </c>
       <c r="B6" s="25" t="s">
-        <v>319</v>
+        <v>314</v>
       </c>
       <c r="C6" s="25" t="s">
         <v>49</v>
@@ -4120,10 +4211,10 @@
         <v>4</v>
       </c>
       <c r="B8" s="25" t="s">
-        <v>320</v>
+        <v>315</v>
       </c>
       <c r="C8" s="25" t="s">
-        <v>321</v>
+        <v>316</v>
       </c>
       <c r="D8" s="25"/>
     </row>
@@ -4132,7 +4223,7 @@
         <v>5</v>
       </c>
       <c r="B9" s="25" t="s">
-        <v>322</v>
+        <v>317</v>
       </c>
       <c r="C9" s="25" t="s">
         <v>52</v>
@@ -4156,10 +4247,10 @@
         <v>7</v>
       </c>
       <c r="B11" s="25" t="s">
-        <v>323</v>
+        <v>318</v>
       </c>
       <c r="C11" s="25" t="s">
-        <v>324</v>
+        <v>319</v>
       </c>
       <c r="D11" s="25"/>
     </row>
@@ -4172,157 +4263,6 @@
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A45619C8-AAF7-43DE-831A-2BED068D71D3}">
-  <dimension ref="A1:K11"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="10.26953125" style="7" customWidth="1"/>
-    <col min="2" max="2" width="21.453125" style="7" customWidth="1"/>
-    <col min="3" max="3" width="28.7265625" style="7" customWidth="1"/>
-    <col min="4" max="4" width="28.54296875" style="7" customWidth="1"/>
-    <col min="5" max="5" width="25.26953125" style="7" customWidth="1"/>
-    <col min="6" max="6" width="21.54296875" style="7" customWidth="1"/>
-    <col min="7" max="7" width="12.26953125" style="7" customWidth="1"/>
-    <col min="8" max="8" width="19.1796875" style="7" customWidth="1"/>
-    <col min="9" max="11" width="23.26953125" style="7" customWidth="1"/>
-    <col min="12" max="16384" width="8.81640625" style="7"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A1" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="8" t="s">
-        <v>55</v>
-      </c>
-      <c r="C1" s="8" t="s">
-        <v>210</v>
-      </c>
-      <c r="D1" s="8" t="s">
-        <v>211</v>
-      </c>
-      <c r="E1" s="8" t="s">
-        <v>212</v>
-      </c>
-      <c r="F1" s="8" t="s">
-        <v>213</v>
-      </c>
-      <c r="G1" s="8" t="s">
-        <v>214</v>
-      </c>
-      <c r="H1" s="8" t="s">
-        <v>215</v>
-      </c>
-      <c r="I1" s="8" t="s">
-        <v>216</v>
-      </c>
-      <c r="J1" s="8" t="s">
-        <v>217</v>
-      </c>
-      <c r="K1" s="8" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" ht="85.9" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2" s="10" t="s">
-        <v>219</v>
-      </c>
-      <c r="C2" s="7" t="s">
-        <v>220</v>
-      </c>
-      <c r="D2" s="7" t="s">
-        <v>221</v>
-      </c>
-      <c r="E2" s="7" t="s">
-        <v>222</v>
-      </c>
-      <c r="F2" s="7" t="s">
-        <v>223</v>
-      </c>
-      <c r="G2" s="7" t="s">
-        <v>224</v>
-      </c>
-      <c r="H2" s="7" t="s">
-        <v>225</v>
-      </c>
-      <c r="I2" s="7" t="s">
-        <v>226</v>
-      </c>
-      <c r="J2" s="7" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A3" s="25">
-        <v>1</v>
-      </c>
-      <c r="B3" s="25" t="s">
-        <v>446</v>
-      </c>
-      <c r="C3" s="27" t="s">
-        <v>377</v>
-      </c>
-      <c r="D3" s="25">
-        <v>1</v>
-      </c>
-      <c r="E3" s="25" t="s">
-        <v>447</v>
-      </c>
-      <c r="F3" s="25" t="s">
-        <v>228</v>
-      </c>
-      <c r="G3" s="25"/>
-      <c r="H3" s="25">
-        <v>903331332</v>
-      </c>
-      <c r="I3" s="34" t="s">
-        <v>448</v>
-      </c>
-      <c r="J3" s="25"/>
-      <c r="K3" s="25"/>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="I4" s="12"/>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="I5" s="12"/>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="I6" s="12"/>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="I7" s="12"/>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="I8" s="12"/>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="I9" s="12"/>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="I10" s="12"/>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="I11" s="12"/>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="6" type="noConversion"/>
-  <hyperlinks>
-    <hyperlink ref="I3" r:id="rId1" display="mailto:nva@example.com" xr:uid="{F6D89C5D-FF1D-47B0-919B-E0B60A9F5428}"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E863D4F3-258D-41FD-90A7-5BEE0F94C0B4}">
   <dimension ref="A1:F2"/>
   <sheetViews>
@@ -4352,10 +4292,10 @@
         <v>3</v>
       </c>
       <c r="D1" s="8" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="E1" s="8" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="F1" s="8" t="s">
         <v>80</v>
@@ -4369,13 +4309,13 @@
         <v>119</v>
       </c>
       <c r="C2" s="7" t="s">
+        <v>205</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>206</v>
+      </c>
+      <c r="E2" s="7" t="s">
         <v>207</v>
-      </c>
-      <c r="D2" s="7" t="s">
-        <v>208</v>
-      </c>
-      <c r="E2" s="7" t="s">
-        <v>209</v>
       </c>
     </row>
   </sheetData>
@@ -4388,12 +4328,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35B69A6E-98BC-434D-A419-FDB6C97F2A28}">
-  <dimension ref="A1:E47"/>
+  <dimension ref="A1:E46"/>
   <sheetViews>
-    <sheetView topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="H21" sqref="H21"/>
+    <sheetView topLeftCell="A29" workbookViewId="0">
+      <selection activeCell="D43" sqref="D43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4408,17 +4348,17 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="4" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="6" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="6" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
@@ -4444,7 +4384,7 @@
     </row>
     <row r="11" spans="1:5" ht="34.9" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="40" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="B11" s="41"/>
       <c r="C11" s="41"/>
@@ -4465,7 +4405,7 @@
     </row>
     <row r="16" spans="1:5" ht="28.9" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="42" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="B16" s="43"/>
       <c r="C16" s="43"/>
@@ -4474,7 +4414,7 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17" s="3" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="B17" s="45" t="s">
         <v>80</v>
@@ -4482,15 +4422,15 @@
       <c r="C17" s="45"/>
       <c r="D17" s="45"/>
       <c r="E17" s="3" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="B18" s="46" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="C18" s="46"/>
       <c r="D18" s="46"/>
@@ -4498,10 +4438,10 @@
     </row>
     <row r="19" spans="1:5" ht="29.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="1" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="B19" s="47" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="C19" s="47"/>
       <c r="D19" s="47"/>
@@ -4512,7 +4452,7 @@
         <v>0</v>
       </c>
       <c r="B20" s="47" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="C20" s="47"/>
       <c r="D20" s="47"/>
@@ -4539,7 +4479,7 @@
     </row>
     <row r="26" spans="1:5" ht="28.9" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A26" s="44" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="B26" s="44"/>
       <c r="C26" s="44"/>
@@ -4548,290 +4488,277 @@
     </row>
     <row r="27" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A27" s="20" t="s">
+        <v>244</v>
+      </c>
+      <c r="B27" s="20" t="s">
+        <v>245</v>
+      </c>
+      <c r="C27" s="20" t="s">
         <v>246</v>
       </c>
-      <c r="B27" s="20" t="s">
+      <c r="D27" s="21" t="s">
         <v>247</v>
       </c>
-      <c r="C27" s="20" t="s">
-        <v>248</v>
-      </c>
-      <c r="D27" s="21" t="s">
-        <v>249</v>
-      </c>
       <c r="E27" s="21" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
     </row>
     <row r="28" spans="1:5" ht="87" x14ac:dyDescent="0.35">
       <c r="A28" s="22" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="B28" s="22" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="C28" s="17" t="s">
         <v>58</v>
       </c>
       <c r="D28" s="19" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="E28" s="18" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
     </row>
     <row r="29" spans="1:5" ht="55.9" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A29" s="22" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="B29" s="22" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="C29" s="17" t="s">
         <v>62</v>
       </c>
       <c r="D29" s="19" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="E29" s="18"/>
     </row>
     <row r="30" spans="1:5" ht="62.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A30" s="22" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="B30" s="22" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="C30" s="17" t="s">
         <v>54</v>
       </c>
       <c r="D30" s="18" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="E30" s="18"/>
     </row>
     <row r="31" spans="1:5" ht="42.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A31" s="22" t="s">
+        <v>258</v>
+      </c>
+      <c r="B31" s="22" t="s">
+        <v>259</v>
+      </c>
+      <c r="C31" s="17" t="s">
         <v>260</v>
       </c>
-      <c r="B31" s="22" t="s">
+      <c r="D31" s="19" t="s">
         <v>261</v>
-      </c>
-      <c r="C31" s="17" t="s">
-        <v>262</v>
-      </c>
-      <c r="D31" s="19" t="s">
-        <v>263</v>
       </c>
       <c r="E31" s="18"/>
     </row>
     <row r="32" spans="1:5" ht="36" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A32" s="22" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="B32" s="22" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="C32" s="17" t="s">
         <v>76</v>
       </c>
       <c r="D32" s="19" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="E32" s="18"/>
     </row>
     <row r="33" spans="1:5" ht="36.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A33" s="23" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="B33" s="23" t="s">
-        <v>295</v>
+        <v>291</v>
       </c>
       <c r="C33" s="17" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
       <c r="D33" s="18"/>
       <c r="E33" s="18"/>
     </row>
     <row r="34" spans="1:5" ht="38.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A34" s="23" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="B34" s="23" t="s">
-        <v>296</v>
+        <v>292</v>
       </c>
       <c r="C34" s="17" t="s">
-        <v>307</v>
+        <v>302</v>
       </c>
       <c r="D34" s="18"/>
       <c r="E34" s="18"/>
     </row>
     <row r="35" spans="1:5" ht="39.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A35" s="22" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="B35" s="22" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
       <c r="C35" s="17" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="D35" s="18"/>
       <c r="E35" s="18"/>
     </row>
     <row r="36" spans="1:5" ht="32.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A36" s="22" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="B36" s="22" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
       <c r="C36" s="17" t="s">
-        <v>308</v>
+        <v>303</v>
       </c>
       <c r="D36" s="18"/>
       <c r="E36" s="18"/>
     </row>
     <row r="37" spans="1:5" ht="42.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A37" s="22" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="B37" s="22" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
       <c r="C37" s="17" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="D37" s="18"/>
       <c r="E37" s="18"/>
     </row>
     <row r="38" spans="1:5" ht="42.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A38" s="22" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="B38" s="22" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
       <c r="C38" s="17" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="D38" s="18"/>
       <c r="E38" s="18"/>
     </row>
     <row r="39" spans="1:5" ht="42.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A39" s="22" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="B39" s="22" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="C39" s="17" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="D39" s="18"/>
       <c r="E39" s="18"/>
     </row>
     <row r="40" spans="1:5" ht="42.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A40" s="22" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="B40" s="22" t="s">
-        <v>301</v>
+        <v>297</v>
       </c>
       <c r="C40" s="17" t="s">
-        <v>293</v>
+        <v>289</v>
       </c>
       <c r="D40" s="18"/>
       <c r="E40" s="18"/>
     </row>
     <row r="41" spans="1:5" ht="42.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A41" s="22" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="B41" s="22" t="s">
-        <v>302</v>
+        <v>298</v>
       </c>
       <c r="C41" s="17" t="s">
-        <v>294</v>
+        <v>290</v>
       </c>
       <c r="D41" s="18"/>
       <c r="E41" s="18"/>
     </row>
     <row r="42" spans="1:5" ht="42.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A42" s="23" t="s">
-        <v>279</v>
-      </c>
-      <c r="B42" s="23" t="s">
-        <v>303</v>
+      <c r="A42" s="22" t="s">
+        <v>277</v>
+      </c>
+      <c r="B42" s="22" t="s">
+        <v>299</v>
       </c>
       <c r="C42" s="17" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="D42" s="18"/>
       <c r="E42" s="18"/>
     </row>
     <row r="43" spans="1:5" ht="42.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A43" s="22" t="s">
-        <v>280</v>
-      </c>
-      <c r="B43" s="22" t="s">
-        <v>304</v>
+      <c r="A43" s="23" t="s">
+        <v>281</v>
+      </c>
+      <c r="B43" s="23" t="s">
+        <v>282</v>
       </c>
       <c r="C43" s="17" t="s">
-        <v>292</v>
+        <v>283</v>
       </c>
       <c r="D43" s="18"/>
       <c r="E43" s="18"/>
     </row>
     <row r="44" spans="1:5" ht="42.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A44" s="23" t="s">
-        <v>284</v>
-      </c>
-      <c r="B44" s="23" t="s">
-        <v>285</v>
+      <c r="A44" s="22" t="s">
+        <v>280</v>
+      </c>
+      <c r="B44" s="22" t="s">
+        <v>300</v>
       </c>
       <c r="C44" s="17" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="D44" s="18"/>
       <c r="E44" s="18"/>
     </row>
     <row r="45" spans="1:5" ht="42.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A45" s="22" t="s">
-        <v>283</v>
+        <v>272</v>
       </c>
       <c r="B45" s="22" t="s">
-        <v>305</v>
+        <v>273</v>
       </c>
       <c r="C45" s="17" t="s">
-        <v>290</v>
+        <v>138</v>
       </c>
       <c r="D45" s="18"/>
       <c r="E45" s="18"/>
     </row>
     <row r="46" spans="1:5" ht="42.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A46" s="22" t="s">
-        <v>274</v>
-      </c>
-      <c r="B46" s="22" t="s">
-        <v>275</v>
-      </c>
-      <c r="C46" s="17" t="s">
-        <v>138</v>
-      </c>
-      <c r="D46" s="18"/>
-      <c r="E46" s="18"/>
-    </row>
-    <row r="47" spans="1:5" ht="42.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A47" s="1" t="s">
-        <v>273</v>
-      </c>
-      <c r="B47" s="1" t="s">
-        <v>306</v>
-      </c>
-      <c r="C47" s="1"/>
-      <c r="D47" s="2"/>
-      <c r="E47" s="2"/>
+      <c r="A46" s="1" t="s">
+        <v>271</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>301</v>
+      </c>
+      <c r="C46" s="1"/>
+      <c r="D46" s="2"/>
+      <c r="E46" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="8">
@@ -4916,114 +4843,114 @@
         <v>7</v>
       </c>
       <c r="B2" s="25" t="s">
-        <v>309</v>
+        <v>304</v>
       </c>
       <c r="C2" s="25" t="s">
-        <v>312</v>
+        <v>307</v>
       </c>
       <c r="D2" s="25" t="s">
-        <v>312</v>
+        <v>307</v>
       </c>
       <c r="E2" s="25" t="s">
-        <v>312</v>
+        <v>307</v>
       </c>
       <c r="F2" s="25" t="s">
-        <v>312</v>
+        <v>307</v>
       </c>
       <c r="G2" s="25" t="s">
+        <v>336</v>
+      </c>
+      <c r="H2" s="25" t="s">
+        <v>339</v>
+      </c>
+      <c r="I2" s="25" t="s">
+        <v>339</v>
+      </c>
+      <c r="J2" s="25" t="s">
         <v>341</v>
       </c>
-      <c r="H2" s="25" t="s">
+      <c r="K2" s="25" t="s">
         <v>344</v>
-      </c>
-      <c r="I2" s="25" t="s">
-        <v>344</v>
-      </c>
-      <c r="J2" s="25" t="s">
-        <v>346</v>
-      </c>
-      <c r="K2" s="25" t="s">
-        <v>349</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A3" s="39"/>
       <c r="B3" s="25" t="s">
-        <v>325</v>
+        <v>320</v>
       </c>
       <c r="C3" s="25" t="s">
+        <v>324</v>
+      </c>
+      <c r="D3" s="25" t="s">
+        <v>324</v>
+      </c>
+      <c r="E3" s="25" t="s">
         <v>329</v>
       </c>
-      <c r="D3" s="25" t="s">
-        <v>329</v>
-      </c>
-      <c r="E3" s="25" t="s">
-        <v>334</v>
-      </c>
       <c r="F3" s="25" t="s">
+        <v>332</v>
+      </c>
+      <c r="G3" s="25" t="s">
         <v>337</v>
       </c>
-      <c r="G3" s="25" t="s">
+      <c r="H3" s="25" t="s">
+        <v>340</v>
+      </c>
+      <c r="I3" s="25" t="s">
+        <v>340</v>
+      </c>
+      <c r="J3" s="25" t="s">
         <v>342</v>
       </c>
-      <c r="H3" s="25" t="s">
+      <c r="K3" s="25" t="s">
         <v>345</v>
-      </c>
-      <c r="I3" s="25" t="s">
-        <v>345</v>
-      </c>
-      <c r="J3" s="25" t="s">
-        <v>347</v>
-      </c>
-      <c r="K3" s="25" t="s">
-        <v>350</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A4" s="39"/>
       <c r="B4" s="25" t="s">
-        <v>326</v>
+        <v>321</v>
       </c>
       <c r="C4" s="25" t="s">
+        <v>325</v>
+      </c>
+      <c r="D4" s="25" t="s">
+        <v>327</v>
+      </c>
+      <c r="E4" s="25" t="s">
         <v>330</v>
       </c>
-      <c r="D4" s="25" t="s">
-        <v>332</v>
-      </c>
-      <c r="E4" s="25" t="s">
-        <v>335</v>
-      </c>
       <c r="F4" s="25" t="s">
+        <v>333</v>
+      </c>
+      <c r="G4" s="25" t="s">
         <v>338</v>
-      </c>
-      <c r="G4" s="25" t="s">
-        <v>343</v>
       </c>
       <c r="H4" s="25"/>
       <c r="I4" s="25"/>
       <c r="J4" s="25" t="s">
-        <v>348</v>
+        <v>343</v>
       </c>
       <c r="K4" s="25" t="s">
-        <v>351</v>
+        <v>346</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A5" s="39"/>
       <c r="B5" s="25" t="s">
-        <v>327</v>
+        <v>322</v>
       </c>
       <c r="C5" s="25" t="s">
+        <v>326</v>
+      </c>
+      <c r="D5" s="25" t="s">
+        <v>328</v>
+      </c>
+      <c r="E5" s="25" t="s">
         <v>331</v>
       </c>
-      <c r="D5" s="25" t="s">
-        <v>333</v>
-      </c>
-      <c r="E5" s="25" t="s">
-        <v>336</v>
-      </c>
       <c r="F5" s="25" t="s">
-        <v>339</v>
+        <v>334</v>
       </c>
       <c r="G5" s="25"/>
       <c r="H5" s="25"/>
@@ -5034,13 +4961,13 @@
     <row r="6" spans="1:11" ht="32.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="39"/>
       <c r="B6" s="25" t="s">
-        <v>328</v>
+        <v>323</v>
       </c>
       <c r="C6" s="25"/>
       <c r="D6" s="25"/>
       <c r="E6" s="25"/>
       <c r="F6" s="25" t="s">
-        <v>340</v>
+        <v>335</v>
       </c>
       <c r="G6" s="25"/>
       <c r="H6" s="25"/>
@@ -5053,28 +4980,28 @@
         <v>1</v>
       </c>
       <c r="B7" s="27" t="s">
-        <v>352</v>
+        <v>347</v>
       </c>
       <c r="C7" s="25" t="s">
-        <v>353</v>
+        <v>348</v>
       </c>
       <c r="D7" s="25" t="s">
-        <v>354</v>
+        <v>349</v>
       </c>
       <c r="E7" s="35" t="s">
-        <v>355</v>
+        <v>350</v>
       </c>
       <c r="F7" s="25">
         <v>901123121</v>
       </c>
       <c r="G7" s="36" t="s">
-        <v>356</v>
+        <v>351</v>
       </c>
       <c r="H7" s="27" t="s">
-        <v>357</v>
+        <v>352</v>
       </c>
       <c r="I7" s="27" t="s">
-        <v>358</v>
+        <v>353</v>
       </c>
       <c r="J7" s="27"/>
       <c r="K7" s="27"/>
@@ -5084,28 +5011,28 @@
         <v>2</v>
       </c>
       <c r="B8" s="27" t="s">
-        <v>359</v>
+        <v>354</v>
       </c>
       <c r="C8" s="25" t="s">
-        <v>360</v>
+        <v>355</v>
       </c>
       <c r="D8" s="25" t="s">
-        <v>361</v>
+        <v>356</v>
       </c>
       <c r="E8" s="35" t="s">
-        <v>362</v>
+        <v>357</v>
       </c>
       <c r="F8" s="25">
         <v>901123122</v>
       </c>
       <c r="G8" s="36" t="s">
-        <v>363</v>
+        <v>358</v>
       </c>
       <c r="H8" s="27" t="s">
-        <v>357</v>
+        <v>352</v>
       </c>
       <c r="I8" s="27" t="s">
-        <v>364</v>
+        <v>359</v>
       </c>
       <c r="J8" s="27"/>
       <c r="K8" s="27"/>
@@ -5115,28 +5042,28 @@
         <v>3</v>
       </c>
       <c r="B9" s="27" t="s">
-        <v>365</v>
+        <v>360</v>
       </c>
       <c r="C9" s="25" t="s">
-        <v>366</v>
+        <v>361</v>
       </c>
       <c r="D9" s="25" t="s">
-        <v>367</v>
+        <v>362</v>
       </c>
       <c r="E9" s="35" t="s">
-        <v>368</v>
+        <v>363</v>
       </c>
       <c r="F9" s="25">
         <v>901123123</v>
       </c>
       <c r="G9" s="36" t="s">
-        <v>369</v>
+        <v>364</v>
       </c>
       <c r="H9" s="27" t="s">
-        <v>357</v>
+        <v>352</v>
       </c>
       <c r="I9" s="27" t="s">
-        <v>370</v>
+        <v>365</v>
       </c>
       <c r="J9" s="27"/>
       <c r="K9" s="27"/>
@@ -5146,28 +5073,28 @@
         <v>4</v>
       </c>
       <c r="B10" s="27" t="s">
-        <v>371</v>
+        <v>366</v>
       </c>
       <c r="C10" s="25" t="s">
-        <v>372</v>
+        <v>367</v>
       </c>
       <c r="D10" s="25" t="s">
-        <v>373</v>
+        <v>368</v>
       </c>
       <c r="E10" s="35" t="s">
-        <v>374</v>
+        <v>369</v>
       </c>
       <c r="F10" s="25">
         <v>901123124</v>
       </c>
       <c r="G10" s="36" t="s">
-        <v>375</v>
+        <v>370</v>
       </c>
       <c r="H10" s="27" t="s">
-        <v>357</v>
+        <v>352</v>
       </c>
       <c r="I10" s="27" t="s">
-        <v>376</v>
+        <v>371</v>
       </c>
       <c r="J10" s="27"/>
       <c r="K10" s="27"/>
@@ -5486,84 +5413,84 @@
         <v>7</v>
       </c>
       <c r="B2" s="25" t="s">
-        <v>309</v>
+        <v>304</v>
       </c>
       <c r="C2" s="25" t="s">
-        <v>312</v>
+        <v>307</v>
       </c>
       <c r="D2" s="25" t="s">
-        <v>312</v>
+        <v>307</v>
       </c>
       <c r="E2" s="25" t="s">
-        <v>385</v>
+        <v>380</v>
       </c>
       <c r="F2" s="38" t="s">
         <v>85</v>
       </c>
       <c r="G2" s="25" t="s">
-        <v>315</v>
+        <v>310</v>
       </c>
       <c r="H2" s="25" t="s">
-        <v>388</v>
+        <v>383</v>
       </c>
       <c r="I2" s="25" t="s">
-        <v>389</v>
+        <v>384</v>
       </c>
       <c r="J2" s="25" t="s">
-        <v>388</v>
+        <v>383</v>
       </c>
       <c r="K2" s="25" t="s">
-        <v>391</v>
+        <v>386</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="87" x14ac:dyDescent="0.35">
       <c r="A3" s="39"/>
       <c r="B3" s="25" t="s">
+        <v>373</v>
+      </c>
+      <c r="C3" s="25" t="s">
+        <v>376</v>
+      </c>
+      <c r="D3" s="25" t="s">
         <v>378</v>
       </c>
-      <c r="C3" s="25" t="s">
+      <c r="E3" s="25" t="s">
         <v>381</v>
-      </c>
-      <c r="D3" s="25" t="s">
-        <v>383</v>
-      </c>
-      <c r="E3" s="25" t="s">
-        <v>386</v>
       </c>
       <c r="F3" s="39"/>
       <c r="G3" s="25" t="s">
-        <v>316</v>
+        <v>311</v>
       </c>
       <c r="H3" s="25" t="s">
-        <v>328</v>
+        <v>323</v>
       </c>
       <c r="I3" s="25" t="s">
-        <v>390</v>
+        <v>385</v>
       </c>
       <c r="J3" s="25" t="s">
-        <v>328</v>
+        <v>323</v>
       </c>
       <c r="K3" s="25" t="s">
-        <v>392</v>
+        <v>387</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A4" s="39"/>
       <c r="B4" s="25" t="s">
+        <v>374</v>
+      </c>
+      <c r="C4" s="25" t="s">
+        <v>377</v>
+      </c>
+      <c r="D4" s="25" t="s">
         <v>379</v>
       </c>
-      <c r="C4" s="25" t="s">
-        <v>382</v>
-      </c>
-      <c r="D4" s="25" t="s">
-        <v>384</v>
-      </c>
       <c r="E4" s="25" t="s">
-        <v>348</v>
+        <v>343</v>
       </c>
       <c r="F4" s="39"/>
       <c r="G4" s="25" t="s">
-        <v>387</v>
+        <v>382</v>
       </c>
       <c r="H4" s="25"/>
       <c r="I4" s="25"/>
@@ -5573,14 +5500,14 @@
     <row r="5" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A5" s="39"/>
       <c r="B5" s="25" t="s">
-        <v>380</v>
+        <v>375</v>
       </c>
       <c r="C5" s="25"/>
       <c r="D5" s="25"/>
       <c r="E5" s="25"/>
       <c r="F5" s="39"/>
       <c r="G5" s="25" t="s">
-        <v>317</v>
+        <v>312</v>
       </c>
       <c r="H5" s="25"/>
       <c r="I5" s="25"/>
@@ -5628,11 +5555,11 @@
       </c>
       <c r="F7" s="25"/>
       <c r="G7" s="27" t="s">
-        <v>352</v>
+        <v>347</v>
       </c>
       <c r="H7" s="25"/>
       <c r="I7" s="25" t="s">
-        <v>393</v>
+        <v>388</v>
       </c>
       <c r="J7" s="25"/>
       <c r="K7" s="25"/>
@@ -5655,7 +5582,7 @@
       </c>
       <c r="F8" s="25"/>
       <c r="G8" s="25" t="s">
-        <v>394</v>
+        <v>389</v>
       </c>
       <c r="H8" s="25"/>
       <c r="I8" s="25" t="s">
@@ -5682,7 +5609,7 @@
       </c>
       <c r="F9" s="25"/>
       <c r="G9" s="25" t="s">
-        <v>395</v>
+        <v>390</v>
       </c>
       <c r="H9" s="25"/>
       <c r="I9" s="25" t="s">
@@ -5843,7 +5770,7 @@
         <v>106</v>
       </c>
       <c r="D2" s="29" t="s">
-        <v>396</v>
+        <v>391</v>
       </c>
       <c r="E2" s="29" t="s">
         <v>107</v>
@@ -5857,10 +5784,10 @@
         <v>1</v>
       </c>
       <c r="B3" s="26" t="s">
-        <v>397</v>
+        <v>392</v>
       </c>
       <c r="C3" s="26" t="s">
-        <v>397</v>
+        <v>392</v>
       </c>
       <c r="D3" s="26">
         <v>1</v>
@@ -5877,10 +5804,10 @@
         <v>2</v>
       </c>
       <c r="B4" s="26" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C4" s="26" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="D4" s="26">
         <v>1</v>
@@ -5897,10 +5824,10 @@
         <v>3</v>
       </c>
       <c r="B5" s="26" t="s">
-        <v>398</v>
+        <v>393</v>
       </c>
       <c r="C5" s="26" t="s">
-        <v>398</v>
+        <v>393</v>
       </c>
       <c r="D5" s="26">
         <v>1</v>
@@ -5917,10 +5844,10 @@
         <v>4</v>
       </c>
       <c r="B6" s="26" t="s">
-        <v>399</v>
+        <v>394</v>
       </c>
       <c r="C6" s="26" t="s">
-        <v>399</v>
+        <v>394</v>
       </c>
       <c r="D6" s="26">
         <v>1</v>
@@ -5984,7 +5911,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="25" t="s">
-        <v>400</v>
+        <v>395</v>
       </c>
       <c r="C3" s="25" t="s">
         <v>111</v>
@@ -5996,7 +5923,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="25" t="s">
-        <v>401</v>
+        <v>396</v>
       </c>
       <c r="C4" s="25" t="s">
         <v>113</v>
@@ -6008,7 +5935,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="25" t="s">
-        <v>402</v>
+        <v>397</v>
       </c>
       <c r="C5" s="25" t="s">
         <v>114</v>
@@ -6020,7 +5947,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="25" t="s">
-        <v>403</v>
+        <v>398</v>
       </c>
       <c r="C6" s="25" t="s">
         <v>115</v>
@@ -6032,7 +5959,7 @@
         <v>5</v>
       </c>
       <c r="B7" s="25" t="s">
-        <v>404</v>
+        <v>399</v>
       </c>
       <c r="C7" s="25" t="s">
         <v>116</v>

</xml_diff>

<commit_message>
[hotfix/master-viet] update file template import (not allowing import account type)
</commit_message>
<xml_diff>
--- a/apps/core/fimport/static/fimport/template/mega-import.xlsx
+++ b/apps/core/fimport/static/fimport/template/mega-import.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PCAdmin\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0327FB89-AC43-4547-B79A-497DE098AF23}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4DD40C6-4954-4C8A-A567-41203BFC281F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="803" firstSheet="10" activeTab="10" xr2:uid="{ABCF866D-F0C2-489F-81F3-6B45D3E3629E}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="803" firstSheet="13" activeTab="19" xr2:uid="{ABCF866D-F0C2-489F-81F3-6B45D3E3629E}"/>
   </bookViews>
   <sheets>
     <sheet name="#account.users" sheetId="1" r:id="rId1"/>
@@ -22,18 +22,17 @@
     <sheet name="#saledata.price.taxcategory" sheetId="19" r:id="rId7"/>
     <sheet name="#saledata.price.tax" sheetId="21" r:id="rId8"/>
     <sheet name="#saledata.account.group" sheetId="11" r:id="rId9"/>
-    <sheet name="#saledata.account.type" sheetId="12" r:id="rId10"/>
-    <sheet name="#saledata.industry" sheetId="13" r:id="rId11"/>
-    <sheet name="#saledata.account" sheetId="15" r:id="rId12"/>
-    <sheet name="#saledata.product.uomgroup" sheetId="16" r:id="rId13"/>
-    <sheet name="#saledata.product.uom" sheetId="20" r:id="rId14"/>
-    <sheet name="#saledata.product.prodcategory" sheetId="18" r:id="rId15"/>
-    <sheet name="#saledata.product.manufacturer" sheetId="23" r:id="rId16"/>
-    <sheet name="#saledata.product" sheetId="22" r:id="rId17"/>
-    <sheet name="#saledata.salutation" sheetId="8" r:id="rId18"/>
-    <sheet name="#saledata.contact" sheetId="9" r:id="rId19"/>
-    <sheet name="#saledata.payment-term" sheetId="14" r:id="rId20"/>
-    <sheet name="Guidelines - Chỉ dẫn" sheetId="6" r:id="rId21"/>
+    <sheet name="#saledata.industry" sheetId="13" r:id="rId10"/>
+    <sheet name="#saledata.account" sheetId="15" r:id="rId11"/>
+    <sheet name="#saledata.product.uomgroup" sheetId="16" r:id="rId12"/>
+    <sheet name="#saledata.product.uom" sheetId="20" r:id="rId13"/>
+    <sheet name="#saledata.product.prodcategory" sheetId="18" r:id="rId14"/>
+    <sheet name="#saledata.product.manufacturer" sheetId="23" r:id="rId15"/>
+    <sheet name="#saledata.product" sheetId="22" r:id="rId16"/>
+    <sheet name="#saledata.salutation" sheetId="8" r:id="rId17"/>
+    <sheet name="#saledata.contact" sheetId="9" r:id="rId18"/>
+    <sheet name="#saledata.payment-term" sheetId="14" r:id="rId19"/>
+    <sheet name="Guidelines - Chỉ dẫn" sheetId="6" r:id="rId20"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -56,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="646" uniqueCount="455">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="630" uniqueCount="444">
   <si>
     <t>STT</t>
   </si>
@@ -446,15 +445,6 @@
   <si>
     <t>- Bắt buộc, định danh
 - Độ dài tối đa: 100
-- Ví dụ: AT001</t>
-  </si>
-  <si>
-    <t>- Tên của loại tài khoản
-- Ví dụ: Khách hàng</t>
-  </si>
-  <si>
-    <t>- Bắt buộc, định danh
-- Độ dài tối đa: 100
 - Ví dụ: 001</t>
   </si>
   <si>
@@ -526,12 +516,6 @@
 - Độ dài tối đa: 150
 - Tên của tài khoản
 - Ví dụ: Công Ty TNHH Minh Tâm Solution</t>
-  </si>
-  <si>
-    <t>- Bắt buộc
-- Danh sách mã liên kết với nhau bằng dấu phẩy.
-- Mã loại tài khoản tại #saledata.account.type
-- Ví dụ: AT001</t>
   </si>
   <si>
     <t>- Bắt buộc
@@ -1188,12 +1172,6 @@
     <t>Account</t>
   </si>
   <si>
-    <t>#saledata.account.type</t>
-  </si>
-  <si>
-    <t>Loại tài khoản</t>
-  </si>
-  <si>
     <t>#saledata.industry</t>
   </si>
   <si>
@@ -1270,9 +1248,6 @@
   </si>
   <si>
     <t>Account Group</t>
-  </si>
-  <si>
-    <t>Account Type</t>
   </si>
   <si>
     <t>Industry</t>
@@ -1590,24 +1565,6 @@
     <t>Type005</t>
   </si>
   <si>
-    <t>AT005</t>
-  </si>
-  <si>
-    <t>Đại lý cấp 1</t>
-  </si>
-  <si>
-    <t>AT006</t>
-  </si>
-  <si>
-    <t>Đại lý cấp 2</t>
-  </si>
-  <si>
-    <t>AT007</t>
-  </si>
-  <si>
-    <t>Nhà đầu tư</t>
-  </si>
-  <si>
     <t>IND001</t>
   </si>
   <si>
@@ -1764,6 +1721,12 @@
     <t>- Bắt buộc
 - Mã loại sản phẩm tại tính năng master data config/ item/ product types
 - Ví dụ: finished_goods</t>
+  </si>
+  <si>
+    <t>- Bắt buộc
+- Danh sách mã liên kết với nhau bằng dấu phẩy.
+- Mã loại tài khoản tại chức năng Master Data Config / Account/ Account Types
+- Ví dụ: AT001</t>
   </si>
 </sst>
 </file>
@@ -2654,93 +2617,10 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1359912D-CDDC-4C74-BCFB-CBE40EB489F2}">
-  <dimension ref="A1:D5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="8.81640625" style="7"/>
-    <col min="2" max="2" width="27" style="7" customWidth="1"/>
-    <col min="3" max="3" width="37.453125" style="7" customWidth="1"/>
-    <col min="4" max="4" width="42.7265625" style="7" customWidth="1"/>
-    <col min="5" max="16384" width="8.81640625" style="7"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A1" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="8" t="s">
-        <v>55</v>
-      </c>
-      <c r="C1" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="D1" s="8" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" ht="56.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2" s="7" t="s">
-        <v>117</v>
-      </c>
-      <c r="C2" s="7" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A3" s="25">
-        <v>1</v>
-      </c>
-      <c r="B3" s="25" t="s">
-        <v>400</v>
-      </c>
-      <c r="C3" s="25" t="s">
-        <v>401</v>
-      </c>
-      <c r="D3" s="25"/>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A4" s="25">
-        <v>2</v>
-      </c>
-      <c r="B4" s="25" t="s">
-        <v>402</v>
-      </c>
-      <c r="C4" s="25" t="s">
-        <v>403</v>
-      </c>
-      <c r="D4" s="25"/>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A5" s="25">
-        <v>3</v>
-      </c>
-      <c r="B5" s="25" t="s">
-        <v>404</v>
-      </c>
-      <c r="C5" s="25" t="s">
-        <v>405</v>
-      </c>
-      <c r="D5" s="25"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ACBC7503-D39D-4D5C-B33A-E4C15DD2E38F}">
   <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
@@ -2772,10 +2652,10 @@
         <v>7</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
@@ -2783,10 +2663,10 @@
         <v>1</v>
       </c>
       <c r="B3" s="25" t="s">
-        <v>406</v>
+        <v>394</v>
       </c>
       <c r="C3" s="25" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="D3" s="25"/>
     </row>
@@ -2795,10 +2675,10 @@
         <v>2</v>
       </c>
       <c r="B4" s="25" t="s">
-        <v>407</v>
+        <v>395</v>
       </c>
       <c r="C4" s="25" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="D4" s="25"/>
     </row>
@@ -2807,10 +2687,10 @@
         <v>3</v>
       </c>
       <c r="B5" s="25" t="s">
-        <v>408</v>
+        <v>396</v>
       </c>
       <c r="C5" s="25" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="D5" s="25"/>
     </row>
@@ -2819,10 +2699,10 @@
         <v>4</v>
       </c>
       <c r="B6" s="25" t="s">
-        <v>409</v>
+        <v>397</v>
       </c>
       <c r="C6" s="25" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="D6" s="25"/>
     </row>
@@ -2832,12 +2712,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{876A0AB4-CD70-4743-A933-50E4AFBD716C}">
   <dimension ref="A1:P5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="O5" sqref="O5"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -2861,46 +2741,46 @@
         <v>55</v>
       </c>
       <c r="C1" s="11" t="s">
+        <v>123</v>
+      </c>
+      <c r="D1" s="11" t="s">
+        <v>124</v>
+      </c>
+      <c r="E1" s="11" t="s">
         <v>125</v>
       </c>
-      <c r="D1" s="11" t="s">
+      <c r="F1" s="11" t="s">
         <v>126</v>
       </c>
-      <c r="E1" s="11" t="s">
+      <c r="G1" s="11" t="s">
         <v>127</v>
       </c>
-      <c r="F1" s="11" t="s">
+      <c r="H1" s="11" t="s">
         <v>128</v>
       </c>
-      <c r="G1" s="11" t="s">
+      <c r="I1" s="11" t="s">
         <v>129</v>
       </c>
-      <c r="H1" s="11" t="s">
+      <c r="J1" s="11" t="s">
         <v>130</v>
       </c>
-      <c r="I1" s="11" t="s">
+      <c r="K1" s="11" t="s">
         <v>131</v>
       </c>
-      <c r="J1" s="11" t="s">
+      <c r="L1" s="11" t="s">
         <v>132</v>
       </c>
-      <c r="K1" s="11" t="s">
+      <c r="M1" s="11" t="s">
         <v>133</v>
       </c>
-      <c r="L1" s="11" t="s">
+      <c r="N1" s="11" t="s">
         <v>134</v>
       </c>
-      <c r="M1" s="11" t="s">
+      <c r="O1" s="11" t="s">
         <v>135</v>
       </c>
-      <c r="N1" s="11" t="s">
+      <c r="P1" s="11" t="s">
         <v>136</v>
-      </c>
-      <c r="O1" s="11" t="s">
-        <v>137</v>
-      </c>
-      <c r="P1" s="11" t="s">
-        <v>138</v>
       </c>
     </row>
     <row r="2" spans="1:16" ht="147.65" customHeight="1" x14ac:dyDescent="0.35">
@@ -2908,49 +2788,49 @@
         <v>7</v>
       </c>
       <c r="B2" s="7" t="s">
+        <v>137</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>138</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>443</v>
+      </c>
+      <c r="E2" s="7" t="s">
         <v>139</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="F2" s="7" t="s">
         <v>140</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="G2" s="7" t="s">
         <v>141</v>
       </c>
-      <c r="E2" s="7" t="s">
+      <c r="H2" s="7" t="s">
         <v>142</v>
       </c>
-      <c r="F2" s="7" t="s">
+      <c r="I2" s="7" t="s">
         <v>143</v>
       </c>
-      <c r="G2" s="7" t="s">
+      <c r="J2" s="7" t="s">
         <v>144</v>
       </c>
-      <c r="H2" s="7" t="s">
+      <c r="K2" s="7" t="s">
         <v>145</v>
       </c>
-      <c r="I2" s="7" t="s">
+      <c r="L2" s="7" t="s">
         <v>146</v>
       </c>
-      <c r="J2" s="7" t="s">
+      <c r="M2" s="7" t="s">
         <v>147</v>
       </c>
-      <c r="K2" s="7" t="s">
+      <c r="N2" s="7" t="s">
         <v>148</v>
       </c>
-      <c r="L2" s="7" t="s">
+      <c r="O2" s="7" t="s">
         <v>149</v>
       </c>
-      <c r="M2" s="7" t="s">
+      <c r="P2" s="7" t="s">
         <v>150</v>
-      </c>
-      <c r="N2" s="7" t="s">
-        <v>151</v>
-      </c>
-      <c r="O2" s="7" t="s">
-        <v>152</v>
-      </c>
-      <c r="P2" s="7" t="s">
-        <v>153</v>
       </c>
     </row>
     <row r="3" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.35">
@@ -2958,25 +2838,25 @@
         <v>1</v>
       </c>
       <c r="B3" s="25" t="s">
-        <v>410</v>
+        <v>398</v>
       </c>
       <c r="C3" s="25" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="D3" s="25" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="E3" s="25">
         <v>1</v>
       </c>
       <c r="F3" s="25" t="s">
-        <v>395</v>
+        <v>389</v>
       </c>
       <c r="G3" s="25" t="s">
-        <v>406</v>
+        <v>394</v>
       </c>
       <c r="H3" s="27" t="s">
-        <v>347</v>
+        <v>341</v>
       </c>
       <c r="I3" s="25"/>
       <c r="J3" s="25"/>
@@ -2988,7 +2868,7 @@
       <c r="N3" s="25"/>
       <c r="O3" s="25"/>
       <c r="P3" s="25" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
     </row>
     <row r="4" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.35">
@@ -2996,25 +2876,25 @@
         <v>2</v>
       </c>
       <c r="B4" s="25" t="s">
-        <v>411</v>
+        <v>399</v>
       </c>
       <c r="C4" s="25" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="D4" s="25" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="E4" s="25">
         <v>1</v>
       </c>
       <c r="F4" s="25" t="s">
-        <v>396</v>
+        <v>390</v>
       </c>
       <c r="G4" s="25" t="s">
-        <v>407</v>
+        <v>395</v>
       </c>
       <c r="H4" s="27" t="s">
-        <v>354</v>
+        <v>348</v>
       </c>
       <c r="I4" s="25"/>
       <c r="J4" s="25"/>
@@ -3026,7 +2906,7 @@
       <c r="N4" s="25"/>
       <c r="O4" s="25"/>
       <c r="P4" s="25" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
     </row>
     <row r="5" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.35">
@@ -3034,25 +2914,25 @@
         <v>3</v>
       </c>
       <c r="B5" s="25" t="s">
-        <v>412</v>
+        <v>400</v>
       </c>
       <c r="C5" s="25" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="D5" s="25" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="E5" s="25">
         <v>1</v>
       </c>
       <c r="F5" s="25" t="s">
-        <v>397</v>
+        <v>391</v>
       </c>
       <c r="G5" s="25" t="s">
-        <v>408</v>
+        <v>396</v>
       </c>
       <c r="H5" s="27" t="s">
-        <v>360</v>
+        <v>354</v>
       </c>
       <c r="I5" s="25"/>
       <c r="J5" s="25"/>
@@ -3064,7 +2944,7 @@
       <c r="N5" s="25"/>
       <c r="O5" s="25"/>
       <c r="P5" s="25" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
     </row>
   </sheetData>
@@ -3073,7 +2953,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B7E404F-3B5C-4DD3-81F3-6BF8C7BC03AA}">
   <dimension ref="A1:D4"/>
   <sheetViews>
@@ -3107,10 +2987,10 @@
         <v>7</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="D2" s="7"/>
     </row>
@@ -3119,10 +2999,10 @@
         <v>1</v>
       </c>
       <c r="B3" s="26" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="C3" s="26" t="s">
-        <v>413</v>
+        <v>401</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
@@ -3130,10 +3010,10 @@
         <v>2</v>
       </c>
       <c r="B4" s="26" t="s">
-        <v>414</v>
+        <v>402</v>
       </c>
       <c r="C4" s="26" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
     </row>
   </sheetData>
@@ -3141,7 +3021,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C9F374A0-00F0-4E1C-9781-A1EAFC0D62B2}">
   <dimension ref="A1:G9"/>
   <sheetViews>
@@ -3171,16 +3051,16 @@
         <v>3</v>
       </c>
       <c r="D1" s="8" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="E1" s="8" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="F1" s="8" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="G1" s="8" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="58" x14ac:dyDescent="0.35">
@@ -3188,16 +3068,16 @@
         <v>7</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>422</v>
+        <v>410</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.35">
@@ -3205,13 +3085,13 @@
         <v>1</v>
       </c>
       <c r="B3" s="26" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="C3" s="26" t="s">
-        <v>415</v>
+        <v>403</v>
       </c>
       <c r="D3" s="15" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="E3" s="25">
         <v>1</v>
@@ -3228,13 +3108,13 @@
         <v>2</v>
       </c>
       <c r="B4" s="26" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="C4" s="26" t="s">
-        <v>416</v>
+        <v>404</v>
       </c>
       <c r="D4" s="15" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="E4" s="25">
         <v>0</v>
@@ -3251,13 +3131,13 @@
         <v>3</v>
       </c>
       <c r="B5" s="26" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="C5" s="26" t="s">
-        <v>417</v>
+        <v>405</v>
       </c>
       <c r="D5" s="15" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="E5" s="25">
         <v>0</v>
@@ -3274,13 +3154,13 @@
         <v>4</v>
       </c>
       <c r="B6" s="26" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="C6" s="26" t="s">
-        <v>418</v>
+        <v>406</v>
       </c>
       <c r="D6" s="15" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="E6" s="25">
         <v>0</v>
@@ -3297,13 +3177,13 @@
         <v>5</v>
       </c>
       <c r="B7" s="26" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="C7" s="26" t="s">
-        <v>419</v>
+        <v>407</v>
       </c>
       <c r="D7" s="15" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="E7" s="25">
         <v>0</v>
@@ -3320,13 +3200,13 @@
         <v>6</v>
       </c>
       <c r="B8" s="26" t="s">
-        <v>420</v>
+        <v>408</v>
       </c>
       <c r="C8" s="26" t="s">
-        <v>421</v>
+        <v>409</v>
       </c>
       <c r="D8" s="15" t="s">
-        <v>414</v>
+        <v>402</v>
       </c>
       <c r="E8" s="32">
         <v>1</v>
@@ -3344,7 +3224,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{103DB413-C452-4A76-9162-EF01DE565453}">
   <dimension ref="A1:D5"/>
   <sheetViews>
@@ -3378,10 +3258,10 @@
         <v>7</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="D2" s="7"/>
     </row>
@@ -3390,13 +3270,13 @@
         <v>1</v>
       </c>
       <c r="B3" s="26" t="s">
-        <v>423</v>
+        <v>411</v>
       </c>
       <c r="C3" s="26" t="s">
-        <v>424</v>
+        <v>412</v>
       </c>
       <c r="D3" s="26" t="s">
-        <v>425</v>
+        <v>413</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
@@ -3404,13 +3284,13 @@
         <v>2</v>
       </c>
       <c r="B4" s="26" t="s">
-        <v>426</v>
+        <v>414</v>
       </c>
       <c r="C4" s="26" t="s">
-        <v>427</v>
+        <v>415</v>
       </c>
       <c r="D4" s="26" t="s">
-        <v>428</v>
+        <v>416</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.35">
@@ -3418,13 +3298,13 @@
         <v>3</v>
       </c>
       <c r="B5" s="26" t="s">
-        <v>429</v>
+        <v>417</v>
       </c>
       <c r="C5" s="26" t="s">
-        <v>430</v>
+        <v>418</v>
       </c>
       <c r="D5" s="26" t="s">
-        <v>431</v>
+        <v>419</v>
       </c>
     </row>
   </sheetData>
@@ -3432,7 +3312,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E783ACB7-D919-4F74-AC1A-D54D8522C4AB}">
   <dimension ref="A1:D5"/>
   <sheetViews>
@@ -3466,10 +3346,10 @@
         <v>7</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>452</v>
+        <v>440</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>453</v>
+        <v>441</v>
       </c>
       <c r="D2" s="7"/>
     </row>
@@ -3481,7 +3361,7 @@
         <v>1</v>
       </c>
       <c r="C3" s="26" t="s">
-        <v>424</v>
+        <v>412</v>
       </c>
       <c r="D3" s="26"/>
     </row>
@@ -3493,7 +3373,7 @@
         <v>2</v>
       </c>
       <c r="C4" s="26" t="s">
-        <v>427</v>
+        <v>415</v>
       </c>
       <c r="D4" s="26"/>
     </row>
@@ -3505,7 +3385,7 @@
         <v>3</v>
       </c>
       <c r="C5" s="26" t="s">
-        <v>430</v>
+        <v>418</v>
       </c>
       <c r="D5" s="26"/>
     </row>
@@ -3514,7 +3394,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA1C2273-23CD-4D05-8CA4-F0EB0A365E8D}">
   <dimension ref="A1:Y5"/>
   <sheetViews>
@@ -3557,70 +3437,70 @@
         <v>3</v>
       </c>
       <c r="D1" s="14" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="E1" s="14" t="s">
         <v>80</v>
       </c>
       <c r="F1" s="14" t="s">
+        <v>158</v>
+      </c>
+      <c r="G1" s="14" t="s">
+        <v>159</v>
+      </c>
+      <c r="H1" s="14" t="s">
+        <v>160</v>
+      </c>
+      <c r="I1" s="14" t="s">
+        <v>438</v>
+      </c>
+      <c r="J1" s="14" t="s">
         <v>161</v>
       </c>
-      <c r="G1" s="14" t="s">
+      <c r="K1" s="14" t="s">
         <v>162</v>
       </c>
-      <c r="H1" s="14" t="s">
+      <c r="L1" s="14" t="s">
         <v>163</v>
       </c>
-      <c r="I1" s="14" t="s">
-        <v>450</v>
-      </c>
-      <c r="J1" s="14" t="s">
+      <c r="M1" s="14" t="s">
         <v>164</v>
       </c>
-      <c r="K1" s="14" t="s">
+      <c r="N1" s="14" t="s">
         <v>165</v>
       </c>
-      <c r="L1" s="14" t="s">
+      <c r="O1" s="14" t="s">
         <v>166</v>
       </c>
-      <c r="M1" s="14" t="s">
+      <c r="P1" s="14" t="s">
         <v>167</v>
       </c>
-      <c r="N1" s="14" t="s">
+      <c r="Q1" s="14" t="s">
         <v>168</v>
       </c>
-      <c r="O1" s="14" t="s">
+      <c r="R1" s="14" t="s">
         <v>169</v>
       </c>
-      <c r="P1" s="14" t="s">
+      <c r="S1" s="14" t="s">
+        <v>433</v>
+      </c>
+      <c r="T1" s="14" t="s">
         <v>170</v>
       </c>
-      <c r="Q1" s="14" t="s">
+      <c r="U1" s="14" t="s">
+        <v>435</v>
+      </c>
+      <c r="V1" s="14" t="s">
+        <v>436</v>
+      </c>
+      <c r="W1" s="14" t="s">
         <v>171</v>
       </c>
-      <c r="R1" s="14" t="s">
+      <c r="X1" s="14" t="s">
         <v>172</v>
       </c>
-      <c r="S1" s="14" t="s">
-        <v>445</v>
-      </c>
-      <c r="T1" s="14" t="s">
+      <c r="Y1" s="14" t="s">
         <v>173</v>
-      </c>
-      <c r="U1" s="14" t="s">
-        <v>447</v>
-      </c>
-      <c r="V1" s="14" t="s">
-        <v>448</v>
-      </c>
-      <c r="W1" s="14" t="s">
-        <v>174</v>
-      </c>
-      <c r="X1" s="14" t="s">
-        <v>175</v>
-      </c>
-      <c r="Y1" s="14" t="s">
-        <v>176</v>
       </c>
     </row>
     <row r="2" spans="1:25" ht="145" x14ac:dyDescent="0.35">
@@ -3628,30 +3508,30 @@
         <v>7</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="D2" s="7"/>
       <c r="E2" s="16"/>
       <c r="F2" s="16" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="G2" s="16" t="s">
-        <v>454</v>
+        <v>442</v>
       </c>
       <c r="H2" s="16" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="I2" s="16" t="s">
-        <v>451</v>
+        <v>439</v>
       </c>
       <c r="J2" s="7" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="K2" s="16" t="s">
-        <v>444</v>
+        <v>432</v>
       </c>
       <c r="L2" s="16"/>
       <c r="M2" s="16"/>
@@ -3659,29 +3539,29 @@
       <c r="O2" s="16"/>
       <c r="P2" s="16"/>
       <c r="Q2" s="16" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="R2" s="16" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="S2" s="16" t="s">
-        <v>446</v>
+        <v>434</v>
       </c>
       <c r="T2" s="16" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="U2" s="16" t="s">
-        <v>449</v>
+        <v>437</v>
       </c>
       <c r="V2" s="16"/>
       <c r="W2" s="16" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="X2" s="16" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="Y2" s="16" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
     </row>
     <row r="3" spans="1:25" x14ac:dyDescent="0.35">
@@ -3689,29 +3569,29 @@
         <v>1</v>
       </c>
       <c r="B3" s="33" t="s">
-        <v>432</v>
+        <v>420</v>
       </c>
       <c r="C3" s="33" t="s">
-        <v>433</v>
+        <v>421</v>
       </c>
       <c r="D3" s="33">
         <v>123</v>
       </c>
       <c r="E3" s="33" t="s">
-        <v>425</v>
+        <v>413</v>
       </c>
       <c r="F3" s="33" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="G3" s="33" t="s">
-        <v>434</v>
+        <v>422</v>
       </c>
       <c r="H3" s="33" t="s">
-        <v>423</v>
+        <v>411</v>
       </c>
       <c r="I3" s="33"/>
       <c r="J3" s="26" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="K3" s="33">
         <v>1</v>
@@ -3722,14 +3602,14 @@
       <c r="O3" s="33"/>
       <c r="P3" s="33"/>
       <c r="Q3" s="26" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="R3" s="33" t="s">
-        <v>393</v>
+        <v>387</v>
       </c>
       <c r="S3" s="33"/>
       <c r="T3" s="26" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="U3" s="33">
         <v>0</v>
@@ -3738,10 +3618,10 @@
         <v>100000</v>
       </c>
       <c r="W3" s="26" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="X3" s="33" t="s">
-        <v>393</v>
+        <v>387</v>
       </c>
       <c r="Y3" s="33">
         <v>0</v>
@@ -3752,27 +3632,27 @@
         <v>2</v>
       </c>
       <c r="B4" s="33" t="s">
-        <v>435</v>
+        <v>423</v>
       </c>
       <c r="C4" s="33" t="s">
-        <v>436</v>
+        <v>424</v>
       </c>
       <c r="D4" s="33"/>
       <c r="E4" s="33" t="s">
-        <v>428</v>
+        <v>416</v>
       </c>
       <c r="F4" s="33" t="s">
-        <v>437</v>
+        <v>425</v>
       </c>
       <c r="G4" s="33" t="s">
-        <v>434</v>
+        <v>422</v>
       </c>
       <c r="H4" s="33" t="s">
-        <v>426</v>
+        <v>414</v>
       </c>
       <c r="I4" s="33"/>
       <c r="J4" s="26" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="K4" s="33">
         <v>0</v>
@@ -3783,16 +3663,16 @@
       <c r="O4" s="33"/>
       <c r="P4" s="33"/>
       <c r="Q4" s="26" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="R4" s="33" t="s">
-        <v>393</v>
+        <v>387</v>
       </c>
       <c r="S4" s="33">
         <v>200000</v>
       </c>
       <c r="T4" s="26" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="U4" s="33">
         <v>0</v>
@@ -3801,10 +3681,10 @@
         <v>200000</v>
       </c>
       <c r="W4" s="26" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="X4" s="33" t="s">
-        <v>393</v>
+        <v>387</v>
       </c>
       <c r="Y4" s="33">
         <v>0</v>
@@ -3815,27 +3695,27 @@
         <v>3</v>
       </c>
       <c r="B5" s="33" t="s">
-        <v>438</v>
+        <v>426</v>
       </c>
       <c r="C5" s="33" t="s">
-        <v>439</v>
+        <v>427</v>
       </c>
       <c r="D5" s="33"/>
       <c r="E5" s="33" t="s">
-        <v>431</v>
+        <v>419</v>
       </c>
       <c r="F5" s="33" t="s">
-        <v>437</v>
+        <v>425</v>
       </c>
       <c r="G5" s="33" t="s">
-        <v>440</v>
+        <v>428</v>
       </c>
       <c r="H5" s="33" t="s">
-        <v>429</v>
+        <v>417</v>
       </c>
       <c r="I5" s="33"/>
       <c r="J5" s="26" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="K5" s="33">
         <v>0</v>
@@ -3846,16 +3726,16 @@
       <c r="O5" s="33"/>
       <c r="P5" s="33"/>
       <c r="Q5" s="26" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="R5" s="33" t="s">
-        <v>393</v>
+        <v>387</v>
       </c>
       <c r="S5" s="33">
         <v>300000</v>
       </c>
       <c r="T5" s="26" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="U5" s="33">
         <v>0</v>
@@ -3864,10 +3744,10 @@
         <v>300000</v>
       </c>
       <c r="W5" s="26" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="X5" s="33" t="s">
-        <v>393</v>
+        <v>387</v>
       </c>
       <c r="Y5" s="33">
         <v>0</v>
@@ -3878,7 +3758,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FDBA7C1B-B0F0-4AC8-A907-82185EA45827}">
   <dimension ref="A1:D4"/>
   <sheetViews>
@@ -3914,13 +3794,13 @@
         <v>7</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
@@ -3931,7 +3811,7 @@
         <v>110</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
@@ -3942,7 +3822,7 @@
         <v>112</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
     </row>
   </sheetData>
@@ -3950,7 +3830,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A45619C8-AAF7-43DE-831A-2BED068D71D3}">
   <dimension ref="A1:K11"/>
   <sheetViews>
@@ -3980,31 +3860,31 @@
         <v>55</v>
       </c>
       <c r="C1" s="8" t="s">
+        <v>205</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>206</v>
+      </c>
+      <c r="E1" s="8" t="s">
+        <v>207</v>
+      </c>
+      <c r="F1" s="8" t="s">
         <v>208</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="G1" s="8" t="s">
         <v>209</v>
       </c>
-      <c r="E1" s="8" t="s">
+      <c r="H1" s="8" t="s">
         <v>210</v>
       </c>
-      <c r="F1" s="8" t="s">
+      <c r="I1" s="8" t="s">
         <v>211</v>
       </c>
-      <c r="G1" s="8" t="s">
+      <c r="J1" s="8" t="s">
         <v>212</v>
       </c>
-      <c r="H1" s="8" t="s">
+      <c r="K1" s="8" t="s">
         <v>213</v>
-      </c>
-      <c r="I1" s="8" t="s">
-        <v>214</v>
-      </c>
-      <c r="J1" s="8" t="s">
-        <v>215</v>
-      </c>
-      <c r="K1" s="8" t="s">
-        <v>216</v>
       </c>
     </row>
     <row r="2" spans="1:11" ht="85.9" customHeight="1" x14ac:dyDescent="0.35">
@@ -4012,31 +3892,31 @@
         <v>7</v>
       </c>
       <c r="B2" s="10" t="s">
+        <v>214</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>215</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>216</v>
+      </c>
+      <c r="E2" s="7" t="s">
         <v>217</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="F2" s="7" t="s">
         <v>218</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="G2" s="7" t="s">
         <v>219</v>
       </c>
-      <c r="E2" s="7" t="s">
+      <c r="H2" s="7" t="s">
         <v>220</v>
       </c>
-      <c r="F2" s="7" t="s">
+      <c r="I2" s="7" t="s">
         <v>221</v>
       </c>
-      <c r="G2" s="7" t="s">
+      <c r="J2" s="7" t="s">
         <v>222</v>
-      </c>
-      <c r="H2" s="7" t="s">
-        <v>223</v>
-      </c>
-      <c r="I2" s="7" t="s">
-        <v>224</v>
-      </c>
-      <c r="J2" s="7" t="s">
-        <v>225</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.35">
@@ -4044,26 +3924,26 @@
         <v>1</v>
       </c>
       <c r="B3" s="25" t="s">
-        <v>441</v>
+        <v>429</v>
       </c>
       <c r="C3" s="27" t="s">
-        <v>372</v>
+        <v>366</v>
       </c>
       <c r="D3" s="25">
         <v>1</v>
       </c>
       <c r="E3" s="25" t="s">
-        <v>442</v>
+        <v>430</v>
       </c>
       <c r="F3" s="25" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="G3" s="25"/>
       <c r="H3" s="25">
         <v>903331332</v>
       </c>
       <c r="I3" s="34" t="s">
-        <v>443</v>
+        <v>431</v>
       </c>
       <c r="J3" s="25"/>
       <c r="K3" s="25"/>
@@ -4097,6 +3977,72 @@
   <hyperlinks>
     <hyperlink ref="I3" r:id="rId1" display="mailto:nva@example.com" xr:uid="{F6D89C5D-FF1D-47B0-919B-E0B60A9F5428}"/>
   </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E863D4F3-258D-41FD-90A7-5BEE0F94C0B4}">
+  <dimension ref="A1:F2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="8.81640625" style="7"/>
+    <col min="2" max="2" width="19.7265625" style="7" customWidth="1"/>
+    <col min="3" max="3" width="26" style="7" customWidth="1"/>
+    <col min="4" max="4" width="23.1796875" style="7" customWidth="1"/>
+    <col min="5" max="5" width="65.7265625" style="7" customWidth="1"/>
+    <col min="6" max="6" width="48.26953125" style="7" customWidth="1"/>
+    <col min="7" max="16384" width="8.81640625" style="7"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A1" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>200</v>
+      </c>
+      <c r="E1" s="8" t="s">
+        <v>201</v>
+      </c>
+      <c r="F1" s="8" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="172.9" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>202</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>203</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>204</v>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D1:D1048576" xr:uid="{7B04A94F-FAB7-487F-8C92-25C376949F35}">
+      <formula1>"0,1"</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -4137,37 +4083,37 @@
         <v>7</v>
       </c>
       <c r="B2" s="25" t="s">
+        <v>298</v>
+      </c>
+      <c r="C2" s="25" t="s">
+        <v>301</v>
+      </c>
+      <c r="D2" s="25" t="s">
         <v>304</v>
-      </c>
-      <c r="C2" s="25" t="s">
-        <v>307</v>
-      </c>
-      <c r="D2" s="25" t="s">
-        <v>310</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A3" s="39"/>
       <c r="B3" s="25" t="s">
+        <v>299</v>
+      </c>
+      <c r="C3" s="25" t="s">
+        <v>302</v>
+      </c>
+      <c r="D3" s="25" t="s">
         <v>305</v>
-      </c>
-      <c r="C3" s="25" t="s">
-        <v>308</v>
-      </c>
-      <c r="D3" s="25" t="s">
-        <v>311</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" s="39"/>
       <c r="B4" s="25" t="s">
+        <v>300</v>
+      </c>
+      <c r="C4" s="25" t="s">
+        <v>303</v>
+      </c>
+      <c r="D4" s="25" t="s">
         <v>306</v>
-      </c>
-      <c r="C4" s="25" t="s">
-        <v>309</v>
-      </c>
-      <c r="D4" s="25" t="s">
-        <v>312</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.35">
@@ -4175,7 +4121,7 @@
         <v>1</v>
       </c>
       <c r="B5" s="25" t="s">
-        <v>313</v>
+        <v>307</v>
       </c>
       <c r="C5" s="25" t="s">
         <v>48</v>
@@ -4187,7 +4133,7 @@
         <v>2</v>
       </c>
       <c r="B6" s="25" t="s">
-        <v>314</v>
+        <v>308</v>
       </c>
       <c r="C6" s="25" t="s">
         <v>49</v>
@@ -4211,10 +4157,10 @@
         <v>4</v>
       </c>
       <c r="B8" s="25" t="s">
-        <v>315</v>
+        <v>309</v>
       </c>
       <c r="C8" s="25" t="s">
-        <v>316</v>
+        <v>310</v>
       </c>
       <c r="D8" s="25"/>
     </row>
@@ -4223,7 +4169,7 @@
         <v>5</v>
       </c>
       <c r="B9" s="25" t="s">
-        <v>317</v>
+        <v>311</v>
       </c>
       <c r="C9" s="25" t="s">
         <v>52</v>
@@ -4247,10 +4193,10 @@
         <v>7</v>
       </c>
       <c r="B11" s="25" t="s">
-        <v>318</v>
+        <v>312</v>
       </c>
       <c r="C11" s="25" t="s">
-        <v>319</v>
+        <v>313</v>
       </c>
       <c r="D11" s="25"/>
     </row>
@@ -4263,77 +4209,11 @@
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E863D4F3-258D-41FD-90A7-5BEE0F94C0B4}">
-  <dimension ref="A1:F2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35B69A6E-98BC-434D-A419-FDB6C97F2A28}">
+  <dimension ref="A1:E45"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="8.81640625" style="7"/>
-    <col min="2" max="2" width="19.7265625" style="7" customWidth="1"/>
-    <col min="3" max="3" width="26" style="7" customWidth="1"/>
-    <col min="4" max="4" width="23.1796875" style="7" customWidth="1"/>
-    <col min="5" max="5" width="65.7265625" style="7" customWidth="1"/>
-    <col min="6" max="6" width="48.26953125" style="7" customWidth="1"/>
-    <col min="7" max="16384" width="8.81640625" style="7"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A1" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="8" t="s">
-        <v>55</v>
-      </c>
-      <c r="C1" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="D1" s="8" t="s">
-        <v>203</v>
-      </c>
-      <c r="E1" s="8" t="s">
-        <v>204</v>
-      </c>
-      <c r="F1" s="8" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" ht="172.9" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2" s="7" t="s">
-        <v>119</v>
-      </c>
-      <c r="C2" s="7" t="s">
-        <v>205</v>
-      </c>
-      <c r="D2" s="7" t="s">
-        <v>206</v>
-      </c>
-      <c r="E2" s="7" t="s">
-        <v>207</v>
-      </c>
-    </row>
-  </sheetData>
-  <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D1:D1048576" xr:uid="{7B04A94F-FAB7-487F-8C92-25C376949F35}">
-      <formula1>"0,1"</formula1>
-    </dataValidation>
-  </dataValidations>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35B69A6E-98BC-434D-A419-FDB6C97F2A28}">
-  <dimension ref="A1:E46"/>
-  <sheetViews>
-    <sheetView topLeftCell="A29" workbookViewId="0">
-      <selection activeCell="D43" sqref="D43"/>
+    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
+      <selection activeCell="G30" sqref="G30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4348,17 +4228,17 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="4" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="6" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="6" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
@@ -4384,7 +4264,7 @@
     </row>
     <row r="11" spans="1:5" ht="34.9" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="40" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="B11" s="41"/>
       <c r="C11" s="41"/>
@@ -4405,7 +4285,7 @@
     </row>
     <row r="16" spans="1:5" ht="28.9" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="42" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="B16" s="43"/>
       <c r="C16" s="43"/>
@@ -4414,7 +4294,7 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17" s="3" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="B17" s="45" t="s">
         <v>80</v>
@@ -4422,15 +4302,15 @@
       <c r="C17" s="45"/>
       <c r="D17" s="45"/>
       <c r="E17" s="3" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="B18" s="46" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="C18" s="46"/>
       <c r="D18" s="46"/>
@@ -4438,10 +4318,10 @@
     </row>
     <row r="19" spans="1:5" ht="29.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="1" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="B19" s="47" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="C19" s="47"/>
       <c r="D19" s="47"/>
@@ -4452,7 +4332,7 @@
         <v>0</v>
       </c>
       <c r="B20" s="47" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="C20" s="47"/>
       <c r="D20" s="47"/>
@@ -4479,7 +4359,7 @@
     </row>
     <row r="26" spans="1:5" ht="28.9" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A26" s="44" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="B26" s="44"/>
       <c r="C26" s="44"/>
@@ -4488,277 +4368,264 @@
     </row>
     <row r="27" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A27" s="20" t="s">
+        <v>241</v>
+      </c>
+      <c r="B27" s="20" t="s">
+        <v>242</v>
+      </c>
+      <c r="C27" s="20" t="s">
+        <v>243</v>
+      </c>
+      <c r="D27" s="21" t="s">
         <v>244</v>
       </c>
-      <c r="B27" s="20" t="s">
-        <v>245</v>
-      </c>
-      <c r="C27" s="20" t="s">
-        <v>246</v>
-      </c>
-      <c r="D27" s="21" t="s">
-        <v>247</v>
-      </c>
       <c r="E27" s="21" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
     </row>
     <row r="28" spans="1:5" ht="87" x14ac:dyDescent="0.35">
       <c r="A28" s="22" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="B28" s="22" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="C28" s="17" t="s">
         <v>58</v>
       </c>
       <c r="D28" s="19" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="E28" s="18" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
     </row>
     <row r="29" spans="1:5" ht="55.9" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A29" s="22" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="B29" s="22" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="C29" s="17" t="s">
         <v>62</v>
       </c>
       <c r="D29" s="19" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="E29" s="18"/>
     </row>
     <row r="30" spans="1:5" ht="62.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A30" s="22" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="B30" s="22" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="C30" s="17" t="s">
         <v>54</v>
       </c>
       <c r="D30" s="18" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="E30" s="18"/>
     </row>
     <row r="31" spans="1:5" ht="42.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A31" s="22" t="s">
+        <v>255</v>
+      </c>
+      <c r="B31" s="22" t="s">
+        <v>256</v>
+      </c>
+      <c r="C31" s="17" t="s">
+        <v>257</v>
+      </c>
+      <c r="D31" s="19" t="s">
         <v>258</v>
-      </c>
-      <c r="B31" s="22" t="s">
-        <v>259</v>
-      </c>
-      <c r="C31" s="17" t="s">
-        <v>260</v>
-      </c>
-      <c r="D31" s="19" t="s">
-        <v>261</v>
       </c>
       <c r="E31" s="18"/>
     </row>
     <row r="32" spans="1:5" ht="36" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A32" s="22" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="B32" s="22" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="C32" s="17" t="s">
         <v>76</v>
       </c>
       <c r="D32" s="19" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="E32" s="18"/>
     </row>
     <row r="33" spans="1:5" ht="36.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A33" s="23" t="s">
-        <v>274</v>
+        <v>269</v>
       </c>
       <c r="B33" s="23" t="s">
-        <v>291</v>
+        <v>286</v>
       </c>
       <c r="C33" s="17" t="s">
-        <v>286</v>
+        <v>281</v>
       </c>
       <c r="D33" s="18"/>
       <c r="E33" s="18"/>
     </row>
     <row r="34" spans="1:5" ht="38.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A34" s="23" t="s">
-        <v>276</v>
+        <v>271</v>
       </c>
       <c r="B34" s="23" t="s">
-        <v>292</v>
+        <v>287</v>
       </c>
       <c r="C34" s="17" t="s">
-        <v>302</v>
+        <v>296</v>
       </c>
       <c r="D34" s="18"/>
       <c r="E34" s="18"/>
     </row>
     <row r="35" spans="1:5" ht="39.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A35" s="22" t="s">
-        <v>275</v>
+        <v>270</v>
       </c>
       <c r="B35" s="22" t="s">
-        <v>293</v>
+        <v>288</v>
       </c>
       <c r="C35" s="17" t="s">
-        <v>285</v>
+        <v>280</v>
       </c>
       <c r="D35" s="18"/>
       <c r="E35" s="18"/>
     </row>
     <row r="36" spans="1:5" ht="32.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A36" s="22" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="B36" s="22" t="s">
-        <v>294</v>
+        <v>289</v>
       </c>
       <c r="C36" s="17" t="s">
-        <v>303</v>
+        <v>297</v>
       </c>
       <c r="D36" s="18"/>
       <c r="E36" s="18"/>
     </row>
     <row r="37" spans="1:5" ht="42.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A37" s="22" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="B37" s="22" t="s">
-        <v>295</v>
+        <v>290</v>
       </c>
       <c r="C37" s="17" t="s">
-        <v>268</v>
+        <v>279</v>
       </c>
       <c r="D37" s="18"/>
       <c r="E37" s="18"/>
     </row>
     <row r="38" spans="1:5" ht="42.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A38" s="22" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="B38" s="22" t="s">
-        <v>296</v>
+        <v>263</v>
       </c>
       <c r="C38" s="17" t="s">
-        <v>284</v>
+        <v>212</v>
       </c>
       <c r="D38" s="18"/>
       <c r="E38" s="18"/>
     </row>
     <row r="39" spans="1:5" ht="42.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A39" s="22" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="B39" s="22" t="s">
-        <v>266</v>
+        <v>291</v>
       </c>
       <c r="C39" s="17" t="s">
-        <v>215</v>
+        <v>284</v>
       </c>
       <c r="D39" s="18"/>
       <c r="E39" s="18"/>
     </row>
     <row r="40" spans="1:5" ht="42.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A40" s="22" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
       <c r="B40" s="22" t="s">
-        <v>297</v>
+        <v>292</v>
       </c>
       <c r="C40" s="17" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
       <c r="D40" s="18"/>
       <c r="E40" s="18"/>
     </row>
     <row r="41" spans="1:5" ht="42.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A41" s="22" t="s">
-        <v>279</v>
+        <v>272</v>
       </c>
       <c r="B41" s="22" t="s">
-        <v>298</v>
+        <v>293</v>
       </c>
       <c r="C41" s="17" t="s">
-        <v>290</v>
+        <v>283</v>
       </c>
       <c r="D41" s="18"/>
       <c r="E41" s="18"/>
     </row>
     <row r="42" spans="1:5" ht="42.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A42" s="22" t="s">
+      <c r="A42" s="23" t="s">
+        <v>276</v>
+      </c>
+      <c r="B42" s="23" t="s">
         <v>277</v>
       </c>
-      <c r="B42" s="22" t="s">
-        <v>299</v>
-      </c>
       <c r="C42" s="17" t="s">
-        <v>288</v>
+        <v>278</v>
       </c>
       <c r="D42" s="18"/>
       <c r="E42" s="18"/>
     </row>
     <row r="43" spans="1:5" ht="42.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A43" s="23" t="s">
-        <v>281</v>
-      </c>
-      <c r="B43" s="23" t="s">
+      <c r="A43" s="22" t="s">
+        <v>275</v>
+      </c>
+      <c r="B43" s="22" t="s">
+        <v>294</v>
+      </c>
+      <c r="C43" s="17" t="s">
         <v>282</v>
-      </c>
-      <c r="C43" s="17" t="s">
-        <v>283</v>
       </c>
       <c r="D43" s="18"/>
       <c r="E43" s="18"/>
     </row>
     <row r="44" spans="1:5" ht="42.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A44" s="22" t="s">
-        <v>280</v>
+        <v>267</v>
       </c>
       <c r="B44" s="22" t="s">
-        <v>300</v>
+        <v>268</v>
       </c>
       <c r="C44" s="17" t="s">
-        <v>287</v>
+        <v>136</v>
       </c>
       <c r="D44" s="18"/>
       <c r="E44" s="18"/>
     </row>
     <row r="45" spans="1:5" ht="42.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A45" s="22" t="s">
-        <v>272</v>
-      </c>
-      <c r="B45" s="22" t="s">
-        <v>273</v>
-      </c>
-      <c r="C45" s="17" t="s">
-        <v>138</v>
-      </c>
-      <c r="D45" s="18"/>
-      <c r="E45" s="18"/>
-    </row>
-    <row r="46" spans="1:5" ht="42.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A46" s="1" t="s">
-        <v>271</v>
-      </c>
-      <c r="B46" s="1" t="s">
-        <v>301</v>
-      </c>
-      <c r="C46" s="1"/>
-      <c r="D46" s="2"/>
-      <c r="E46" s="2"/>
+      <c r="A45" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>295</v>
+      </c>
+      <c r="C45" s="1"/>
+      <c r="D45" s="2"/>
+      <c r="E45" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="8">
@@ -4843,114 +4710,114 @@
         <v>7</v>
       </c>
       <c r="B2" s="25" t="s">
-        <v>304</v>
+        <v>298</v>
       </c>
       <c r="C2" s="25" t="s">
-        <v>307</v>
+        <v>301</v>
       </c>
       <c r="D2" s="25" t="s">
-        <v>307</v>
+        <v>301</v>
       </c>
       <c r="E2" s="25" t="s">
-        <v>307</v>
+        <v>301</v>
       </c>
       <c r="F2" s="25" t="s">
-        <v>307</v>
+        <v>301</v>
       </c>
       <c r="G2" s="25" t="s">
-        <v>336</v>
+        <v>330</v>
       </c>
       <c r="H2" s="25" t="s">
-        <v>339</v>
+        <v>333</v>
       </c>
       <c r="I2" s="25" t="s">
-        <v>339</v>
+        <v>333</v>
       </c>
       <c r="J2" s="25" t="s">
-        <v>341</v>
+        <v>335</v>
       </c>
       <c r="K2" s="25" t="s">
-        <v>344</v>
+        <v>338</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A3" s="39"/>
       <c r="B3" s="25" t="s">
-        <v>320</v>
+        <v>314</v>
       </c>
       <c r="C3" s="25" t="s">
-        <v>324</v>
+        <v>318</v>
       </c>
       <c r="D3" s="25" t="s">
-        <v>324</v>
+        <v>318</v>
       </c>
       <c r="E3" s="25" t="s">
-        <v>329</v>
+        <v>323</v>
       </c>
       <c r="F3" s="25" t="s">
-        <v>332</v>
+        <v>326</v>
       </c>
       <c r="G3" s="25" t="s">
-        <v>337</v>
+        <v>331</v>
       </c>
       <c r="H3" s="25" t="s">
-        <v>340</v>
+        <v>334</v>
       </c>
       <c r="I3" s="25" t="s">
-        <v>340</v>
+        <v>334</v>
       </c>
       <c r="J3" s="25" t="s">
-        <v>342</v>
+        <v>336</v>
       </c>
       <c r="K3" s="25" t="s">
-        <v>345</v>
+        <v>339</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A4" s="39"/>
       <c r="B4" s="25" t="s">
+        <v>315</v>
+      </c>
+      <c r="C4" s="25" t="s">
+        <v>319</v>
+      </c>
+      <c r="D4" s="25" t="s">
         <v>321</v>
       </c>
-      <c r="C4" s="25" t="s">
-        <v>325</v>
-      </c>
-      <c r="D4" s="25" t="s">
+      <c r="E4" s="25" t="s">
+        <v>324</v>
+      </c>
+      <c r="F4" s="25" t="s">
         <v>327</v>
       </c>
-      <c r="E4" s="25" t="s">
-        <v>330</v>
-      </c>
-      <c r="F4" s="25" t="s">
-        <v>333</v>
-      </c>
       <c r="G4" s="25" t="s">
-        <v>338</v>
+        <v>332</v>
       </c>
       <c r="H4" s="25"/>
       <c r="I4" s="25"/>
       <c r="J4" s="25" t="s">
-        <v>343</v>
+        <v>337</v>
       </c>
       <c r="K4" s="25" t="s">
-        <v>346</v>
+        <v>340</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A5" s="39"/>
       <c r="B5" s="25" t="s">
+        <v>316</v>
+      </c>
+      <c r="C5" s="25" t="s">
+        <v>320</v>
+      </c>
+      <c r="D5" s="25" t="s">
         <v>322</v>
       </c>
-      <c r="C5" s="25" t="s">
-        <v>326</v>
-      </c>
-      <c r="D5" s="25" t="s">
+      <c r="E5" s="25" t="s">
+        <v>325</v>
+      </c>
+      <c r="F5" s="25" t="s">
         <v>328</v>
-      </c>
-      <c r="E5" s="25" t="s">
-        <v>331</v>
-      </c>
-      <c r="F5" s="25" t="s">
-        <v>334</v>
       </c>
       <c r="G5" s="25"/>
       <c r="H5" s="25"/>
@@ -4961,13 +4828,13 @@
     <row r="6" spans="1:11" ht="32.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="39"/>
       <c r="B6" s="25" t="s">
-        <v>323</v>
+        <v>317</v>
       </c>
       <c r="C6" s="25"/>
       <c r="D6" s="25"/>
       <c r="E6" s="25"/>
       <c r="F6" s="25" t="s">
-        <v>335</v>
+        <v>329</v>
       </c>
       <c r="G6" s="25"/>
       <c r="H6" s="25"/>
@@ -4980,28 +4847,28 @@
         <v>1</v>
       </c>
       <c r="B7" s="27" t="s">
-        <v>347</v>
+        <v>341</v>
       </c>
       <c r="C7" s="25" t="s">
-        <v>348</v>
+        <v>342</v>
       </c>
       <c r="D7" s="25" t="s">
-        <v>349</v>
+        <v>343</v>
       </c>
       <c r="E7" s="35" t="s">
-        <v>350</v>
+        <v>344</v>
       </c>
       <c r="F7" s="25">
         <v>901123121</v>
       </c>
       <c r="G7" s="36" t="s">
-        <v>351</v>
+        <v>345</v>
       </c>
       <c r="H7" s="27" t="s">
-        <v>352</v>
+        <v>346</v>
       </c>
       <c r="I7" s="27" t="s">
-        <v>353</v>
+        <v>347</v>
       </c>
       <c r="J7" s="27"/>
       <c r="K7" s="27"/>
@@ -5011,28 +4878,28 @@
         <v>2</v>
       </c>
       <c r="B8" s="27" t="s">
-        <v>354</v>
+        <v>348</v>
       </c>
       <c r="C8" s="25" t="s">
-        <v>355</v>
+        <v>349</v>
       </c>
       <c r="D8" s="25" t="s">
-        <v>356</v>
+        <v>350</v>
       </c>
       <c r="E8" s="35" t="s">
-        <v>357</v>
+        <v>351</v>
       </c>
       <c r="F8" s="25">
         <v>901123122</v>
       </c>
       <c r="G8" s="36" t="s">
-        <v>358</v>
+        <v>352</v>
       </c>
       <c r="H8" s="27" t="s">
-        <v>352</v>
+        <v>346</v>
       </c>
       <c r="I8" s="27" t="s">
-        <v>359</v>
+        <v>353</v>
       </c>
       <c r="J8" s="27"/>
       <c r="K8" s="27"/>
@@ -5042,28 +4909,28 @@
         <v>3</v>
       </c>
       <c r="B9" s="27" t="s">
-        <v>360</v>
+        <v>354</v>
       </c>
       <c r="C9" s="25" t="s">
-        <v>361</v>
+        <v>355</v>
       </c>
       <c r="D9" s="25" t="s">
-        <v>362</v>
+        <v>356</v>
       </c>
       <c r="E9" s="35" t="s">
-        <v>363</v>
+        <v>357</v>
       </c>
       <c r="F9" s="25">
         <v>901123123</v>
       </c>
       <c r="G9" s="36" t="s">
-        <v>364</v>
+        <v>358</v>
       </c>
       <c r="H9" s="27" t="s">
-        <v>352</v>
+        <v>346</v>
       </c>
       <c r="I9" s="27" t="s">
-        <v>365</v>
+        <v>359</v>
       </c>
       <c r="J9" s="27"/>
       <c r="K9" s="27"/>
@@ -5073,28 +4940,28 @@
         <v>4</v>
       </c>
       <c r="B10" s="27" t="s">
-        <v>366</v>
+        <v>360</v>
       </c>
       <c r="C10" s="25" t="s">
-        <v>367</v>
+        <v>361</v>
       </c>
       <c r="D10" s="25" t="s">
-        <v>368</v>
+        <v>362</v>
       </c>
       <c r="E10" s="35" t="s">
-        <v>369</v>
+        <v>363</v>
       </c>
       <c r="F10" s="25">
         <v>901123124</v>
       </c>
       <c r="G10" s="36" t="s">
-        <v>370</v>
+        <v>364</v>
       </c>
       <c r="H10" s="27" t="s">
-        <v>352</v>
+        <v>346</v>
       </c>
       <c r="I10" s="27" t="s">
-        <v>371</v>
+        <v>365</v>
       </c>
       <c r="J10" s="27"/>
       <c r="K10" s="27"/>
@@ -5413,84 +5280,84 @@
         <v>7</v>
       </c>
       <c r="B2" s="25" t="s">
-        <v>304</v>
+        <v>298</v>
       </c>
       <c r="C2" s="25" t="s">
-        <v>307</v>
+        <v>301</v>
       </c>
       <c r="D2" s="25" t="s">
-        <v>307</v>
+        <v>301</v>
       </c>
       <c r="E2" s="25" t="s">
-        <v>380</v>
+        <v>374</v>
       </c>
       <c r="F2" s="38" t="s">
         <v>85</v>
       </c>
       <c r="G2" s="25" t="s">
-        <v>310</v>
+        <v>304</v>
       </c>
       <c r="H2" s="25" t="s">
-        <v>383</v>
+        <v>377</v>
       </c>
       <c r="I2" s="25" t="s">
-        <v>384</v>
+        <v>378</v>
       </c>
       <c r="J2" s="25" t="s">
-        <v>383</v>
+        <v>377</v>
       </c>
       <c r="K2" s="25" t="s">
-        <v>386</v>
+        <v>380</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="87" x14ac:dyDescent="0.35">
       <c r="A3" s="39"/>
       <c r="B3" s="25" t="s">
-        <v>373</v>
+        <v>367</v>
       </c>
       <c r="C3" s="25" t="s">
-        <v>376</v>
+        <v>370</v>
       </c>
       <c r="D3" s="25" t="s">
-        <v>378</v>
+        <v>372</v>
       </c>
       <c r="E3" s="25" t="s">
-        <v>381</v>
+        <v>375</v>
       </c>
       <c r="F3" s="39"/>
       <c r="G3" s="25" t="s">
-        <v>311</v>
+        <v>305</v>
       </c>
       <c r="H3" s="25" t="s">
-        <v>323</v>
+        <v>317</v>
       </c>
       <c r="I3" s="25" t="s">
-        <v>385</v>
+        <v>379</v>
       </c>
       <c r="J3" s="25" t="s">
-        <v>323</v>
+        <v>317</v>
       </c>
       <c r="K3" s="25" t="s">
-        <v>387</v>
+        <v>381</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A4" s="39"/>
       <c r="B4" s="25" t="s">
-        <v>374</v>
+        <v>368</v>
       </c>
       <c r="C4" s="25" t="s">
-        <v>377</v>
+        <v>371</v>
       </c>
       <c r="D4" s="25" t="s">
-        <v>379</v>
+        <v>373</v>
       </c>
       <c r="E4" s="25" t="s">
-        <v>343</v>
+        <v>337</v>
       </c>
       <c r="F4" s="39"/>
       <c r="G4" s="25" t="s">
-        <v>382</v>
+        <v>376</v>
       </c>
       <c r="H4" s="25"/>
       <c r="I4" s="25"/>
@@ -5500,14 +5367,14 @@
     <row r="5" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A5" s="39"/>
       <c r="B5" s="25" t="s">
-        <v>375</v>
+        <v>369</v>
       </c>
       <c r="C5" s="25"/>
       <c r="D5" s="25"/>
       <c r="E5" s="25"/>
       <c r="F5" s="39"/>
       <c r="G5" s="25" t="s">
-        <v>312</v>
+        <v>306</v>
       </c>
       <c r="H5" s="25"/>
       <c r="I5" s="25"/>
@@ -5555,11 +5422,11 @@
       </c>
       <c r="F7" s="25"/>
       <c r="G7" s="27" t="s">
-        <v>347</v>
+        <v>341</v>
       </c>
       <c r="H7" s="25"/>
       <c r="I7" s="25" t="s">
-        <v>388</v>
+        <v>382</v>
       </c>
       <c r="J7" s="25"/>
       <c r="K7" s="25"/>
@@ -5582,7 +5449,7 @@
       </c>
       <c r="F8" s="25"/>
       <c r="G8" s="25" t="s">
-        <v>389</v>
+        <v>383</v>
       </c>
       <c r="H8" s="25"/>
       <c r="I8" s="25" t="s">
@@ -5609,7 +5476,7 @@
       </c>
       <c r="F9" s="25"/>
       <c r="G9" s="25" t="s">
-        <v>390</v>
+        <v>384</v>
       </c>
       <c r="H9" s="25"/>
       <c r="I9" s="25" t="s">
@@ -5770,7 +5637,7 @@
         <v>106</v>
       </c>
       <c r="D2" s="29" t="s">
-        <v>391</v>
+        <v>385</v>
       </c>
       <c r="E2" s="29" t="s">
         <v>107</v>
@@ -5784,10 +5651,10 @@
         <v>1</v>
       </c>
       <c r="B3" s="26" t="s">
-        <v>392</v>
+        <v>386</v>
       </c>
       <c r="C3" s="26" t="s">
-        <v>392</v>
+        <v>386</v>
       </c>
       <c r="D3" s="26">
         <v>1</v>
@@ -5804,10 +5671,10 @@
         <v>2</v>
       </c>
       <c r="B4" s="26" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="C4" s="26" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="D4" s="26">
         <v>1</v>
@@ -5824,10 +5691,10 @@
         <v>3</v>
       </c>
       <c r="B5" s="26" t="s">
-        <v>393</v>
+        <v>387</v>
       </c>
       <c r="C5" s="26" t="s">
-        <v>393</v>
+        <v>387</v>
       </c>
       <c r="D5" s="26">
         <v>1</v>
@@ -5844,10 +5711,10 @@
         <v>4</v>
       </c>
       <c r="B6" s="26" t="s">
-        <v>394</v>
+        <v>388</v>
       </c>
       <c r="C6" s="26" t="s">
-        <v>394</v>
+        <v>388</v>
       </c>
       <c r="D6" s="26">
         <v>1</v>
@@ -5911,7 +5778,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="25" t="s">
-        <v>395</v>
+        <v>389</v>
       </c>
       <c r="C3" s="25" t="s">
         <v>111</v>
@@ -5923,7 +5790,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="25" t="s">
-        <v>396</v>
+        <v>390</v>
       </c>
       <c r="C4" s="25" t="s">
         <v>113</v>
@@ -5935,7 +5802,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="25" t="s">
-        <v>397</v>
+        <v>391</v>
       </c>
       <c r="C5" s="25" t="s">
         <v>114</v>
@@ -5947,7 +5814,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="25" t="s">
-        <v>398</v>
+        <v>392</v>
       </c>
       <c r="C6" s="25" t="s">
         <v>115</v>
@@ -5959,7 +5826,7 @@
         <v>5</v>
       </c>
       <c r="B7" s="25" t="s">
-        <v>399</v>
+        <v>393</v>
       </c>
       <c r="C7" s="25" t="s">
         <v>116</v>

</xml_diff>

<commit_message>
[hotfix/master-viet] fix template import
</commit_message>
<xml_diff>
--- a/apps/core/fimport/static/fimport/template/mega-import.xlsx
+++ b/apps/core/fimport/static/fimport/template/mega-import.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PCAdmin\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4DD40C6-4954-4C8A-A567-41203BFC281F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75B98320-EA4A-4876-BF85-453034496394}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="803" firstSheet="13" activeTab="19" xr2:uid="{ABCF866D-F0C2-489F-81F3-6B45D3E3629E}"/>
   </bookViews>
@@ -55,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="630" uniqueCount="444">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="583" uniqueCount="413">
   <si>
     <t>STT</t>
   </si>
@@ -1274,33 +1274,6 @@
     <t xml:space="preserve">Nhóm tài khoản </t>
   </si>
   <si>
-    <t>- Bắt buộc, định danh</t>
-  </si>
-  <si>
-    <t>- Chỉ chứa chữ cái, số, gạch dưới, gạch ngang</t>
-  </si>
-  <si>
-    <t>- Ví dụ: BGD</t>
-  </si>
-  <si>
-    <t>- Bắt buộc</t>
-  </si>
-  <si>
-    <t>- Tên đại diện cho vai trò</t>
-  </si>
-  <si>
-    <t>- Ví dụ: Ban Giám Đốc</t>
-  </si>
-  <si>
-    <t>- Thành viên của phòng ban</t>
-  </si>
-  <si>
-    <t>- Danh sách mã nhân viên liên kết với nhau bằng dấu phẩy #hr.employees.</t>
-  </si>
-  <si>
-    <t>- Ví dụ: EMP0001,EMP0002</t>
-  </si>
-  <si>
     <t>KDBL</t>
   </si>
   <si>
@@ -1322,87 +1295,6 @@
     <t>Kỹ thuật triển khai</t>
   </si>
   <si>
-    <t>- Độ dài tối đa 150</t>
-  </si>
-  <si>
-    <t>- Chỉ chứa chữ cái, số, gạch dưới, gạch ngang.</t>
-  </si>
-  <si>
-    <t>- Mã định danh cho nhân viên</t>
-  </si>
-  <si>
-    <t>- Ví dụ: EMP0001</t>
-  </si>
-  <si>
-    <t>- Độ dài tối đa: 100</t>
-  </si>
-  <si>
-    <t>- Tên của nhân viên</t>
-  </si>
-  <si>
-    <t>- Ví dụ: A</t>
-  </si>
-  <si>
-    <t>- Họ của nhân viên</t>
-  </si>
-  <si>
-    <t>- Ví dụ: Nguyễn Văn</t>
-  </si>
-  <si>
-    <t>- Độ dài tối đa: 150</t>
-  </si>
-  <si>
-    <t>- Địa chỉ thư điện tử của nhân viên</t>
-  </si>
-  <si>
-    <t>- Ví dụ: anv@example.com</t>
-  </si>
-  <si>
-    <t>- Độ dài tối đa: 25</t>
-  </si>
-  <si>
-    <t>- Định dạng số điện thoại ở VN</t>
-  </si>
-  <si>
-    <t>- Số điện thoại liên lạc của nhân viên</t>
-  </si>
-  <si>
-    <t>- Ví dụ: 0987654321</t>
-  </si>
-  <si>
-    <t>- Mã người dùng tại #account.users</t>
-  </si>
-  <si>
-    <t>- Người dùng liên kết với nhân viên</t>
-  </si>
-  <si>
-    <t>- Ví dụ: anv</t>
-  </si>
-  <si>
-    <t>- Định dạng ngày-tháng-năm (DD-MM-YYYY)</t>
-  </si>
-  <si>
-    <t>- Ví dụ: 31-01-1970</t>
-  </si>
-  <si>
-    <t>- Mã của phòng ban tại #hr.groups</t>
-  </si>
-  <si>
-    <t>- Phòng ban mà nhân viên thuộc về</t>
-  </si>
-  <si>
-    <t>- Ví dụ: QLDH</t>
-  </si>
-  <si>
-    <t>- Mã của vai trò tại #hr.roles</t>
-  </si>
-  <si>
-    <t>- Danh sách mã vai trò liên kết với nhau bằng dấu phẩy.</t>
-  </si>
-  <si>
-    <t>- Ví dụ: QL</t>
-  </si>
-  <si>
     <t>HQ002</t>
   </si>
   <si>
@@ -1479,51 +1371,6 @@
   </si>
   <si>
     <t>HQ007</t>
-  </si>
-  <si>
-    <t>- Mã của nhóm (còn được gọi là phòng ban)</t>
-  </si>
-  <si>
-    <t>- Bao gồm chữ cái, số, gạch ngang, gạch dưới.</t>
-  </si>
-  <si>
-    <t>Ví dụ: QLDH</t>
-  </si>
-  <si>
-    <t>- Tên của nhóm</t>
-  </si>
-  <si>
-    <t>- Ví dụ: Quản Lý Điều Hành</t>
-  </si>
-  <si>
-    <t>- Mã định danh của phân cấp nhóm tại #hr.groups.level</t>
-  </si>
-  <si>
-    <t>- Ví dụ: 1</t>
-  </si>
-  <si>
-    <t>- Mã định danh của nhóm mà phân bổ cấp trên/lớp trên cho nhóm này tại #hr.groups</t>
-  </si>
-  <si>
-    <t>- Vui lòng đặt dòng không có lớp cha ở trên để đảm bảo nó được tạo trước khi được tại các con.</t>
-  </si>
-  <si>
-    <t>- Nhân viên liên kết sẽ tự động cập nhật thành nhóm này</t>
-  </si>
-  <si>
-    <t>- Mã nhân viên của trưởng quản lý nhóm</t>
-  </si>
-  <si>
-    <t>- Tiêu đề của quản lý trưởng</t>
-  </si>
-  <si>
-    <t>- Ví dụ: Tổng Giám Đốc</t>
-  </si>
-  <si>
-    <t>- Mô tả của quản lý phó</t>
-  </si>
-  <si>
-    <t>- Ví dụ: Phó Giám Đốc</t>
   </si>
   <si>
     <t>Trưởng phòng Kinh doanh</t>
@@ -1727,6 +1574,110 @@
 - Danh sách mã liên kết với nhau bằng dấu phẩy.
 - Mã loại tài khoản tại chức năng Master Data Config / Account/ Account Types
 - Ví dụ: AT001</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  - Bắt buộc, định danh
+  - Chỉ chứa chữ cái, số, gạch dưới, gạch ngang
+  - Ví dụ: BGD</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - Bắt buộc
+ - Tên đại diện cho vai trò
+ - Ví dụ: Ban Giám Đốc</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - Thành viên của phòng ban
+ - Danh sách mã nhân viên liên kết với nhau bằng dấu phẩy #hr.employees
+ - Ví dụ: EMP0001,EMP0002</t>
+  </si>
+  <si>
+    <t>1. Bắt buộc, định danh
+2. Độ dài tối đa 100
+3. Chỉ chứa chữ cái, số, gạch dưới, gạch ngang.
+4.Mã định danh cho nhân viên
+5.Ví dụ: EMP0001</t>
+  </si>
+  <si>
+    <t>1.Bắt buộc
+2.Độ dài tối đa: 100
+3.Tên của nhân viên
+4.Ví dụ: A</t>
+  </si>
+  <si>
+    <t>1.Bắt buộc
+2.Độ dài tối đa: 100
+3.Họ của nhân viên
+4.Ví dụ: Nguyễn Văn</t>
+  </si>
+  <si>
+    <t>1.Bắt buộc
+2.Độ dài tối đa: 150
+3.Địa chỉ thư điện tử của nhân viên
+4.Ví dụ: anv@example.com</t>
+  </si>
+  <si>
+    <t>1.Bắt buộc
+2.Độ dài tối đa: 25
+3.Định dạng số điện thoại ở VN
+4.Số điện thoại liên lạc của nhân viên
+5.Ví dụ: 0987654321</t>
+  </si>
+  <si>
+    <t>1.Mã người dùng tại #account.users
+2.Người dùng liên kết với nhân viên
+3.Ví dụ: anv</t>
+  </si>
+  <si>
+    <t>1.Định dạng ngày-tháng-năm (DD-MM-YYYY)
+2.Ví dụ: 31-01-1970</t>
+  </si>
+  <si>
+    <t>1.Mã của phòng ban tại #hr.groups
+2.Phòng ban mà nhân viên thuộc về</t>
+  </si>
+  <si>
+    <t>1.Mã của vai trò tại #hr.roles
+2.Danh sách mã vai trò liên kết với nhau bằng dấu phẩy.
+3.Ví dụ: QL</t>
+  </si>
+  <si>
+    <t>- Bắt buộc, định danh
+- Mã của nhóm (còn được gọi là phòng ban)
+- Bao gồm chữ cái, số, gạch ngang, gạch dưới.
+-Ví dụ: QLDH</t>
+  </si>
+  <si>
+    <t>- Bắt buộc
+- Tên của nhóm
+- Ví dụ: Quản Lý Điều Hành</t>
+  </si>
+  <si>
+    <t>- Bắt buộc
+- Mã định danh của phân cấp nhóm tại #hr.groups.level
+- Ví dụ: 1</t>
+  </si>
+  <si>
+    <t>- Mã định danh của nhóm mà phân bổ cấp trên/lớp trên cho nhóm này tại #hr.groups
+- Vui lòng đặt dòng không có lớp cha ở trên để đảm bảo nó được tạo trước khi được tại các con.
+- Ví dụ: QLDH</t>
+  </si>
+  <si>
+    <t>- Thành viên của phòng ban
+- Danh sách mã nhân viên liên kết với nhau bằng dấu phẩy #hr.employees.
+- Nhân viên liên kết sẽ tự động cập nhật thành nhóm này
+- Ví dụ: EMP0001,EMP0002</t>
+  </si>
+  <si>
+    <t>- Mã nhân viên của trưởng quản lý nhóm
+- Ví dụ: EMP0001</t>
+  </si>
+  <si>
+    <t>- Tiêu đề của quản lý trưởng
+- Ví dụ: Tổng Giám Đốc</t>
+  </si>
+  <si>
+    <t>- Mô tả của quản lý phó
+- Ví dụ: Phó Giám Đốc</t>
   </si>
 </sst>
 </file>
@@ -1947,7 +1898,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -2016,9 +1967,6 @@
     <xf numFmtId="0" fontId="10" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -2056,12 +2004,6 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2084,6 +2026,18 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="11" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="10" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2659,52 +2613,52 @@
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A3" s="25">
+      <c r="A3" s="24">
         <v>1</v>
       </c>
-      <c r="B3" s="25" t="s">
-        <v>394</v>
-      </c>
-      <c r="C3" s="25" t="s">
+      <c r="B3" s="24" t="s">
+        <v>343</v>
+      </c>
+      <c r="C3" s="24" t="s">
         <v>119</v>
       </c>
-      <c r="D3" s="25"/>
+      <c r="D3" s="24"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A4" s="25">
+      <c r="A4" s="24">
         <v>2</v>
       </c>
-      <c r="B4" s="25" t="s">
-        <v>395</v>
-      </c>
-      <c r="C4" s="25" t="s">
+      <c r="B4" s="24" t="s">
+        <v>344</v>
+      </c>
+      <c r="C4" s="24" t="s">
         <v>120</v>
       </c>
-      <c r="D4" s="25"/>
+      <c r="D4" s="24"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A5" s="25">
+      <c r="A5" s="24">
         <v>3</v>
       </c>
-      <c r="B5" s="25" t="s">
-        <v>396</v>
-      </c>
-      <c r="C5" s="25" t="s">
+      <c r="B5" s="24" t="s">
+        <v>345</v>
+      </c>
+      <c r="C5" s="24" t="s">
         <v>121</v>
       </c>
-      <c r="D5" s="25"/>
+      <c r="D5" s="24"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A6" s="25">
+      <c r="A6" s="24">
         <v>4</v>
       </c>
-      <c r="B6" s="25" t="s">
-        <v>397</v>
-      </c>
-      <c r="C6" s="25" t="s">
+      <c r="B6" s="24" t="s">
+        <v>346</v>
+      </c>
+      <c r="C6" s="24" t="s">
         <v>122</v>
       </c>
-      <c r="D6" s="25"/>
+      <c r="D6" s="24"/>
     </row>
   </sheetData>
   <phoneticPr fontId="6" type="noConversion"/>
@@ -2794,7 +2748,7 @@
         <v>138</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>443</v>
+        <v>392</v>
       </c>
       <c r="E2" s="7" t="s">
         <v>139</v>
@@ -2834,116 +2788,116 @@
       </c>
     </row>
     <row r="3" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="25">
+      <c r="A3" s="24">
         <v>1</v>
       </c>
-      <c r="B3" s="25" t="s">
-        <v>398</v>
-      </c>
-      <c r="C3" s="25" t="s">
+      <c r="B3" s="24" t="s">
+        <v>347</v>
+      </c>
+      <c r="C3" s="24" t="s">
         <v>151</v>
       </c>
-      <c r="D3" s="25" t="s">
+      <c r="D3" s="24" t="s">
         <v>152</v>
       </c>
-      <c r="E3" s="25">
+      <c r="E3" s="24">
         <v>1</v>
       </c>
-      <c r="F3" s="25" t="s">
-        <v>389</v>
-      </c>
-      <c r="G3" s="25" t="s">
-        <v>394</v>
-      </c>
-      <c r="H3" s="27" t="s">
-        <v>341</v>
-      </c>
-      <c r="I3" s="25"/>
-      <c r="J3" s="25"/>
-      <c r="K3" s="25"/>
-      <c r="L3" s="25">
+      <c r="F3" s="24" t="s">
+        <v>338</v>
+      </c>
+      <c r="G3" s="24" t="s">
+        <v>343</v>
+      </c>
+      <c r="H3" s="26" t="s">
+        <v>305</v>
+      </c>
+      <c r="I3" s="24"/>
+      <c r="J3" s="24"/>
+      <c r="K3" s="24"/>
+      <c r="L3" s="24">
         <v>311001023</v>
       </c>
-      <c r="M3" s="25"/>
-      <c r="N3" s="25"/>
-      <c r="O3" s="25"/>
-      <c r="P3" s="25" t="s">
+      <c r="M3" s="24"/>
+      <c r="N3" s="24"/>
+      <c r="O3" s="24"/>
+      <c r="P3" s="24" t="s">
         <v>154</v>
       </c>
     </row>
     <row r="4" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="25">
+      <c r="A4" s="24">
         <v>2</v>
       </c>
-      <c r="B4" s="25" t="s">
-        <v>399</v>
-      </c>
-      <c r="C4" s="25" t="s">
+      <c r="B4" s="24" t="s">
+        <v>348</v>
+      </c>
+      <c r="C4" s="24" t="s">
         <v>153</v>
       </c>
-      <c r="D4" s="25" t="s">
+      <c r="D4" s="24" t="s">
         <v>152</v>
       </c>
-      <c r="E4" s="25">
+      <c r="E4" s="24">
         <v>1</v>
       </c>
-      <c r="F4" s="25" t="s">
-        <v>390</v>
-      </c>
-      <c r="G4" s="25" t="s">
-        <v>395</v>
-      </c>
-      <c r="H4" s="27" t="s">
-        <v>348</v>
-      </c>
-      <c r="I4" s="25"/>
-      <c r="J4" s="25"/>
-      <c r="K4" s="25"/>
-      <c r="L4" s="25">
+      <c r="F4" s="24" t="s">
+        <v>339</v>
+      </c>
+      <c r="G4" s="24" t="s">
+        <v>344</v>
+      </c>
+      <c r="H4" s="26" t="s">
+        <v>312</v>
+      </c>
+      <c r="I4" s="24"/>
+      <c r="J4" s="24"/>
+      <c r="K4" s="24"/>
+      <c r="L4" s="24">
         <v>311001014</v>
       </c>
-      <c r="M4" s="25"/>
-      <c r="N4" s="25"/>
-      <c r="O4" s="25"/>
-      <c r="P4" s="25" t="s">
+      <c r="M4" s="24"/>
+      <c r="N4" s="24"/>
+      <c r="O4" s="24"/>
+      <c r="P4" s="24" t="s">
         <v>154</v>
       </c>
     </row>
     <row r="5" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="25">
+      <c r="A5" s="24">
         <v>3</v>
       </c>
-      <c r="B5" s="25" t="s">
-        <v>400</v>
-      </c>
-      <c r="C5" s="25" t="s">
+      <c r="B5" s="24" t="s">
+        <v>349</v>
+      </c>
+      <c r="C5" s="24" t="s">
         <v>155</v>
       </c>
-      <c r="D5" s="25" t="s">
+      <c r="D5" s="24" t="s">
         <v>156</v>
       </c>
-      <c r="E5" s="25">
+      <c r="E5" s="24">
         <v>1</v>
       </c>
-      <c r="F5" s="25" t="s">
-        <v>391</v>
-      </c>
-      <c r="G5" s="25" t="s">
-        <v>396</v>
-      </c>
-      <c r="H5" s="27" t="s">
-        <v>354</v>
-      </c>
-      <c r="I5" s="25"/>
-      <c r="J5" s="25"/>
-      <c r="K5" s="25"/>
-      <c r="L5" s="25">
+      <c r="F5" s="24" t="s">
+        <v>340</v>
+      </c>
+      <c r="G5" s="24" t="s">
+        <v>345</v>
+      </c>
+      <c r="H5" s="26" t="s">
+        <v>318</v>
+      </c>
+      <c r="I5" s="24"/>
+      <c r="J5" s="24"/>
+      <c r="K5" s="24"/>
+      <c r="L5" s="24">
         <v>311001015</v>
       </c>
-      <c r="M5" s="25"/>
-      <c r="N5" s="25"/>
-      <c r="O5" s="25"/>
-      <c r="P5" s="25" t="s">
+      <c r="M5" s="24"/>
+      <c r="N5" s="24"/>
+      <c r="O5" s="24"/>
+      <c r="P5" s="24" t="s">
         <v>154</v>
       </c>
     </row>
@@ -2995,24 +2949,24 @@
       <c r="D2" s="7"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A3" s="26">
+      <c r="A3" s="25">
         <v>1</v>
       </c>
-      <c r="B3" s="26" t="s">
+      <c r="B3" s="25" t="s">
         <v>195</v>
       </c>
-      <c r="C3" s="26" t="s">
-        <v>401</v>
+      <c r="C3" s="25" t="s">
+        <v>350</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A4" s="26">
+      <c r="A4" s="25">
         <v>2</v>
       </c>
-      <c r="B4" s="26" t="s">
-        <v>402</v>
-      </c>
-      <c r="C4" s="26" t="s">
+      <c r="B4" s="25" t="s">
+        <v>351</v>
+      </c>
+      <c r="C4" s="25" t="s">
         <v>167</v>
       </c>
     </row>
@@ -3077,147 +3031,147 @@
         <v>178</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>410</v>
+        <v>359</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A3" s="26">
+      <c r="A3" s="25">
         <v>1</v>
       </c>
-      <c r="B3" s="26" t="s">
+      <c r="B3" s="25" t="s">
         <v>194</v>
       </c>
-      <c r="C3" s="26" t="s">
-        <v>403</v>
+      <c r="C3" s="25" t="s">
+        <v>352</v>
       </c>
       <c r="D3" s="15" t="s">
         <v>195</v>
       </c>
-      <c r="E3" s="25">
+      <c r="E3" s="24">
         <v>1</v>
       </c>
-      <c r="F3" s="26">
+      <c r="F3" s="25">
         <v>1</v>
       </c>
-      <c r="G3" s="26">
+      <c r="G3" s="25">
         <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A4" s="26">
+      <c r="A4" s="25">
         <v>2</v>
       </c>
-      <c r="B4" s="26" t="s">
+      <c r="B4" s="25" t="s">
         <v>196</v>
       </c>
-      <c r="C4" s="26" t="s">
-        <v>404</v>
+      <c r="C4" s="25" t="s">
+        <v>353</v>
       </c>
       <c r="D4" s="15" t="s">
         <v>195</v>
       </c>
-      <c r="E4" s="25">
+      <c r="E4" s="24">
         <v>0</v>
       </c>
-      <c r="F4" s="26">
+      <c r="F4" s="25">
         <v>1</v>
       </c>
-      <c r="G4" s="26">
+      <c r="G4" s="25">
         <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A5" s="26">
+      <c r="A5" s="25">
         <v>3</v>
       </c>
-      <c r="B5" s="26" t="s">
+      <c r="B5" s="25" t="s">
         <v>197</v>
       </c>
-      <c r="C5" s="26" t="s">
-        <v>405</v>
+      <c r="C5" s="25" t="s">
+        <v>354</v>
       </c>
       <c r="D5" s="15" t="s">
         <v>195</v>
       </c>
-      <c r="E5" s="25">
+      <c r="E5" s="24">
         <v>0</v>
       </c>
-      <c r="F5" s="26">
+      <c r="F5" s="25">
         <v>1</v>
       </c>
-      <c r="G5" s="26">
+      <c r="G5" s="25">
         <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A6" s="26">
+      <c r="A6" s="25">
         <v>4</v>
       </c>
-      <c r="B6" s="26" t="s">
+      <c r="B6" s="25" t="s">
         <v>198</v>
       </c>
-      <c r="C6" s="26" t="s">
-        <v>406</v>
+      <c r="C6" s="25" t="s">
+        <v>355</v>
       </c>
       <c r="D6" s="15" t="s">
         <v>195</v>
       </c>
-      <c r="E6" s="25">
+      <c r="E6" s="24">
         <v>0</v>
       </c>
-      <c r="F6" s="26">
+      <c r="F6" s="25">
         <v>1</v>
       </c>
-      <c r="G6" s="26">
+      <c r="G6" s="25">
         <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A7" s="26">
+      <c r="A7" s="25">
         <v>5</v>
       </c>
-      <c r="B7" s="26" t="s">
+      <c r="B7" s="25" t="s">
         <v>199</v>
       </c>
-      <c r="C7" s="26" t="s">
-        <v>407</v>
+      <c r="C7" s="25" t="s">
+        <v>356</v>
       </c>
       <c r="D7" s="15" t="s">
         <v>195</v>
       </c>
-      <c r="E7" s="25">
+      <c r="E7" s="24">
         <v>0</v>
       </c>
-      <c r="F7" s="26">
+      <c r="F7" s="25">
         <v>1</v>
       </c>
-      <c r="G7" s="26">
+      <c r="G7" s="25">
         <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A8" s="26">
+      <c r="A8" s="25">
         <v>6</v>
       </c>
-      <c r="B8" s="26" t="s">
-        <v>408</v>
-      </c>
-      <c r="C8" s="26" t="s">
-        <v>409</v>
+      <c r="B8" s="25" t="s">
+        <v>357</v>
+      </c>
+      <c r="C8" s="25" t="s">
+        <v>358</v>
       </c>
       <c r="D8" s="15" t="s">
-        <v>402</v>
-      </c>
-      <c r="E8" s="32">
+        <v>351</v>
+      </c>
+      <c r="E8" s="31">
         <v>1</v>
       </c>
-      <c r="F8" s="26">
+      <c r="F8" s="25">
         <v>1</v>
       </c>
-      <c r="G8" s="26"/>
+      <c r="G8" s="25"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="E9" s="31"/>
+      <c r="E9" s="30"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3266,45 +3220,45 @@
       <c r="D2" s="7"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A3" s="26">
+      <c r="A3" s="25">
         <v>1</v>
       </c>
-      <c r="B3" s="26" t="s">
-        <v>411</v>
-      </c>
-      <c r="C3" s="26" t="s">
-        <v>412</v>
-      </c>
-      <c r="D3" s="26" t="s">
-        <v>413</v>
+      <c r="B3" s="25" t="s">
+        <v>360</v>
+      </c>
+      <c r="C3" s="25" t="s">
+        <v>361</v>
+      </c>
+      <c r="D3" s="25" t="s">
+        <v>362</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A4" s="26">
+      <c r="A4" s="25">
         <v>2</v>
       </c>
-      <c r="B4" s="26" t="s">
-        <v>414</v>
-      </c>
-      <c r="C4" s="26" t="s">
-        <v>415</v>
-      </c>
-      <c r="D4" s="26" t="s">
-        <v>416</v>
+      <c r="B4" s="25" t="s">
+        <v>363</v>
+      </c>
+      <c r="C4" s="25" t="s">
+        <v>364</v>
+      </c>
+      <c r="D4" s="25" t="s">
+        <v>365</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A5" s="26">
+      <c r="A5" s="25">
         <v>3</v>
       </c>
-      <c r="B5" s="26" t="s">
-        <v>417</v>
-      </c>
-      <c r="C5" s="26" t="s">
-        <v>418</v>
-      </c>
-      <c r="D5" s="26" t="s">
-        <v>419</v>
+      <c r="B5" s="25" t="s">
+        <v>366</v>
+      </c>
+      <c r="C5" s="25" t="s">
+        <v>367</v>
+      </c>
+      <c r="D5" s="25" t="s">
+        <v>368</v>
       </c>
     </row>
   </sheetData>
@@ -3346,48 +3300,48 @@
         <v>7</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>440</v>
+        <v>389</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>441</v>
+        <v>390</v>
       </c>
       <c r="D2" s="7"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A3" s="26">
+      <c r="A3" s="25">
         <v>1</v>
       </c>
-      <c r="B3" s="26">
+      <c r="B3" s="25">
         <v>1</v>
       </c>
-      <c r="C3" s="26" t="s">
-        <v>412</v>
-      </c>
-      <c r="D3" s="26"/>
+      <c r="C3" s="25" t="s">
+        <v>361</v>
+      </c>
+      <c r="D3" s="25"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A4" s="26">
+      <c r="A4" s="25">
         <v>2</v>
       </c>
-      <c r="B4" s="26">
+      <c r="B4" s="25">
         <v>2</v>
       </c>
-      <c r="C4" s="26" t="s">
-        <v>415</v>
-      </c>
-      <c r="D4" s="26"/>
+      <c r="C4" s="25" t="s">
+        <v>364</v>
+      </c>
+      <c r="D4" s="25"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A5" s="26">
+      <c r="A5" s="25">
         <v>3</v>
       </c>
-      <c r="B5" s="26">
+      <c r="B5" s="25">
         <v>3</v>
       </c>
-      <c r="C5" s="26" t="s">
-        <v>418</v>
-      </c>
-      <c r="D5" s="26"/>
+      <c r="C5" s="25" t="s">
+        <v>367</v>
+      </c>
+      <c r="D5" s="25"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3452,7 +3406,7 @@
         <v>160</v>
       </c>
       <c r="I1" s="14" t="s">
-        <v>438</v>
+        <v>387</v>
       </c>
       <c r="J1" s="14" t="s">
         <v>161</v>
@@ -3482,16 +3436,16 @@
         <v>169</v>
       </c>
       <c r="S1" s="14" t="s">
-        <v>433</v>
+        <v>382</v>
       </c>
       <c r="T1" s="14" t="s">
         <v>170</v>
       </c>
       <c r="U1" s="14" t="s">
-        <v>435</v>
+        <v>384</v>
       </c>
       <c r="V1" s="14" t="s">
-        <v>436</v>
+        <v>385</v>
       </c>
       <c r="W1" s="14" t="s">
         <v>171</v>
@@ -3519,19 +3473,19 @@
         <v>176</v>
       </c>
       <c r="G2" s="16" t="s">
-        <v>442</v>
+        <v>391</v>
       </c>
       <c r="H2" s="16" t="s">
         <v>177</v>
       </c>
       <c r="I2" s="16" t="s">
-        <v>439</v>
+        <v>388</v>
       </c>
       <c r="J2" s="7" t="s">
         <v>178</v>
       </c>
       <c r="K2" s="16" t="s">
-        <v>432</v>
+        <v>381</v>
       </c>
       <c r="L2" s="16"/>
       <c r="M2" s="16"/>
@@ -3545,13 +3499,13 @@
         <v>180</v>
       </c>
       <c r="S2" s="16" t="s">
-        <v>434</v>
+        <v>383</v>
       </c>
       <c r="T2" s="16" t="s">
         <v>181</v>
       </c>
       <c r="U2" s="16" t="s">
-        <v>437</v>
+        <v>386</v>
       </c>
       <c r="V2" s="16"/>
       <c r="W2" s="16" t="s">
@@ -3565,191 +3519,191 @@
       </c>
     </row>
     <row r="3" spans="1:25" x14ac:dyDescent="0.35">
-      <c r="A3" s="33">
+      <c r="A3" s="32">
         <v>1</v>
       </c>
-      <c r="B3" s="33" t="s">
-        <v>420</v>
-      </c>
-      <c r="C3" s="33" t="s">
-        <v>421</v>
-      </c>
-      <c r="D3" s="33">
+      <c r="B3" s="32" t="s">
+        <v>369</v>
+      </c>
+      <c r="C3" s="32" t="s">
+        <v>370</v>
+      </c>
+      <c r="D3" s="32">
         <v>123</v>
       </c>
-      <c r="E3" s="33" t="s">
-        <v>413</v>
-      </c>
-      <c r="F3" s="33" t="s">
+      <c r="E3" s="32" t="s">
+        <v>362</v>
+      </c>
+      <c r="F3" s="32" t="s">
         <v>185</v>
       </c>
-      <c r="G3" s="33" t="s">
-        <v>422</v>
-      </c>
-      <c r="H3" s="33" t="s">
-        <v>411</v>
-      </c>
-      <c r="I3" s="33"/>
-      <c r="J3" s="26" t="s">
+      <c r="G3" s="32" t="s">
+        <v>371</v>
+      </c>
+      <c r="H3" s="32" t="s">
+        <v>360</v>
+      </c>
+      <c r="I3" s="32"/>
+      <c r="J3" s="25" t="s">
         <v>195</v>
       </c>
-      <c r="K3" s="33">
+      <c r="K3" s="32">
         <v>1</v>
       </c>
-      <c r="L3" s="33"/>
-      <c r="M3" s="33"/>
-      <c r="N3" s="33"/>
-      <c r="O3" s="33"/>
-      <c r="P3" s="33"/>
-      <c r="Q3" s="26" t="s">
+      <c r="L3" s="32"/>
+      <c r="M3" s="32"/>
+      <c r="N3" s="32"/>
+      <c r="O3" s="32"/>
+      <c r="P3" s="32"/>
+      <c r="Q3" s="25" t="s">
         <v>194</v>
       </c>
-      <c r="R3" s="33" t="s">
-        <v>387</v>
-      </c>
-      <c r="S3" s="33"/>
-      <c r="T3" s="26" t="s">
+      <c r="R3" s="32" t="s">
+        <v>336</v>
+      </c>
+      <c r="S3" s="32"/>
+      <c r="T3" s="25" t="s">
         <v>194</v>
       </c>
-      <c r="U3" s="33">
+      <c r="U3" s="32">
         <v>0</v>
       </c>
-      <c r="V3" s="26">
+      <c r="V3" s="25">
         <v>100000</v>
       </c>
-      <c r="W3" s="26" t="s">
+      <c r="W3" s="25" t="s">
         <v>194</v>
       </c>
-      <c r="X3" s="33" t="s">
-        <v>387</v>
-      </c>
-      <c r="Y3" s="33">
+      <c r="X3" s="32" t="s">
+        <v>336</v>
+      </c>
+      <c r="Y3" s="32">
         <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:25" x14ac:dyDescent="0.35">
-      <c r="A4" s="33">
+      <c r="A4" s="32">
         <v>2</v>
       </c>
-      <c r="B4" s="33" t="s">
-        <v>423</v>
-      </c>
-      <c r="C4" s="33" t="s">
-        <v>424</v>
-      </c>
-      <c r="D4" s="33"/>
-      <c r="E4" s="33" t="s">
-        <v>416</v>
-      </c>
-      <c r="F4" s="33" t="s">
-        <v>425</v>
-      </c>
-      <c r="G4" s="33" t="s">
-        <v>422</v>
-      </c>
-      <c r="H4" s="33" t="s">
-        <v>414</v>
-      </c>
-      <c r="I4" s="33"/>
-      <c r="J4" s="26" t="s">
+      <c r="B4" s="32" t="s">
+        <v>372</v>
+      </c>
+      <c r="C4" s="32" t="s">
+        <v>373</v>
+      </c>
+      <c r="D4" s="32"/>
+      <c r="E4" s="32" t="s">
+        <v>365</v>
+      </c>
+      <c r="F4" s="32" t="s">
+        <v>374</v>
+      </c>
+      <c r="G4" s="32" t="s">
+        <v>371</v>
+      </c>
+      <c r="H4" s="32" t="s">
+        <v>363</v>
+      </c>
+      <c r="I4" s="32"/>
+      <c r="J4" s="25" t="s">
         <v>195</v>
       </c>
-      <c r="K4" s="33">
+      <c r="K4" s="32">
         <v>0</v>
       </c>
-      <c r="L4" s="33"/>
-      <c r="M4" s="33"/>
-      <c r="N4" s="33"/>
-      <c r="O4" s="33"/>
-      <c r="P4" s="33"/>
-      <c r="Q4" s="26" t="s">
+      <c r="L4" s="32"/>
+      <c r="M4" s="32"/>
+      <c r="N4" s="32"/>
+      <c r="O4" s="32"/>
+      <c r="P4" s="32"/>
+      <c r="Q4" s="25" t="s">
         <v>194</v>
       </c>
-      <c r="R4" s="33" t="s">
-        <v>387</v>
-      </c>
-      <c r="S4" s="33">
+      <c r="R4" s="32" t="s">
+        <v>336</v>
+      </c>
+      <c r="S4" s="32">
         <v>200000</v>
       </c>
-      <c r="T4" s="26" t="s">
+      <c r="T4" s="25" t="s">
         <v>194</v>
       </c>
-      <c r="U4" s="33">
+      <c r="U4" s="32">
         <v>0</v>
       </c>
-      <c r="V4" s="26">
+      <c r="V4" s="25">
         <v>200000</v>
       </c>
-      <c r="W4" s="26" t="s">
+      <c r="W4" s="25" t="s">
         <v>194</v>
       </c>
-      <c r="X4" s="33" t="s">
-        <v>387</v>
-      </c>
-      <c r="Y4" s="33">
+      <c r="X4" s="32" t="s">
+        <v>336</v>
+      </c>
+      <c r="Y4" s="32">
         <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:25" x14ac:dyDescent="0.35">
-      <c r="A5" s="33">
+      <c r="A5" s="32">
         <v>3</v>
       </c>
-      <c r="B5" s="33" t="s">
-        <v>426</v>
-      </c>
-      <c r="C5" s="33" t="s">
-        <v>427</v>
-      </c>
-      <c r="D5" s="33"/>
-      <c r="E5" s="33" t="s">
-        <v>419</v>
-      </c>
-      <c r="F5" s="33" t="s">
-        <v>425</v>
-      </c>
-      <c r="G5" s="33" t="s">
-        <v>428</v>
-      </c>
-      <c r="H5" s="33" t="s">
-        <v>417</v>
-      </c>
-      <c r="I5" s="33"/>
-      <c r="J5" s="26" t="s">
+      <c r="B5" s="32" t="s">
+        <v>375</v>
+      </c>
+      <c r="C5" s="32" t="s">
+        <v>376</v>
+      </c>
+      <c r="D5" s="32"/>
+      <c r="E5" s="32" t="s">
+        <v>368</v>
+      </c>
+      <c r="F5" s="32" t="s">
+        <v>374</v>
+      </c>
+      <c r="G5" s="32" t="s">
+        <v>377</v>
+      </c>
+      <c r="H5" s="32" t="s">
+        <v>366</v>
+      </c>
+      <c r="I5" s="32"/>
+      <c r="J5" s="25" t="s">
         <v>195</v>
       </c>
-      <c r="K5" s="33">
+      <c r="K5" s="32">
         <v>0</v>
       </c>
-      <c r="L5" s="33"/>
-      <c r="M5" s="33"/>
-      <c r="N5" s="33"/>
-      <c r="O5" s="33"/>
-      <c r="P5" s="33"/>
-      <c r="Q5" s="26" t="s">
+      <c r="L5" s="32"/>
+      <c r="M5" s="32"/>
+      <c r="N5" s="32"/>
+      <c r="O5" s="32"/>
+      <c r="P5" s="32"/>
+      <c r="Q5" s="25" t="s">
         <v>194</v>
       </c>
-      <c r="R5" s="33" t="s">
-        <v>387</v>
-      </c>
-      <c r="S5" s="33">
+      <c r="R5" s="32" t="s">
+        <v>336</v>
+      </c>
+      <c r="S5" s="32">
         <v>300000</v>
       </c>
-      <c r="T5" s="26" t="s">
+      <c r="T5" s="25" t="s">
         <v>194</v>
       </c>
-      <c r="U5" s="33">
+      <c r="U5" s="32">
         <v>0</v>
       </c>
-      <c r="V5" s="26">
+      <c r="V5" s="25">
         <v>300000</v>
       </c>
-      <c r="W5" s="26" t="s">
+      <c r="W5" s="25" t="s">
         <v>194</v>
       </c>
-      <c r="X5" s="33" t="s">
-        <v>387</v>
-      </c>
-      <c r="Y5" s="33">
+      <c r="X5" s="32" t="s">
+        <v>336</v>
+      </c>
+      <c r="Y5" s="32">
         <v>0</v>
       </c>
     </row>
@@ -3920,33 +3874,33 @@
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A3" s="25">
+      <c r="A3" s="24">
         <v>1</v>
       </c>
-      <c r="B3" s="25" t="s">
-        <v>429</v>
-      </c>
-      <c r="C3" s="27" t="s">
-        <v>366</v>
-      </c>
-      <c r="D3" s="25">
+      <c r="B3" s="24" t="s">
+        <v>378</v>
+      </c>
+      <c r="C3" s="26" t="s">
+        <v>330</v>
+      </c>
+      <c r="D3" s="24">
         <v>1</v>
       </c>
-      <c r="E3" s="25" t="s">
-        <v>430</v>
-      </c>
-      <c r="F3" s="25" t="s">
+      <c r="E3" s="24" t="s">
+        <v>379</v>
+      </c>
+      <c r="F3" s="24" t="s">
         <v>223</v>
       </c>
-      <c r="G3" s="25"/>
-      <c r="H3" s="25">
+      <c r="G3" s="24"/>
+      <c r="H3" s="24">
         <v>903331332</v>
       </c>
-      <c r="I3" s="34" t="s">
-        <v>431</v>
-      </c>
-      <c r="J3" s="25"/>
-      <c r="K3" s="25"/>
+      <c r="I3" s="33" t="s">
+        <v>380</v>
+      </c>
+      <c r="J3" s="24"/>
+      <c r="K3" s="24"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.35">
       <c r="I4" s="12"/>
@@ -4049,10 +4003,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C373C485-720B-481D-9EE6-F43D8158DF65}">
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4065,145 +4019,118 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="46" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="24" t="s">
+      <c r="B1" s="46" t="s">
         <v>45</v>
       </c>
-      <c r="C1" s="24" t="s">
+      <c r="C1" s="46" t="s">
         <v>46</v>
       </c>
-      <c r="D1" s="24" t="s">
+      <c r="D1" s="46" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="75.650000000000006" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="38" t="s">
+      <c r="A2" s="48" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="25" t="s">
+      <c r="B2" s="45" t="s">
+        <v>393</v>
+      </c>
+      <c r="C2" s="45" t="s">
+        <v>394</v>
+      </c>
+      <c r="D2" s="45" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A3" s="45">
+        <v>1</v>
+      </c>
+      <c r="B3" s="45" t="s">
         <v>298</v>
       </c>
-      <c r="C2" s="25" t="s">
+      <c r="C3" s="45" t="s">
+        <v>48</v>
+      </c>
+      <c r="D3" s="45"/>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A4" s="45">
+        <v>2</v>
+      </c>
+      <c r="B4" s="45" t="s">
+        <v>299</v>
+      </c>
+      <c r="C4" s="45" t="s">
+        <v>49</v>
+      </c>
+      <c r="D4" s="45"/>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A5" s="45">
+        <v>3</v>
+      </c>
+      <c r="B5" s="45" t="s">
+        <v>50</v>
+      </c>
+      <c r="C5" s="45" t="s">
+        <v>51</v>
+      </c>
+      <c r="D5" s="47"/>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A6" s="45">
+        <v>4</v>
+      </c>
+      <c r="B6" s="45" t="s">
+        <v>300</v>
+      </c>
+      <c r="C6" s="45" t="s">
         <v>301</v>
       </c>
-      <c r="D2" s="25" t="s">
+      <c r="D6" s="45"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A7" s="45">
+        <v>5</v>
+      </c>
+      <c r="B7" s="45" t="s">
+        <v>302</v>
+      </c>
+      <c r="C7" s="45" t="s">
+        <v>52</v>
+      </c>
+      <c r="D7" s="45"/>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A8" s="45">
+        <v>6</v>
+      </c>
+      <c r="B8" s="45" t="s">
+        <v>53</v>
+      </c>
+      <c r="C8" s="45" t="s">
+        <v>54</v>
+      </c>
+      <c r="D8" s="45"/>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A9" s="45">
+        <v>7</v>
+      </c>
+      <c r="B9" s="45" t="s">
+        <v>303</v>
+      </c>
+      <c r="C9" s="45" t="s">
         <v>304</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" ht="29" x14ac:dyDescent="0.35">
-      <c r="A3" s="39"/>
-      <c r="B3" s="25" t="s">
-        <v>299</v>
-      </c>
-      <c r="C3" s="25" t="s">
-        <v>302</v>
-      </c>
-      <c r="D3" s="25" t="s">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A4" s="39"/>
-      <c r="B4" s="25" t="s">
-        <v>300</v>
-      </c>
-      <c r="C4" s="25" t="s">
-        <v>303</v>
-      </c>
-      <c r="D4" s="25" t="s">
-        <v>306</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A5" s="25">
-        <v>1</v>
-      </c>
-      <c r="B5" s="25" t="s">
-        <v>307</v>
-      </c>
-      <c r="C5" s="25" t="s">
-        <v>48</v>
-      </c>
-      <c r="D5" s="25"/>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A6" s="25">
-        <v>2</v>
-      </c>
-      <c r="B6" s="25" t="s">
-        <v>308</v>
-      </c>
-      <c r="C6" s="25" t="s">
-        <v>49</v>
-      </c>
-      <c r="D6" s="25"/>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A7" s="25">
-        <v>3</v>
-      </c>
-      <c r="B7" s="25" t="s">
-        <v>50</v>
-      </c>
-      <c r="C7" s="25" t="s">
-        <v>51</v>
-      </c>
-      <c r="D7" s="27"/>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A8" s="25">
-        <v>4</v>
-      </c>
-      <c r="B8" s="25" t="s">
-        <v>309</v>
-      </c>
-      <c r="C8" s="25" t="s">
-        <v>310</v>
-      </c>
-      <c r="D8" s="25"/>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A9" s="25">
-        <v>5</v>
-      </c>
-      <c r="B9" s="25" t="s">
-        <v>311</v>
-      </c>
-      <c r="C9" s="25" t="s">
-        <v>52</v>
-      </c>
-      <c r="D9" s="25"/>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A10" s="25">
-        <v>6</v>
-      </c>
-      <c r="B10" s="25" t="s">
-        <v>53</v>
-      </c>
-      <c r="C10" s="25" t="s">
-        <v>54</v>
-      </c>
-      <c r="D10" s="25"/>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A11" s="25">
-        <v>7</v>
-      </c>
-      <c r="B11" s="25" t="s">
-        <v>312</v>
-      </c>
-      <c r="C11" s="25" t="s">
-        <v>313</v>
-      </c>
-      <c r="D11" s="25"/>
+      <c r="D9" s="45"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A2:A4"/>
-  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -4213,7 +4140,7 @@
   <dimension ref="A1:E45"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
-      <selection activeCell="G30" sqref="G30"/>
+      <selection activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4263,13 +4190,13 @@
       <c r="A10" s="6"/>
     </row>
     <row r="11" spans="1:5" ht="34.9" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="40" t="s">
+      <c r="A11" s="37" t="s">
         <v>231</v>
       </c>
-      <c r="B11" s="41"/>
-      <c r="C11" s="41"/>
-      <c r="D11" s="41"/>
-      <c r="E11" s="41"/>
+      <c r="B11" s="38"/>
+      <c r="C11" s="38"/>
+      <c r="D11" s="38"/>
+      <c r="E11" s="38"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" s="6"/>
@@ -4284,23 +4211,23 @@
       <c r="A15" s="6"/>
     </row>
     <row r="16" spans="1:5" ht="28.9" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="42" t="s">
+      <c r="A16" s="39" t="s">
         <v>232</v>
       </c>
-      <c r="B16" s="43"/>
-      <c r="C16" s="43"/>
-      <c r="D16" s="43"/>
-      <c r="E16" s="43"/>
+      <c r="B16" s="40"/>
+      <c r="C16" s="40"/>
+      <c r="D16" s="40"/>
+      <c r="E16" s="40"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17" s="3" t="s">
         <v>233</v>
       </c>
-      <c r="B17" s="45" t="s">
+      <c r="B17" s="42" t="s">
         <v>80</v>
       </c>
-      <c r="C17" s="45"/>
-      <c r="D17" s="45"/>
+      <c r="C17" s="42"/>
+      <c r="D17" s="42"/>
       <c r="E17" s="3" t="s">
         <v>234</v>
       </c>
@@ -4309,40 +4236,40 @@
       <c r="A18" s="1" t="s">
         <v>235</v>
       </c>
-      <c r="B18" s="46" t="s">
+      <c r="B18" s="43" t="s">
         <v>236</v>
       </c>
-      <c r="C18" s="46"/>
-      <c r="D18" s="46"/>
+      <c r="C18" s="43"/>
+      <c r="D18" s="43"/>
       <c r="E18" s="1"/>
     </row>
     <row r="19" spans="1:5" ht="29.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="1" t="s">
         <v>237</v>
       </c>
-      <c r="B19" s="47" t="s">
+      <c r="B19" s="44" t="s">
         <v>238</v>
       </c>
-      <c r="C19" s="47"/>
-      <c r="D19" s="47"/>
+      <c r="C19" s="44"/>
+      <c r="D19" s="44"/>
       <c r="E19" s="1"/>
     </row>
     <row r="20" spans="1:5" ht="34.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B20" s="47" t="s">
+      <c r="B20" s="44" t="s">
         <v>239</v>
       </c>
-      <c r="C20" s="47"/>
-      <c r="D20" s="47"/>
+      <c r="C20" s="44"/>
+      <c r="D20" s="44"/>
       <c r="E20" s="1"/>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A21" s="1"/>
-      <c r="B21" s="46"/>
-      <c r="C21" s="46"/>
-      <c r="D21" s="46"/>
+      <c r="B21" s="43"/>
+      <c r="C21" s="43"/>
+      <c r="D21" s="43"/>
       <c r="E21" s="1"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.35">
@@ -4358,13 +4285,13 @@
       <c r="A25"/>
     </row>
     <row r="26" spans="1:5" ht="28.9" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="44" t="s">
+      <c r="A26" s="41" t="s">
         <v>240</v>
       </c>
-      <c r="B26" s="44"/>
-      <c r="C26" s="44"/>
-      <c r="D26" s="44"/>
-      <c r="E26" s="44"/>
+      <c r="B26" s="41"/>
+      <c r="C26" s="41"/>
+      <c r="D26" s="41"/>
+      <c r="E26" s="41"/>
     </row>
     <row r="27" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A27" s="20" t="s">
@@ -4649,10 +4576,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{18F2B7B4-0119-40B2-9AE3-A031B16A0EEC}">
-  <dimension ref="A1:K20"/>
+  <dimension ref="A1:K16"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L2" sqref="L2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4671,441 +4598,336 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A1" s="37" t="s">
+      <c r="A1" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="37" t="s">
+      <c r="B1" s="36" t="s">
         <v>55</v>
       </c>
-      <c r="C1" s="37" t="s">
+      <c r="C1" s="36" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="37" t="s">
+      <c r="D1" s="36" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="37" t="s">
+      <c r="E1" s="36" t="s">
         <v>56</v>
       </c>
-      <c r="F1" s="37" t="s">
+      <c r="F1" s="36" t="s">
         <v>57</v>
       </c>
-      <c r="G1" s="37" t="s">
+      <c r="G1" s="36" t="s">
         <v>58</v>
       </c>
-      <c r="H1" s="37" t="s">
+      <c r="H1" s="36" t="s">
         <v>59</v>
       </c>
-      <c r="I1" s="37" t="s">
+      <c r="I1" s="36" t="s">
         <v>60</v>
       </c>
-      <c r="J1" s="37" t="s">
+      <c r="J1" s="36" t="s">
         <v>61</v>
       </c>
-      <c r="K1" s="37" t="s">
+      <c r="K1" s="36" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="2" spans="1:11" ht="146.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="39" t="s">
+      <c r="A2" s="24" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="25" t="s">
-        <v>298</v>
-      </c>
-      <c r="C2" s="25" t="s">
-        <v>301</v>
-      </c>
-      <c r="D2" s="25" t="s">
-        <v>301</v>
-      </c>
-      <c r="E2" s="25" t="s">
-        <v>301</v>
-      </c>
-      <c r="F2" s="25" t="s">
-        <v>301</v>
-      </c>
-      <c r="G2" s="25" t="s">
-        <v>330</v>
-      </c>
-      <c r="H2" s="25" t="s">
-        <v>333</v>
-      </c>
-      <c r="I2" s="25" t="s">
-        <v>333</v>
-      </c>
-      <c r="J2" s="25" t="s">
-        <v>335</v>
-      </c>
-      <c r="K2" s="25" t="s">
-        <v>338</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A3" s="39"/>
-      <c r="B3" s="25" t="s">
+      <c r="B2" s="24" t="s">
+        <v>396</v>
+      </c>
+      <c r="C2" s="24" t="s">
+        <v>397</v>
+      </c>
+      <c r="D2" s="24" t="s">
+        <v>398</v>
+      </c>
+      <c r="E2" s="24" t="s">
+        <v>399</v>
+      </c>
+      <c r="F2" s="24" t="s">
+        <v>400</v>
+      </c>
+      <c r="G2" s="24" t="s">
+        <v>401</v>
+      </c>
+      <c r="H2" s="24" t="s">
+        <v>402</v>
+      </c>
+      <c r="I2" s="24" t="s">
+        <v>402</v>
+      </c>
+      <c r="J2" s="24" t="s">
+        <v>403</v>
+      </c>
+      <c r="K2" s="24" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A3" s="26">
+        <v>1</v>
+      </c>
+      <c r="B3" s="26" t="s">
+        <v>305</v>
+      </c>
+      <c r="C3" s="24" t="s">
+        <v>306</v>
+      </c>
+      <c r="D3" s="24" t="s">
+        <v>307</v>
+      </c>
+      <c r="E3" s="34" t="s">
+        <v>308</v>
+      </c>
+      <c r="F3" s="24">
+        <v>901123121</v>
+      </c>
+      <c r="G3" s="35" t="s">
+        <v>309</v>
+      </c>
+      <c r="H3" s="26" t="s">
+        <v>310</v>
+      </c>
+      <c r="I3" s="26" t="s">
+        <v>311</v>
+      </c>
+      <c r="J3" s="26"/>
+      <c r="K3" s="26"/>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A4" s="26">
+        <v>2</v>
+      </c>
+      <c r="B4" s="26" t="s">
+        <v>312</v>
+      </c>
+      <c r="C4" s="24" t="s">
+        <v>313</v>
+      </c>
+      <c r="D4" s="24" t="s">
         <v>314</v>
       </c>
-      <c r="C3" s="25" t="s">
+      <c r="E4" s="34" t="s">
+        <v>315</v>
+      </c>
+      <c r="F4" s="24">
+        <v>901123122</v>
+      </c>
+      <c r="G4" s="35" t="s">
+        <v>316</v>
+      </c>
+      <c r="H4" s="26" t="s">
+        <v>310</v>
+      </c>
+      <c r="I4" s="26" t="s">
+        <v>317</v>
+      </c>
+      <c r="J4" s="26"/>
+      <c r="K4" s="26"/>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A5" s="26">
+        <v>3</v>
+      </c>
+      <c r="B5" s="26" t="s">
         <v>318</v>
       </c>
-      <c r="D3" s="25" t="s">
-        <v>318</v>
-      </c>
-      <c r="E3" s="25" t="s">
+      <c r="C5" s="24" t="s">
+        <v>319</v>
+      </c>
+      <c r="D5" s="24" t="s">
+        <v>320</v>
+      </c>
+      <c r="E5" s="34" t="s">
+        <v>321</v>
+      </c>
+      <c r="F5" s="24">
+        <v>901123123</v>
+      </c>
+      <c r="G5" s="35" t="s">
+        <v>322</v>
+      </c>
+      <c r="H5" s="26" t="s">
+        <v>310</v>
+      </c>
+      <c r="I5" s="26" t="s">
         <v>323</v>
       </c>
-      <c r="F3" s="25" t="s">
+      <c r="J5" s="26"/>
+      <c r="K5" s="26"/>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A6" s="26">
+        <v>4</v>
+      </c>
+      <c r="B6" s="26" t="s">
+        <v>324</v>
+      </c>
+      <c r="C6" s="24" t="s">
+        <v>325</v>
+      </c>
+      <c r="D6" s="24" t="s">
         <v>326</v>
       </c>
-      <c r="G3" s="25" t="s">
-        <v>331</v>
-      </c>
-      <c r="H3" s="25" t="s">
-        <v>334</v>
-      </c>
-      <c r="I3" s="25" t="s">
-        <v>334</v>
-      </c>
-      <c r="J3" s="25" t="s">
-        <v>336</v>
-      </c>
-      <c r="K3" s="25" t="s">
-        <v>339</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A4" s="39"/>
-      <c r="B4" s="25" t="s">
-        <v>315</v>
-      </c>
-      <c r="C4" s="25" t="s">
-        <v>319</v>
-      </c>
-      <c r="D4" s="25" t="s">
-        <v>321</v>
-      </c>
-      <c r="E4" s="25" t="s">
-        <v>324</v>
-      </c>
-      <c r="F4" s="25" t="s">
+      <c r="E6" s="34" t="s">
         <v>327</v>
       </c>
-      <c r="G4" s="25" t="s">
-        <v>332</v>
-      </c>
-      <c r="H4" s="25"/>
-      <c r="I4" s="25"/>
-      <c r="J4" s="25" t="s">
-        <v>337</v>
-      </c>
-      <c r="K4" s="25" t="s">
-        <v>340</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" ht="29" x14ac:dyDescent="0.35">
-      <c r="A5" s="39"/>
-      <c r="B5" s="25" t="s">
-        <v>316</v>
-      </c>
-      <c r="C5" s="25" t="s">
-        <v>320</v>
-      </c>
-      <c r="D5" s="25" t="s">
-        <v>322</v>
-      </c>
-      <c r="E5" s="25" t="s">
-        <v>325</v>
-      </c>
-      <c r="F5" s="25" t="s">
+      <c r="F6" s="24">
+        <v>901123124</v>
+      </c>
+      <c r="G6" s="35" t="s">
         <v>328</v>
       </c>
-      <c r="G5" s="25"/>
-      <c r="H5" s="25"/>
-      <c r="I5" s="25"/>
-      <c r="J5" s="25"/>
-      <c r="K5" s="25"/>
-    </row>
-    <row r="6" spans="1:11" ht="32.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="39"/>
-      <c r="B6" s="25" t="s">
-        <v>317</v>
-      </c>
-      <c r="C6" s="25"/>
-      <c r="D6" s="25"/>
-      <c r="E6" s="25"/>
-      <c r="F6" s="25" t="s">
+      <c r="H6" s="26" t="s">
+        <v>310</v>
+      </c>
+      <c r="I6" s="26" t="s">
         <v>329</v>
       </c>
-      <c r="G6" s="25"/>
-      <c r="H6" s="25"/>
-      <c r="I6" s="25"/>
-      <c r="J6" s="25"/>
-      <c r="K6" s="25"/>
+      <c r="J6" s="26"/>
+      <c r="K6" s="26"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A7" s="27">
-        <v>1</v>
-      </c>
-      <c r="B7" s="27" t="s">
-        <v>341</v>
-      </c>
-      <c r="C7" s="25" t="s">
-        <v>342</v>
-      </c>
-      <c r="D7" s="25" t="s">
-        <v>343</v>
-      </c>
-      <c r="E7" s="35" t="s">
-        <v>344</v>
-      </c>
-      <c r="F7" s="25">
-        <v>901123121</v>
-      </c>
-      <c r="G7" s="36" t="s">
-        <v>345</v>
-      </c>
-      <c r="H7" s="27" t="s">
-        <v>346</v>
-      </c>
-      <c r="I7" s="27" t="s">
-        <v>347</v>
-      </c>
-      <c r="J7" s="27"/>
-      <c r="K7" s="27"/>
+      <c r="A7" s="26"/>
+      <c r="B7" s="26"/>
+      <c r="C7" s="24"/>
+      <c r="D7" s="24"/>
+      <c r="E7" s="34"/>
+      <c r="F7" s="24"/>
+      <c r="G7" s="35"/>
+      <c r="H7" s="26"/>
+      <c r="I7" s="26"/>
+      <c r="J7" s="26"/>
+      <c r="K7" s="26"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A8" s="27">
-        <v>2</v>
-      </c>
-      <c r="B8" s="27" t="s">
-        <v>348</v>
-      </c>
-      <c r="C8" s="25" t="s">
-        <v>349</v>
-      </c>
-      <c r="D8" s="25" t="s">
-        <v>350</v>
-      </c>
-      <c r="E8" s="35" t="s">
-        <v>351</v>
-      </c>
-      <c r="F8" s="25">
-        <v>901123122</v>
-      </c>
-      <c r="G8" s="36" t="s">
-        <v>352</v>
-      </c>
-      <c r="H8" s="27" t="s">
-        <v>346</v>
-      </c>
-      <c r="I8" s="27" t="s">
-        <v>353</v>
-      </c>
-      <c r="J8" s="27"/>
-      <c r="K8" s="27"/>
+      <c r="A8" s="26"/>
+      <c r="B8" s="26"/>
+      <c r="C8" s="24"/>
+      <c r="D8" s="24"/>
+      <c r="E8" s="34"/>
+      <c r="F8" s="24"/>
+      <c r="G8" s="35"/>
+      <c r="H8" s="26"/>
+      <c r="I8" s="26"/>
+      <c r="J8" s="26"/>
+      <c r="K8" s="26"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A9" s="27">
-        <v>3</v>
-      </c>
-      <c r="B9" s="27" t="s">
-        <v>354</v>
-      </c>
-      <c r="C9" s="25" t="s">
-        <v>355</v>
-      </c>
-      <c r="D9" s="25" t="s">
-        <v>356</v>
-      </c>
-      <c r="E9" s="35" t="s">
-        <v>357</v>
-      </c>
-      <c r="F9" s="25">
-        <v>901123123</v>
-      </c>
-      <c r="G9" s="36" t="s">
-        <v>358</v>
-      </c>
-      <c r="H9" s="27" t="s">
-        <v>346</v>
-      </c>
-      <c r="I9" s="27" t="s">
-        <v>359</v>
-      </c>
-      <c r="J9" s="27"/>
-      <c r="K9" s="27"/>
+      <c r="A9" s="26"/>
+      <c r="B9" s="26"/>
+      <c r="C9" s="24"/>
+      <c r="D9" s="24"/>
+      <c r="E9" s="34"/>
+      <c r="F9" s="24"/>
+      <c r="G9" s="35"/>
+      <c r="H9" s="26"/>
+      <c r="I9" s="26"/>
+      <c r="J9" s="26"/>
+      <c r="K9" s="26"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A10" s="27">
-        <v>4</v>
-      </c>
-      <c r="B10" s="27" t="s">
-        <v>360</v>
-      </c>
-      <c r="C10" s="25" t="s">
-        <v>361</v>
-      </c>
-      <c r="D10" s="25" t="s">
-        <v>362</v>
-      </c>
-      <c r="E10" s="35" t="s">
-        <v>363</v>
-      </c>
-      <c r="F10" s="25">
-        <v>901123124</v>
-      </c>
-      <c r="G10" s="36" t="s">
-        <v>364</v>
-      </c>
-      <c r="H10" s="27" t="s">
-        <v>346</v>
-      </c>
-      <c r="I10" s="27" t="s">
-        <v>365</v>
-      </c>
-      <c r="J10" s="27"/>
-      <c r="K10" s="27"/>
+      <c r="A10" s="26"/>
+      <c r="B10" s="26"/>
+      <c r="C10" s="24"/>
+      <c r="D10" s="24"/>
+      <c r="E10" s="34"/>
+      <c r="F10" s="24"/>
+      <c r="G10" s="35"/>
+      <c r="H10" s="26"/>
+      <c r="I10" s="27"/>
+      <c r="J10" s="26"/>
+      <c r="K10" s="26"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A11" s="27"/>
-      <c r="B11" s="27"/>
-      <c r="C11" s="25"/>
-      <c r="D11" s="25"/>
-      <c r="E11" s="35"/>
-      <c r="F11" s="25"/>
-      <c r="G11" s="36"/>
-      <c r="H11" s="27"/>
+      <c r="A11" s="26"/>
+      <c r="B11" s="26"/>
+      <c r="C11" s="24"/>
+      <c r="D11" s="24"/>
+      <c r="E11" s="34"/>
+      <c r="F11" s="24"/>
+      <c r="G11" s="35"/>
+      <c r="H11" s="26"/>
       <c r="I11" s="27"/>
-      <c r="J11" s="27"/>
-      <c r="K11" s="27"/>
+      <c r="J11" s="26"/>
+      <c r="K11" s="26"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A12" s="27"/>
-      <c r="B12" s="27"/>
-      <c r="C12" s="25"/>
-      <c r="D12" s="25"/>
-      <c r="E12" s="35"/>
-      <c r="F12" s="25"/>
-      <c r="G12" s="36"/>
-      <c r="H12" s="27"/>
+      <c r="A12" s="26"/>
+      <c r="B12" s="26"/>
+      <c r="C12" s="24"/>
+      <c r="D12" s="24"/>
+      <c r="E12" s="34"/>
+      <c r="F12" s="24"/>
+      <c r="G12" s="35"/>
+      <c r="H12" s="26"/>
       <c r="I12" s="27"/>
-      <c r="J12" s="27"/>
-      <c r="K12" s="27"/>
+      <c r="J12" s="26"/>
+      <c r="K12" s="26"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A13" s="27"/>
-      <c r="B13" s="27"/>
-      <c r="C13" s="25"/>
-      <c r="D13" s="25"/>
-      <c r="E13" s="35"/>
-      <c r="F13" s="25"/>
-      <c r="G13" s="36"/>
-      <c r="H13" s="27"/>
+      <c r="A13" s="26"/>
+      <c r="B13" s="26"/>
+      <c r="C13" s="24"/>
+      <c r="D13" s="24"/>
+      <c r="E13" s="34"/>
+      <c r="F13" s="24"/>
+      <c r="G13" s="35"/>
+      <c r="H13" s="26"/>
       <c r="I13" s="27"/>
-      <c r="J13" s="27"/>
-      <c r="K13" s="27"/>
+      <c r="J13" s="26"/>
+      <c r="K13" s="26"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A14" s="27"/>
-      <c r="B14" s="27"/>
-      <c r="C14" s="25"/>
-      <c r="D14" s="25"/>
-      <c r="E14" s="35"/>
-      <c r="F14" s="25"/>
-      <c r="G14" s="36"/>
-      <c r="H14" s="27"/>
-      <c r="I14" s="28"/>
-      <c r="J14" s="27"/>
-      <c r="K14" s="27"/>
+      <c r="A14" s="26"/>
+      <c r="B14" s="26"/>
+      <c r="C14" s="24"/>
+      <c r="D14" s="24"/>
+      <c r="E14" s="34"/>
+      <c r="F14" s="24"/>
+      <c r="G14" s="35"/>
+      <c r="H14" s="26"/>
+      <c r="I14" s="26"/>
+      <c r="J14" s="26"/>
+      <c r="K14" s="26"/>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A15" s="27"/>
-      <c r="B15" s="27"/>
-      <c r="C15" s="25"/>
-      <c r="D15" s="25"/>
-      <c r="E15" s="35"/>
-      <c r="F15" s="25"/>
-      <c r="G15" s="36"/>
-      <c r="H15" s="27"/>
-      <c r="I15" s="28"/>
-      <c r="J15" s="27"/>
-      <c r="K15" s="27"/>
+      <c r="A15" s="26"/>
+      <c r="B15" s="26"/>
+      <c r="C15" s="24"/>
+      <c r="D15" s="24"/>
+      <c r="E15" s="34"/>
+      <c r="F15" s="24"/>
+      <c r="G15" s="35"/>
+      <c r="H15" s="26"/>
+      <c r="I15" s="26"/>
+      <c r="J15" s="26"/>
+      <c r="K15" s="26"/>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A16" s="27"/>
-      <c r="B16" s="27"/>
-      <c r="C16" s="25"/>
-      <c r="D16" s="25"/>
-      <c r="E16" s="35"/>
-      <c r="F16" s="25"/>
-      <c r="G16" s="36"/>
-      <c r="H16" s="27"/>
-      <c r="I16" s="28"/>
-      <c r="J16" s="27"/>
-      <c r="K16" s="27"/>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A17" s="27"/>
-      <c r="B17" s="27"/>
-      <c r="C17" s="25"/>
-      <c r="D17" s="25"/>
-      <c r="E17" s="35"/>
-      <c r="F17" s="25"/>
-      <c r="G17" s="36"/>
-      <c r="H17" s="27"/>
-      <c r="I17" s="28"/>
-      <c r="J17" s="27"/>
-      <c r="K17" s="27"/>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A18" s="27"/>
-      <c r="B18" s="27"/>
-      <c r="C18" s="25"/>
-      <c r="D18" s="25"/>
-      <c r="E18" s="35"/>
-      <c r="F18" s="25"/>
-      <c r="G18" s="36"/>
-      <c r="H18" s="27"/>
-      <c r="I18" s="27"/>
-      <c r="J18" s="27"/>
-      <c r="K18" s="27"/>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A19" s="27"/>
-      <c r="B19" s="27"/>
-      <c r="C19" s="25"/>
-      <c r="D19" s="25"/>
-      <c r="E19" s="35"/>
-      <c r="F19" s="25"/>
-      <c r="G19" s="36"/>
-      <c r="H19" s="27"/>
-      <c r="I19" s="27"/>
-      <c r="J19" s="27"/>
-      <c r="K19" s="27"/>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A20" s="27"/>
-      <c r="B20" s="27"/>
-      <c r="C20" s="25"/>
-      <c r="D20" s="25"/>
-      <c r="E20" s="35"/>
-      <c r="F20" s="25"/>
-      <c r="G20" s="36"/>
-      <c r="H20" s="27"/>
-      <c r="I20" s="27"/>
-      <c r="J20" s="27"/>
-      <c r="K20" s="27"/>
+      <c r="A16" s="26"/>
+      <c r="B16" s="26"/>
+      <c r="C16" s="24"/>
+      <c r="D16" s="24"/>
+      <c r="E16" s="34"/>
+      <c r="F16" s="24"/>
+      <c r="G16" s="35"/>
+      <c r="H16" s="26"/>
+      <c r="I16" s="26"/>
+      <c r="J16" s="26"/>
+      <c r="K16" s="26"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A2:A6"/>
-  </mergeCells>
   <phoneticPr fontId="6" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="E7" r:id="rId1" display="mailto:huy.thieu@example.com" xr:uid="{4A4BF452-E085-4C44-A19D-95C21B647037}"/>
-    <hyperlink ref="E8" r:id="rId2" display="mailto:hien.pham@example.com" xr:uid="{60160983-CEC5-4076-9255-285C06F3D878}"/>
-    <hyperlink ref="E9" r:id="rId3" display="mailto:trung.duong@example.com" xr:uid="{6C206E72-BFB0-42F0-98FF-885550E07C35}"/>
-    <hyperlink ref="E10" r:id="rId4" display="mailto:linh.nguyen@example.com" xr:uid="{03D36B46-AE10-4A7E-A689-ACDC9359BA2C}"/>
+    <hyperlink ref="E3" r:id="rId1" display="mailto:huy.thieu@example.com" xr:uid="{4A4BF452-E085-4C44-A19D-95C21B647037}"/>
+    <hyperlink ref="E4" r:id="rId2" display="mailto:hien.pham@example.com" xr:uid="{60160983-CEC5-4076-9255-285C06F3D878}"/>
+    <hyperlink ref="E5" r:id="rId3" display="mailto:trung.duong@example.com" xr:uid="{6C206E72-BFB0-42F0-98FF-885550E07C35}"/>
+    <hyperlink ref="E6" r:id="rId4" display="mailto:linh.nguyen@example.com" xr:uid="{03D36B46-AE10-4A7E-A689-ACDC9359BA2C}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -5218,10 +5040,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{13B36471-B49B-4FB2-BB36-0F0FCC8EE11D}">
-  <dimension ref="A1:K9"/>
+  <dimension ref="A1:K6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -5241,255 +5063,180 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="46" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="24" t="s">
+      <c r="B1" s="46" t="s">
         <v>55</v>
       </c>
-      <c r="C1" s="24" t="s">
+      <c r="C1" s="46" t="s">
         <v>46</v>
       </c>
-      <c r="D1" s="24" t="s">
+      <c r="D1" s="46" t="s">
         <v>78</v>
       </c>
-      <c r="E1" s="24" t="s">
+      <c r="E1" s="46" t="s">
         <v>79</v>
       </c>
-      <c r="F1" s="24" t="s">
+      <c r="F1" s="46" t="s">
         <v>80</v>
       </c>
-      <c r="G1" s="24" t="s">
+      <c r="G1" s="46" t="s">
         <v>47</v>
       </c>
-      <c r="H1" s="24" t="s">
+      <c r="H1" s="46" t="s">
         <v>81</v>
       </c>
-      <c r="I1" s="24" t="s">
+      <c r="I1" s="46" t="s">
         <v>82</v>
       </c>
-      <c r="J1" s="24" t="s">
+      <c r="J1" s="46" t="s">
         <v>83</v>
       </c>
-      <c r="K1" s="24" t="s">
+      <c r="K1" s="46" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="92" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="38" t="s">
+    <row r="2" spans="1:11" ht="174" x14ac:dyDescent="0.35">
+      <c r="A2" s="48" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="25" t="s">
-        <v>298</v>
-      </c>
-      <c r="C2" s="25" t="s">
-        <v>301</v>
-      </c>
-      <c r="D2" s="25" t="s">
-        <v>301</v>
-      </c>
-      <c r="E2" s="25" t="s">
-        <v>374</v>
-      </c>
-      <c r="F2" s="38" t="s">
+      <c r="B2" s="45" t="s">
+        <v>405</v>
+      </c>
+      <c r="C2" s="45" t="s">
+        <v>406</v>
+      </c>
+      <c r="D2" s="45" t="s">
+        <v>407</v>
+      </c>
+      <c r="E2" s="45" t="s">
+        <v>408</v>
+      </c>
+      <c r="F2" s="48" t="s">
         <v>85</v>
       </c>
-      <c r="G2" s="25" t="s">
-        <v>304</v>
-      </c>
-      <c r="H2" s="25" t="s">
-        <v>377</v>
-      </c>
-      <c r="I2" s="25" t="s">
-        <v>378</v>
-      </c>
-      <c r="J2" s="25" t="s">
-        <v>377</v>
-      </c>
-      <c r="K2" s="25" t="s">
-        <v>380</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" ht="87" x14ac:dyDescent="0.35">
-      <c r="A3" s="39"/>
-      <c r="B3" s="25" t="s">
-        <v>367</v>
-      </c>
-      <c r="C3" s="25" t="s">
-        <v>370</v>
-      </c>
-      <c r="D3" s="25" t="s">
-        <v>372</v>
-      </c>
-      <c r="E3" s="25" t="s">
-        <v>375</v>
-      </c>
-      <c r="F3" s="39"/>
-      <c r="G3" s="25" t="s">
+      <c r="G2" s="45" t="s">
+        <v>409</v>
+      </c>
+      <c r="H2" s="45" t="s">
+        <v>410</v>
+      </c>
+      <c r="I2" s="45" t="s">
+        <v>411</v>
+      </c>
+      <c r="J2" s="45" t="s">
+        <v>410</v>
+      </c>
+      <c r="K2" s="45" t="s">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A3" s="45">
+        <v>1</v>
+      </c>
+      <c r="B3" s="45" t="s">
+        <v>86</v>
+      </c>
+      <c r="C3" s="45" t="s">
+        <v>71</v>
+      </c>
+      <c r="D3" s="45">
+        <v>1</v>
+      </c>
+      <c r="E3" s="45"/>
+      <c r="F3" s="45"/>
+      <c r="G3" s="45"/>
+      <c r="H3" s="45"/>
+      <c r="I3" s="45" t="s">
+        <v>52</v>
+      </c>
+      <c r="J3" s="45"/>
+      <c r="K3" s="45"/>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A4" s="45">
+        <v>2</v>
+      </c>
+      <c r="B4" s="45" t="s">
+        <v>87</v>
+      </c>
+      <c r="C4" s="45" t="s">
+        <v>88</v>
+      </c>
+      <c r="D4" s="45">
+        <v>2</v>
+      </c>
+      <c r="E4" s="45" t="s">
+        <v>86</v>
+      </c>
+      <c r="F4" s="45"/>
+      <c r="G4" s="47" t="s">
         <v>305</v>
       </c>
-      <c r="H3" s="25" t="s">
-        <v>317</v>
-      </c>
-      <c r="I3" s="25" t="s">
-        <v>379</v>
-      </c>
-      <c r="J3" s="25" t="s">
-        <v>317</v>
-      </c>
-      <c r="K3" s="25" t="s">
-        <v>381</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A4" s="39"/>
-      <c r="B4" s="25" t="s">
-        <v>368</v>
-      </c>
-      <c r="C4" s="25" t="s">
-        <v>371</v>
-      </c>
-      <c r="D4" s="25" t="s">
-        <v>373</v>
-      </c>
-      <c r="E4" s="25" t="s">
-        <v>337</v>
-      </c>
-      <c r="F4" s="39"/>
-      <c r="G4" s="25" t="s">
-        <v>376</v>
-      </c>
-      <c r="H4" s="25"/>
-      <c r="I4" s="25"/>
-      <c r="J4" s="25"/>
-      <c r="K4" s="25"/>
-    </row>
-    <row r="5" spans="1:11" ht="29" x14ac:dyDescent="0.35">
-      <c r="A5" s="39"/>
-      <c r="B5" s="25" t="s">
-        <v>369</v>
-      </c>
-      <c r="C5" s="25"/>
-      <c r="D5" s="25"/>
-      <c r="E5" s="25"/>
-      <c r="F5" s="39"/>
-      <c r="G5" s="25" t="s">
-        <v>306</v>
-      </c>
-      <c r="H5" s="25"/>
-      <c r="I5" s="25"/>
-      <c r="J5" s="25"/>
-      <c r="K5" s="25"/>
+      <c r="H4" s="45"/>
+      <c r="I4" s="45" t="s">
+        <v>331</v>
+      </c>
+      <c r="J4" s="45"/>
+      <c r="K4" s="45"/>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A5" s="45">
+        <v>3</v>
+      </c>
+      <c r="B5" s="45" t="s">
+        <v>50</v>
+      </c>
+      <c r="C5" s="45" t="s">
+        <v>89</v>
+      </c>
+      <c r="D5" s="45">
+        <v>2</v>
+      </c>
+      <c r="E5" s="45" t="s">
+        <v>86</v>
+      </c>
+      <c r="F5" s="45"/>
+      <c r="G5" s="45" t="s">
+        <v>332</v>
+      </c>
+      <c r="H5" s="45"/>
+      <c r="I5" s="45" t="s">
+        <v>90</v>
+      </c>
+      <c r="J5" s="45"/>
+      <c r="K5" s="45"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A6" s="25">
-        <v>1</v>
-      </c>
-      <c r="B6" s="25" t="s">
+      <c r="A6" s="45">
+        <v>4</v>
+      </c>
+      <c r="B6" s="45" t="s">
+        <v>91</v>
+      </c>
+      <c r="C6" s="45" t="s">
+        <v>92</v>
+      </c>
+      <c r="D6" s="45">
+        <v>2</v>
+      </c>
+      <c r="E6" s="45" t="s">
         <v>86</v>
       </c>
-      <c r="C6" s="25" t="s">
-        <v>71</v>
-      </c>
-      <c r="D6" s="25">
-        <v>1</v>
-      </c>
-      <c r="E6" s="25"/>
-      <c r="F6" s="25"/>
-      <c r="G6" s="25"/>
-      <c r="H6" s="25"/>
-      <c r="I6" s="25" t="s">
-        <v>52</v>
-      </c>
-      <c r="J6" s="25"/>
-      <c r="K6" s="25"/>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A7" s="25">
-        <v>2</v>
-      </c>
-      <c r="B7" s="25" t="s">
-        <v>87</v>
-      </c>
-      <c r="C7" s="25" t="s">
-        <v>88</v>
-      </c>
-      <c r="D7" s="25">
-        <v>2</v>
-      </c>
-      <c r="E7" s="25" t="s">
-        <v>86</v>
-      </c>
-      <c r="F7" s="25"/>
-      <c r="G7" s="27" t="s">
-        <v>341</v>
-      </c>
-      <c r="H7" s="25"/>
-      <c r="I7" s="25" t="s">
-        <v>382</v>
-      </c>
-      <c r="J7" s="25"/>
-      <c r="K7" s="25"/>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A8" s="25">
-        <v>3</v>
-      </c>
-      <c r="B8" s="25" t="s">
-        <v>50</v>
-      </c>
-      <c r="C8" s="25" t="s">
-        <v>89</v>
-      </c>
-      <c r="D8" s="25">
-        <v>2</v>
-      </c>
-      <c r="E8" s="25" t="s">
-        <v>86</v>
-      </c>
-      <c r="F8" s="25"/>
-      <c r="G8" s="25" t="s">
-        <v>383</v>
-      </c>
-      <c r="H8" s="25"/>
-      <c r="I8" s="25" t="s">
-        <v>90</v>
-      </c>
-      <c r="J8" s="25"/>
-      <c r="K8" s="25"/>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A9" s="25">
-        <v>4</v>
-      </c>
-      <c r="B9" s="25" t="s">
-        <v>91</v>
-      </c>
-      <c r="C9" s="25" t="s">
-        <v>92</v>
-      </c>
-      <c r="D9" s="25">
-        <v>2</v>
-      </c>
-      <c r="E9" s="25" t="s">
-        <v>86</v>
-      </c>
-      <c r="F9" s="25"/>
-      <c r="G9" s="25" t="s">
-        <v>384</v>
-      </c>
-      <c r="H9" s="25"/>
-      <c r="I9" s="25" t="s">
+      <c r="F6" s="45"/>
+      <c r="G6" s="45" t="s">
+        <v>333</v>
+      </c>
+      <c r="H6" s="45"/>
+      <c r="I6" s="45" t="s">
         <v>93</v>
       </c>
-      <c r="J9" s="25"/>
-      <c r="K9" s="25"/>
+      <c r="J6" s="45"/>
+      <c r="K6" s="45"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="A2:A5"/>
-    <mergeCell ref="F2:F5"/>
-  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -5573,16 +5320,16 @@
       </c>
     </row>
     <row r="2" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A2" s="29" t="s">
+      <c r="A2" s="28" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="29" t="s">
+      <c r="B2" s="28" t="s">
         <v>99</v>
       </c>
-      <c r="C2" s="29" t="s">
+      <c r="C2" s="28" t="s">
         <v>100</v>
       </c>
-      <c r="D2" s="29"/>
+      <c r="D2" s="28"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5627,102 +5374,102 @@
       </c>
     </row>
     <row r="2" spans="1:6" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="A2" s="29" t="s">
+      <c r="A2" s="28" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="29" t="s">
+      <c r="B2" s="28" t="s">
         <v>105</v>
       </c>
-      <c r="C2" s="29" t="s">
+      <c r="C2" s="28" t="s">
         <v>106</v>
       </c>
-      <c r="D2" s="29" t="s">
-        <v>385</v>
-      </c>
-      <c r="E2" s="29" t="s">
+      <c r="D2" s="28" t="s">
+        <v>334</v>
+      </c>
+      <c r="E2" s="28" t="s">
         <v>107</v>
       </c>
-      <c r="F2" s="30" t="s">
+      <c r="F2" s="29" t="s">
         <v>108</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A3" s="26">
+      <c r="A3" s="25">
         <v>1</v>
       </c>
-      <c r="B3" s="26" t="s">
-        <v>386</v>
-      </c>
-      <c r="C3" s="26" t="s">
-        <v>386</v>
-      </c>
-      <c r="D3" s="26">
+      <c r="B3" s="25" t="s">
+        <v>335</v>
+      </c>
+      <c r="C3" s="25" t="s">
+        <v>335</v>
+      </c>
+      <c r="D3" s="25">
         <v>1</v>
       </c>
-      <c r="E3" s="26" t="s">
+      <c r="E3" s="25" t="s">
         <v>101</v>
       </c>
-      <c r="F3" s="26">
+      <c r="F3" s="25">
         <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A4" s="26">
+      <c r="A4" s="25">
         <v>2</v>
       </c>
-      <c r="B4" s="26" t="s">
+      <c r="B4" s="25" t="s">
         <v>186</v>
       </c>
-      <c r="C4" s="26" t="s">
+      <c r="C4" s="25" t="s">
         <v>186</v>
       </c>
-      <c r="D4" s="26">
+      <c r="D4" s="25">
         <v>1</v>
       </c>
-      <c r="E4" s="26" t="s">
+      <c r="E4" s="25" t="s">
         <v>101</v>
       </c>
-      <c r="F4" s="26">
+      <c r="F4" s="25">
         <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A5" s="26">
+      <c r="A5" s="25">
         <v>3</v>
       </c>
-      <c r="B5" s="26" t="s">
-        <v>387</v>
-      </c>
-      <c r="C5" s="26" t="s">
-        <v>387</v>
-      </c>
-      <c r="D5" s="26">
+      <c r="B5" s="25" t="s">
+        <v>336</v>
+      </c>
+      <c r="C5" s="25" t="s">
+        <v>336</v>
+      </c>
+      <c r="D5" s="25">
         <v>1</v>
       </c>
-      <c r="E5" s="26" t="s">
+      <c r="E5" s="25" t="s">
         <v>101</v>
       </c>
-      <c r="F5" s="26">
+      <c r="F5" s="25">
         <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A6" s="26">
+      <c r="A6" s="25">
         <v>4</v>
       </c>
-      <c r="B6" s="26" t="s">
-        <v>388</v>
-      </c>
-      <c r="C6" s="26" t="s">
-        <v>388</v>
-      </c>
-      <c r="D6" s="26">
+      <c r="B6" s="25" t="s">
+        <v>337</v>
+      </c>
+      <c r="C6" s="25" t="s">
+        <v>337</v>
+      </c>
+      <c r="D6" s="25">
         <v>1</v>
       </c>
-      <c r="E6" s="26" t="s">
+      <c r="E6" s="25" t="s">
         <v>101</v>
       </c>
-      <c r="F6" s="26">
+      <c r="F6" s="25">
         <v>10</v>
       </c>
     </row>
@@ -5774,64 +5521,64 @@
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A3" s="25">
+      <c r="A3" s="24">
         <v>1</v>
       </c>
-      <c r="B3" s="25" t="s">
-        <v>389</v>
-      </c>
-      <c r="C3" s="25" t="s">
+      <c r="B3" s="24" t="s">
+        <v>338</v>
+      </c>
+      <c r="C3" s="24" t="s">
         <v>111</v>
       </c>
-      <c r="D3" s="25"/>
+      <c r="D3" s="24"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A4" s="25">
+      <c r="A4" s="24">
         <v>2</v>
       </c>
-      <c r="B4" s="25" t="s">
-        <v>390</v>
-      </c>
-      <c r="C4" s="25" t="s">
+      <c r="B4" s="24" t="s">
+        <v>339</v>
+      </c>
+      <c r="C4" s="24" t="s">
         <v>113</v>
       </c>
-      <c r="D4" s="25"/>
+      <c r="D4" s="24"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A5" s="25">
+      <c r="A5" s="24">
         <v>3</v>
       </c>
-      <c r="B5" s="25" t="s">
-        <v>391</v>
-      </c>
-      <c r="C5" s="25" t="s">
+      <c r="B5" s="24" t="s">
+        <v>340</v>
+      </c>
+      <c r="C5" s="24" t="s">
         <v>114</v>
       </c>
-      <c r="D5" s="25"/>
+      <c r="D5" s="24"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A6" s="25">
+      <c r="A6" s="24">
         <v>4</v>
       </c>
-      <c r="B6" s="25" t="s">
-        <v>392</v>
-      </c>
-      <c r="C6" s="25" t="s">
+      <c r="B6" s="24" t="s">
+        <v>341</v>
+      </c>
+      <c r="C6" s="24" t="s">
         <v>115</v>
       </c>
-      <c r="D6" s="25"/>
+      <c r="D6" s="24"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A7" s="25">
+      <c r="A7" s="24">
         <v>5</v>
       </c>
-      <c r="B7" s="25" t="s">
-        <v>393</v>
-      </c>
-      <c r="C7" s="25" t="s">
+      <c r="B7" s="24" t="s">
+        <v>342</v>
+      </c>
+      <c r="C7" s="24" t="s">
         <v>116</v>
       </c>
-      <c r="D7" s="25"/>
+      <c r="D7" s="24"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>